<commit_message>
Update NBA prices - 2025-12-09 01:41 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -204,6 +204,84 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>2</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>2</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>2</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="4" name="Image 4" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -500,7 +578,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,6 +589,15 @@
     <col width="25" customWidth="1" min="1" max="1"/>
     <col width="25" customWidth="1" min="2" max="2"/>
     <col width="3" customWidth="1" min="3" max="3"/>
+    <col width="25" customWidth="1" min="4" max="4"/>
+    <col width="25" customWidth="1" min="5" max="5"/>
+    <col width="3" customWidth="1" min="6" max="6"/>
+    <col width="25" customWidth="1" min="7" max="7"/>
+    <col width="25" customWidth="1" min="8" max="8"/>
+    <col width="3" customWidth="1" min="9" max="9"/>
+    <col width="25" customWidth="1" min="10" max="10"/>
+    <col width="25" customWidth="1" min="11" max="11"/>
+    <col width="3" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -520,6 +607,24 @@
         </is>
       </c>
       <c r="B1" s="2" t="n"/>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>SAC @ IND</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="n"/>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>PHX @ MIN</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="n"/>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>SAS @ NOP</t>
+        </is>
+      </c>
+      <c r="K1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -528,6 +633,24 @@
         </is>
       </c>
       <c r="B2" s="2" t="n"/>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>LIVE / 2025-12-08</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="n"/>
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>LIVE / 2025-12-08</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="n"/>
+      <c r="J2" s="3" t="inlineStr">
+        <is>
+          <t>LIVE / 2025-12-08</t>
+        </is>
+      </c>
+      <c r="K2" s="2" t="n"/>
     </row>
     <row r="3" ht="112.5" customHeight="1"/>
     <row r="4">
@@ -536,13 +659,40 @@
           <t>Captured: 07:39 PM</t>
         </is>
       </c>
+      <c r="D4" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 08:41 PM</t>
+        </is>
+      </c>
+      <c r="G4" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 08:41 PM</t>
+        </is>
+      </c>
+      <c r="J4" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 08:41 PM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="16">
     <mergeCell ref="A4:B4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D3:E3"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="G3:H3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-09 06:16 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="2025-12-08" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="2025-12-09" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -232,6 +233,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -257,6 +261,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -276,6 +283,64 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>2</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>2</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -697,4 +762,83 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="25" customWidth="1" min="1" max="1"/>
+    <col width="25" customWidth="1" min="2" max="2"/>
+    <col width="3" customWidth="1" min="3" max="3"/>
+    <col width="25" customWidth="1" min="4" max="4"/>
+    <col width="25" customWidth="1" min="5" max="5"/>
+    <col width="3" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>MIA @ ORL</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="n"/>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>NYK @ TOR</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>11:00 PM / 2025-12-09</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n"/>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>1:30 AM / 2025-12-09</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="n"/>
+    </row>
+    <row r="3" ht="112.5" customHeight="1"/>
+    <row r="4">
+      <c r="A4" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 01:16 AM</t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 01:16 AM</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A3:B3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update NBA prices - 2025-12-09 07:14 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -322,6 +322,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -341,6 +344,59 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>2</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>2</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="4" name="Image 4" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -770,7 +826,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -784,6 +840,12 @@
     <col width="25" customWidth="1" min="4" max="4"/>
     <col width="25" customWidth="1" min="5" max="5"/>
     <col width="3" customWidth="1" min="6" max="6"/>
+    <col width="25" customWidth="1" min="7" max="7"/>
+    <col width="25" customWidth="1" min="8" max="8"/>
+    <col width="3" customWidth="1" min="9" max="9"/>
+    <col width="25" customWidth="1" min="10" max="10"/>
+    <col width="25" customWidth="1" min="11" max="11"/>
+    <col width="3" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -799,6 +861,18 @@
         </is>
       </c>
       <c r="E1" s="2" t="n"/>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>MIA @ ORL</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="n"/>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>NYK @ TOR</t>
+        </is>
+      </c>
+      <c r="K1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -813,6 +887,18 @@
         </is>
       </c>
       <c r="E2" s="2" t="n"/>
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>11:00 PM / 2025-12-09</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="n"/>
+      <c r="J2" s="3" t="inlineStr">
+        <is>
+          <t>1:30 AM / 2025-12-09</t>
+        </is>
+      </c>
+      <c r="K2" s="2" t="n"/>
     </row>
     <row r="3" ht="112.5" customHeight="1"/>
     <row r="4">
@@ -826,17 +912,35 @@
           <t>Captured: 01:16 AM</t>
         </is>
       </c>
+      <c r="G4" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 02:14 AM</t>
+        </is>
+      </c>
+      <c r="J4" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 02:14 AM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="16">
     <mergeCell ref="A4:B4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="J1:K1"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="A3:B3"/>
+    <mergeCell ref="G3:H3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-09 08:15 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -378,6 +378,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -397,6 +400,59 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>12</col>
+      <colOff>0</colOff>
+      <row>2</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="5" name="Image 5" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>15</col>
+      <colOff>0</colOff>
+      <row>2</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="6" name="Image 6" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -826,7 +882,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -846,6 +902,12 @@
     <col width="25" customWidth="1" min="10" max="10"/>
     <col width="25" customWidth="1" min="11" max="11"/>
     <col width="3" customWidth="1" min="12" max="12"/>
+    <col width="25" customWidth="1" min="13" max="13"/>
+    <col width="25" customWidth="1" min="14" max="14"/>
+    <col width="3" customWidth="1" min="15" max="15"/>
+    <col width="25" customWidth="1" min="16" max="16"/>
+    <col width="25" customWidth="1" min="17" max="17"/>
+    <col width="3" customWidth="1" min="18" max="18"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -873,6 +935,18 @@
         </is>
       </c>
       <c r="K1" s="2" t="n"/>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>MIA @ ORL</t>
+        </is>
+      </c>
+      <c r="N1" s="2" t="n"/>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>NYK @ TOR</t>
+        </is>
+      </c>
+      <c r="Q1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -899,6 +973,18 @@
         </is>
       </c>
       <c r="K2" s="2" t="n"/>
+      <c r="M2" s="3" t="inlineStr">
+        <is>
+          <t>11:00 PM / 2025-12-09</t>
+        </is>
+      </c>
+      <c r="N2" s="2" t="n"/>
+      <c r="P2" s="3" t="inlineStr">
+        <is>
+          <t>1:30 AM / 2025-12-09</t>
+        </is>
+      </c>
+      <c r="Q2" s="2" t="n"/>
     </row>
     <row r="3" ht="112.5" customHeight="1"/>
     <row r="4">
@@ -922,25 +1008,43 @@
           <t>Captured: 02:14 AM</t>
         </is>
       </c>
+      <c r="M4" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 03:15 AM</t>
+        </is>
+      </c>
+      <c r="P4" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 03:15 AM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="24">
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="D3:E3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="P3:Q3"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J2:K2"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="M4:N4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-09 09:14 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -434,6 +434,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -453,6 +456,59 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>18</col>
+      <colOff>0</colOff>
+      <row>2</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="7" name="Image 7" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>21</col>
+      <colOff>0</colOff>
+      <row>2</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="8" name="Image 8" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId8"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -882,7 +938,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -908,6 +964,12 @@
     <col width="25" customWidth="1" min="16" max="16"/>
     <col width="25" customWidth="1" min="17" max="17"/>
     <col width="3" customWidth="1" min="18" max="18"/>
+    <col width="25" customWidth="1" min="19" max="19"/>
+    <col width="25" customWidth="1" min="20" max="20"/>
+    <col width="3" customWidth="1" min="21" max="21"/>
+    <col width="25" customWidth="1" min="22" max="22"/>
+    <col width="25" customWidth="1" min="23" max="23"/>
+    <col width="3" customWidth="1" min="24" max="24"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -947,6 +1009,18 @@
         </is>
       </c>
       <c r="Q1" s="2" t="n"/>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>MIA @ ORL</t>
+        </is>
+      </c>
+      <c r="T1" s="2" t="n"/>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>NYK @ TOR</t>
+        </is>
+      </c>
+      <c r="W1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -985,6 +1059,18 @@
         </is>
       </c>
       <c r="Q2" s="2" t="n"/>
+      <c r="S2" s="3" t="inlineStr">
+        <is>
+          <t>11:00 PM / 2025-12-09</t>
+        </is>
+      </c>
+      <c r="T2" s="2" t="n"/>
+      <c r="V2" s="3" t="inlineStr">
+        <is>
+          <t>1:30 AM / 2025-12-09</t>
+        </is>
+      </c>
+      <c r="W2" s="2" t="n"/>
     </row>
     <row r="3" ht="112.5" customHeight="1"/>
     <row r="4">
@@ -1018,18 +1104,33 @@
           <t>Captured: 03:15 AM</t>
         </is>
       </c>
+      <c r="S4" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 04:14 AM</t>
+        </is>
+      </c>
+      <c r="V4" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 04:14 AM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="32">
     <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="V2:W2"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="M1:N1"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="V4:W4"/>
     <mergeCell ref="M2:N2"/>
+    <mergeCell ref="S2:T2"/>
     <mergeCell ref="D2:E2"/>
+    <mergeCell ref="V1:W1"/>
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="G3:H3"/>
@@ -1044,7 +1145,10 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J2:K2"/>
+    <mergeCell ref="S1:T1"/>
     <mergeCell ref="M4:N4"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="V3:W3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-09 10:13 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -39,6 +39,11 @@
       <i val="1"/>
       <color rgb="00666666"/>
       <sz val="9"/>
+    </font>
+    <font>
+      <color rgb="000066CC"/>
+      <sz val="8"/>
+      <u val="single"/>
     </font>
   </fonts>
   <fills count="3">
@@ -94,7 +99,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -104,6 +109,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -490,6 +498,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -509,6 +520,59 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>24</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="9" name="Image 9" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>27</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="10" name="Image 10" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId10"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -938,7 +1002,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:AC5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -970,6 +1034,12 @@
     <col width="25" customWidth="1" min="22" max="22"/>
     <col width="25" customWidth="1" min="23" max="23"/>
     <col width="3" customWidth="1" min="24" max="24"/>
+    <col width="25" customWidth="1" min="25" max="25"/>
+    <col width="25" customWidth="1" min="26" max="26"/>
+    <col width="3" customWidth="1" min="27" max="27"/>
+    <col width="25" customWidth="1" min="28" max="28"/>
+    <col width="25" customWidth="1" min="29" max="29"/>
+    <col width="3" customWidth="1" min="30" max="30"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1021,6 +1091,18 @@
         </is>
       </c>
       <c r="W1" s="2" t="n"/>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>MIA @ ORL</t>
+        </is>
+      </c>
+      <c r="Z1" s="2" t="n"/>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>NYK @ TOR</t>
+        </is>
+      </c>
+      <c r="AC1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -1071,9 +1153,32 @@
         </is>
       </c>
       <c r="W2" s="2" t="n"/>
+      <c r="Y2" s="3" t="inlineStr">
+        <is>
+          <t>11:00 PM / 2025-12-09</t>
+        </is>
+      </c>
+      <c r="Z2" s="2" t="n"/>
+      <c r="AB2" s="3" t="inlineStr">
+        <is>
+          <t>1:30 AM / 2025-12-09</t>
+        </is>
+      </c>
+      <c r="AC2" s="2" t="n"/>
     </row>
-    <row r="3" ht="112.5" customHeight="1"/>
-    <row r="4">
+    <row r="3" ht="112.5" customHeight="1">
+      <c r="Y3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-mia-orl-2025-12-09</t>
+        </is>
+      </c>
+      <c r="AB3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-nyk-tor-2025-12-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="112.5" customHeight="1">
       <c r="A4" s="4" t="inlineStr">
         <is>
           <t>Captured: 01:16 AM</t>
@@ -1112,30 +1217,51 @@
       <c r="V4" s="4" t="inlineStr">
         <is>
           <t>Captured: 04:14 AM</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="Y5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 05:13 AM</t>
+        </is>
+      </c>
+      <c r="AB5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 05:13 AM</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="42">
     <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="Y4:Z4"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G2:H2"/>
+    <mergeCell ref="Y3:Z3"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="AB5:AC5"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="S3:T3"/>
+    <mergeCell ref="AB4:AC4"/>
     <mergeCell ref="V4:W4"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="S2:T2"/>
+    <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="V1:W1"/>
+    <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="Y1:Z1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="A2:B2"/>
+    <mergeCell ref="AB2:AC2"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="D3:E3"/>
@@ -1149,6 +1275,7 @@
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="S4:T4"/>
     <mergeCell ref="V3:W3"/>
+    <mergeCell ref="AB3:AC3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-09 11:11 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -554,6 +554,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -573,6 +576,59 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>30</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="11" name="Image 11" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>33</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="12" name="Image 12" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId12"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1002,7 +1058,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC5"/>
+  <dimension ref="A1:AI5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1040,6 +1096,12 @@
     <col width="25" customWidth="1" min="28" max="28"/>
     <col width="25" customWidth="1" min="29" max="29"/>
     <col width="3" customWidth="1" min="30" max="30"/>
+    <col width="25" customWidth="1" min="31" max="31"/>
+    <col width="25" customWidth="1" min="32" max="32"/>
+    <col width="3" customWidth="1" min="33" max="33"/>
+    <col width="25" customWidth="1" min="34" max="34"/>
+    <col width="25" customWidth="1" min="35" max="35"/>
+    <col width="3" customWidth="1" min="36" max="36"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1103,6 +1165,18 @@
         </is>
       </c>
       <c r="AC1" s="2" t="n"/>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>MIA @ ORL</t>
+        </is>
+      </c>
+      <c r="AF1" s="2" t="n"/>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>NYK @ TOR</t>
+        </is>
+      </c>
+      <c r="AI1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -1165,6 +1239,18 @@
         </is>
       </c>
       <c r="AC2" s="2" t="n"/>
+      <c r="AE2" s="3" t="inlineStr">
+        <is>
+          <t>11:00 PM / 2025-12-09</t>
+        </is>
+      </c>
+      <c r="AF2" s="2" t="n"/>
+      <c r="AH2" s="3" t="inlineStr">
+        <is>
+          <t>1:30 AM / 2025-12-09</t>
+        </is>
+      </c>
+      <c r="AI2" s="2" t="n"/>
     </row>
     <row r="3" ht="112.5" customHeight="1">
       <c r="Y3" s="5" t="inlineStr">
@@ -1177,6 +1263,16 @@
           <t>https://polymarket.com/event/nba-nyk-tor-2025-12-09</t>
         </is>
       </c>
+      <c r="AE3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-mia-orl-2025-12-09</t>
+        </is>
+      </c>
+      <c r="AH3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-nyk-tor-2025-12-09</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="112.5" customHeight="1">
       <c r="A4" s="4" t="inlineStr">
@@ -1231,12 +1327,23 @@
           <t>Captured: 05:13 AM</t>
         </is>
       </c>
+      <c r="AE5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 06:11 AM</t>
+        </is>
+      </c>
+      <c r="AH5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 06:11 AM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="42">
+  <mergeCells count="52">
     <mergeCell ref="P4:Q4"/>
     <mergeCell ref="Y4:Z4"/>
     <mergeCell ref="V2:W2"/>
+    <mergeCell ref="AH3:AI3"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="Y3:Z3"/>
@@ -1245,15 +1352,21 @@
     <mergeCell ref="AB5:AC5"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="M1:N1"/>
+    <mergeCell ref="AH5:AI5"/>
     <mergeCell ref="S3:T3"/>
     <mergeCell ref="AB4:AC4"/>
     <mergeCell ref="V4:W4"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="S2:T2"/>
+    <mergeCell ref="AE3:AF3"/>
     <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="D2:E2"/>
+    <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="AH4:AI4"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="AE2:AF2"/>
+    <mergeCell ref="AH1:AI1"/>
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="Y5:Z5"/>
     <mergeCell ref="Y1:Z1"/>
@@ -1262,6 +1375,7 @@
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="D3:E3"/>
@@ -1269,9 +1383,11 @@
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="AH2:AI2"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="S1:T1"/>
+    <mergeCell ref="AE5:AF5"/>
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="S4:T4"/>
     <mergeCell ref="V3:W3"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-09 12:18 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -610,6 +610,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -629,6 +632,59 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>36</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="13" name="Image 13" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>39</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="14" name="Image 14" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId14"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1058,7 +1114,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AI5"/>
+  <dimension ref="A1:AO5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1102,6 +1158,12 @@
     <col width="25" customWidth="1" min="34" max="34"/>
     <col width="25" customWidth="1" min="35" max="35"/>
     <col width="3" customWidth="1" min="36" max="36"/>
+    <col width="25" customWidth="1" min="37" max="37"/>
+    <col width="25" customWidth="1" min="38" max="38"/>
+    <col width="3" customWidth="1" min="39" max="39"/>
+    <col width="25" customWidth="1" min="40" max="40"/>
+    <col width="25" customWidth="1" min="41" max="41"/>
+    <col width="3" customWidth="1" min="42" max="42"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1177,6 +1239,18 @@
         </is>
       </c>
       <c r="AI1" s="2" t="n"/>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>MIA @ ORL</t>
+        </is>
+      </c>
+      <c r="AL1" s="2" t="n"/>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>NYK @ TOR</t>
+        </is>
+      </c>
+      <c r="AO1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -1251,6 +1325,18 @@
         </is>
       </c>
       <c r="AI2" s="2" t="n"/>
+      <c r="AK2" s="3" t="inlineStr">
+        <is>
+          <t>11:00 PM / 2025-12-09</t>
+        </is>
+      </c>
+      <c r="AL2" s="2" t="n"/>
+      <c r="AN2" s="3" t="inlineStr">
+        <is>
+          <t>1:30 AM / 2025-12-09</t>
+        </is>
+      </c>
+      <c r="AO2" s="2" t="n"/>
     </row>
     <row r="3" ht="112.5" customHeight="1">
       <c r="Y3" s="5" t="inlineStr">
@@ -1273,6 +1359,16 @@
           <t>https://polymarket.com/event/nba-nyk-tor-2025-12-09</t>
         </is>
       </c>
+      <c r="AK3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-mia-orl-2025-12-09</t>
+        </is>
+      </c>
+      <c r="AN3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-nyk-tor-2025-12-09</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="112.5" customHeight="1">
       <c r="A4" s="4" t="inlineStr">
@@ -1337,13 +1433,24 @@
           <t>Captured: 06:11 AM</t>
         </is>
       </c>
+      <c r="AK5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 07:18 AM</t>
+        </is>
+      </c>
+      <c r="AN5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 07:18 AM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="52">
+  <mergeCells count="62">
     <mergeCell ref="P4:Q4"/>
     <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="AH3:AI3"/>
     <mergeCell ref="V2:W2"/>
-    <mergeCell ref="AH3:AI3"/>
+    <mergeCell ref="AN3:AO3"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="Y3:Z3"/>
@@ -1355,14 +1462,18 @@
     <mergeCell ref="AH5:AI5"/>
     <mergeCell ref="S3:T3"/>
     <mergeCell ref="AB4:AC4"/>
+    <mergeCell ref="AN5:AO5"/>
+    <mergeCell ref="AK4:AL4"/>
     <mergeCell ref="V4:W4"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="AE3:AF3"/>
     <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="D2:E2"/>
+    <mergeCell ref="AH4:AI4"/>
     <mergeCell ref="AE4:AF4"/>
-    <mergeCell ref="AH4:AI4"/>
+    <mergeCell ref="AK3:AL3"/>
+    <mergeCell ref="AN4:AO4"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="AE2:AF2"/>
@@ -1370,13 +1481,17 @@
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="Y5:Z5"/>
     <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AN1:AO1"/>
+    <mergeCell ref="AK5:AL5"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AK1:AL1"/>
     <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="D4:E4"/>
+    <mergeCell ref="AN2:AO2"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="A4:B4"/>
@@ -1387,6 +1502,7 @@
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="S1:T1"/>
+    <mergeCell ref="AK2:AL2"/>
     <mergeCell ref="AE5:AF5"/>
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="S4:T4"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-09 13:23 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -666,6 +666,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -685,6 +688,59 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>42</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="15" name="Image 15" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>45</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="16" name="Image 16" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId16"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1114,7 +1170,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AO5"/>
+  <dimension ref="A1:AU5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1164,6 +1220,12 @@
     <col width="25" customWidth="1" min="40" max="40"/>
     <col width="25" customWidth="1" min="41" max="41"/>
     <col width="3" customWidth="1" min="42" max="42"/>
+    <col width="25" customWidth="1" min="43" max="43"/>
+    <col width="25" customWidth="1" min="44" max="44"/>
+    <col width="3" customWidth="1" min="45" max="45"/>
+    <col width="25" customWidth="1" min="46" max="46"/>
+    <col width="25" customWidth="1" min="47" max="47"/>
+    <col width="3" customWidth="1" min="48" max="48"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1251,6 +1313,18 @@
         </is>
       </c>
       <c r="AO1" s="2" t="n"/>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>MIA @ ORL</t>
+        </is>
+      </c>
+      <c r="AR1" s="2" t="n"/>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>NYK @ TOR</t>
+        </is>
+      </c>
+      <c r="AU1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -1337,6 +1411,18 @@
         </is>
       </c>
       <c r="AO2" s="2" t="n"/>
+      <c r="AQ2" s="3" t="inlineStr">
+        <is>
+          <t>11:00 PM / 2025-12-09</t>
+        </is>
+      </c>
+      <c r="AR2" s="2" t="n"/>
+      <c r="AT2" s="3" t="inlineStr">
+        <is>
+          <t>1:30 AM / 2025-12-09</t>
+        </is>
+      </c>
+      <c r="AU2" s="2" t="n"/>
     </row>
     <row r="3" ht="112.5" customHeight="1">
       <c r="Y3" s="5" t="inlineStr">
@@ -1369,6 +1455,16 @@
           <t>https://polymarket.com/event/nba-nyk-tor-2025-12-09</t>
         </is>
       </c>
+      <c r="AQ3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-mia-orl-2025-12-09</t>
+        </is>
+      </c>
+      <c r="AT3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-nyk-tor-2025-12-09</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="112.5" customHeight="1">
       <c r="A4" s="4" t="inlineStr">
@@ -1443,13 +1539,23 @@
           <t>Captured: 07:18 AM</t>
         </is>
       </c>
+      <c r="AQ5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 08:23 AM</t>
+        </is>
+      </c>
+      <c r="AT5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 08:23 AM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="62">
+  <mergeCells count="72">
     <mergeCell ref="P4:Q4"/>
     <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="V2:W2"/>
     <mergeCell ref="AH3:AI3"/>
-    <mergeCell ref="V2:W2"/>
     <mergeCell ref="AN3:AO3"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G2:H2"/>
@@ -1461,9 +1567,10 @@
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="AH5:AI5"/>
     <mergeCell ref="S3:T3"/>
+    <mergeCell ref="AN5:AO5"/>
     <mergeCell ref="AB4:AC4"/>
-    <mergeCell ref="AN5:AO5"/>
     <mergeCell ref="AK4:AL4"/>
+    <mergeCell ref="AT3:AU3"/>
     <mergeCell ref="V4:W4"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="S2:T2"/>
@@ -1471,9 +1578,9 @@
     <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="AH4:AI4"/>
-    <mergeCell ref="AE4:AF4"/>
     <mergeCell ref="AK3:AL3"/>
     <mergeCell ref="AN4:AO4"/>
+    <mergeCell ref="AE4:AF4"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="AE2:AF2"/>
@@ -1482,18 +1589,25 @@
     <mergeCell ref="Y5:Z5"/>
     <mergeCell ref="Y1:Z1"/>
     <mergeCell ref="AN1:AO1"/>
+    <mergeCell ref="AQ3:AR3"/>
+    <mergeCell ref="AT5:AU5"/>
     <mergeCell ref="AK5:AL5"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="G3:H3"/>
+    <mergeCell ref="AT4:AU4"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="A2:B2"/>
+    <mergeCell ref="AQ2:AR2"/>
     <mergeCell ref="AB2:AC2"/>
     <mergeCell ref="AK1:AL1"/>
     <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="AN2:AO2"/>
     <mergeCell ref="M3:N3"/>
+    <mergeCell ref="AQ1:AR1"/>
+    <mergeCell ref="AQ5:AR5"/>
     <mergeCell ref="D3:E3"/>
+    <mergeCell ref="AQ4:AR4"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="J3:K3"/>
@@ -1502,8 +1616,10 @@
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="S1:T1"/>
+    <mergeCell ref="AT2:AU2"/>
     <mergeCell ref="AK2:AL2"/>
     <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AT1:AU1"/>
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="S4:T4"/>
     <mergeCell ref="V3:W3"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-09 15:12 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -722,6 +722,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -741,6 +744,59 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>48</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="17" name="Image 17" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>51</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="18" name="Image 18" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId18"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1170,7 +1226,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AU5"/>
+  <dimension ref="A1:BA5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1226,6 +1282,12 @@
     <col width="25" customWidth="1" min="46" max="46"/>
     <col width="25" customWidth="1" min="47" max="47"/>
     <col width="3" customWidth="1" min="48" max="48"/>
+    <col width="25" customWidth="1" min="49" max="49"/>
+    <col width="25" customWidth="1" min="50" max="50"/>
+    <col width="3" customWidth="1" min="51" max="51"/>
+    <col width="25" customWidth="1" min="52" max="52"/>
+    <col width="25" customWidth="1" min="53" max="53"/>
+    <col width="3" customWidth="1" min="54" max="54"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1325,6 +1387,18 @@
         </is>
       </c>
       <c r="AU1" s="2" t="n"/>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>MIA @ ORL</t>
+        </is>
+      </c>
+      <c r="AX1" s="2" t="n"/>
+      <c r="AZ1" s="1" t="inlineStr">
+        <is>
+          <t>NYK @ TOR</t>
+        </is>
+      </c>
+      <c r="BA1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -1423,6 +1497,18 @@
         </is>
       </c>
       <c r="AU2" s="2" t="n"/>
+      <c r="AW2" s="3" t="inlineStr">
+        <is>
+          <t>11:00 PM / 2025-12-09</t>
+        </is>
+      </c>
+      <c r="AX2" s="2" t="n"/>
+      <c r="AZ2" s="3" t="inlineStr">
+        <is>
+          <t>1:30 AM / 2025-12-09</t>
+        </is>
+      </c>
+      <c r="BA2" s="2" t="n"/>
     </row>
     <row r="3" ht="112.5" customHeight="1">
       <c r="Y3" s="5" t="inlineStr">
@@ -1465,6 +1551,16 @@
           <t>https://polymarket.com/event/nba-nyk-tor-2025-12-09</t>
         </is>
       </c>
+      <c r="AW3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-mia-orl-2025-12-09</t>
+        </is>
+      </c>
+      <c r="AZ3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-nyk-tor-2025-12-09</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="112.5" customHeight="1">
       <c r="A4" s="4" t="inlineStr">
@@ -1549,81 +1645,101 @@
           <t>Captured: 08:23 AM</t>
         </is>
       </c>
+      <c r="AW5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 10:12 AM</t>
+        </is>
+      </c>
+      <c r="AZ5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 10:12 AM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="72">
-    <mergeCell ref="P4:Q4"/>
+  <mergeCells count="82">
     <mergeCell ref="Y4:Z4"/>
     <mergeCell ref="V2:W2"/>
-    <mergeCell ref="AH3:AI3"/>
     <mergeCell ref="AN3:AO3"/>
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="AN5:AO5"/>
+    <mergeCell ref="AT3:AU3"/>
+    <mergeCell ref="AW4:AX4"/>
+    <mergeCell ref="AZ5:BA5"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AT5:AU5"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="AQ2:AR2"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="AQ1:AR1"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AT1:AU1"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="AZ1:BA1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="AK4:AL4"/>
+    <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="AH1:AI1"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="AK1:AL1"/>
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="AW1:AX1"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="P4:Q4"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="Y3:Z3"/>
-    <mergeCell ref="J1:K1"/>
     <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="AB5:AC5"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="AH5:AI5"/>
     <mergeCell ref="S3:T3"/>
-    <mergeCell ref="AN5:AO5"/>
-    <mergeCell ref="AB4:AC4"/>
-    <mergeCell ref="AK4:AL4"/>
-    <mergeCell ref="AT3:AU3"/>
-    <mergeCell ref="V4:W4"/>
     <mergeCell ref="M2:N2"/>
-    <mergeCell ref="S2:T2"/>
     <mergeCell ref="AE3:AF3"/>
+    <mergeCell ref="AH4:AI4"/>
     <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="AH4:AI4"/>
-    <mergeCell ref="AK3:AL3"/>
-    <mergeCell ref="AN4:AO4"/>
-    <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="AW3:AX3"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="AE2:AF2"/>
-    <mergeCell ref="AH1:AI1"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AQ3:AR3"/>
     <mergeCell ref="AN1:AO1"/>
-    <mergeCell ref="AQ3:AR3"/>
-    <mergeCell ref="AT5:AU5"/>
-    <mergeCell ref="AK5:AL5"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="AT4:AU4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="AQ2:AR2"/>
+    <mergeCell ref="AW5:AX5"/>
     <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AK1:AL1"/>
-    <mergeCell ref="AE1:AF1"/>
-    <mergeCell ref="D4:E4"/>
     <mergeCell ref="AN2:AO2"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="AQ1:AR1"/>
-    <mergeCell ref="AQ5:AR5"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="AQ4:AR4"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="J3:K3"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="AZ3:BA3"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J2:K2"/>
-    <mergeCell ref="S1:T1"/>
     <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AK2:AL2"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AT1:AU1"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="AH3:AI3"/>
+    <mergeCell ref="AW2:AX2"/>
+    <mergeCell ref="AH5:AI5"/>
+    <mergeCell ref="AB4:AC4"/>
+    <mergeCell ref="V4:W4"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="AK3:AL3"/>
+    <mergeCell ref="AN4:AO4"/>
+    <mergeCell ref="AE2:AF2"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="AT4:AU4"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="AQ5:AR5"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="AZ2:BA2"/>
     <mergeCell ref="M4:N4"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="AE4:AF4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-09 16:14 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -778,6 +778,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -797,6 +800,59 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>54</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="19" name="Image 19" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>57</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="20" name="Image 20" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId20"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1226,7 +1282,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BA5"/>
+  <dimension ref="A1:BG5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1288,6 +1344,12 @@
     <col width="25" customWidth="1" min="52" max="52"/>
     <col width="25" customWidth="1" min="53" max="53"/>
     <col width="3" customWidth="1" min="54" max="54"/>
+    <col width="25" customWidth="1" min="55" max="55"/>
+    <col width="25" customWidth="1" min="56" max="56"/>
+    <col width="3" customWidth="1" min="57" max="57"/>
+    <col width="25" customWidth="1" min="58" max="58"/>
+    <col width="25" customWidth="1" min="59" max="59"/>
+    <col width="3" customWidth="1" min="60" max="60"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1399,6 +1461,18 @@
         </is>
       </c>
       <c r="BA1" s="2" t="n"/>
+      <c r="BC1" s="1" t="inlineStr">
+        <is>
+          <t>MIA @ ORL</t>
+        </is>
+      </c>
+      <c r="BD1" s="2" t="n"/>
+      <c r="BF1" s="1" t="inlineStr">
+        <is>
+          <t>NYK @ TOR</t>
+        </is>
+      </c>
+      <c r="BG1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -1509,6 +1583,18 @@
         </is>
       </c>
       <c r="BA2" s="2" t="n"/>
+      <c r="BC2" s="3" t="inlineStr">
+        <is>
+          <t>11:00 PM / 2025-12-09</t>
+        </is>
+      </c>
+      <c r="BD2" s="2" t="n"/>
+      <c r="BF2" s="3" t="inlineStr">
+        <is>
+          <t>1:30 AM / 2025-12-09</t>
+        </is>
+      </c>
+      <c r="BG2" s="2" t="n"/>
     </row>
     <row r="3" ht="112.5" customHeight="1">
       <c r="Y3" s="5" t="inlineStr">
@@ -1561,6 +1647,16 @@
           <t>https://polymarket.com/event/nba-nyk-tor-2025-12-09</t>
         </is>
       </c>
+      <c r="BC3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-mia-orl-2025-12-09</t>
+        </is>
+      </c>
+      <c r="BF3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-nyk-tor-2025-12-09</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="112.5" customHeight="1">
       <c r="A4" s="4" t="inlineStr">
@@ -1655,9 +1751,19 @@
           <t>Captured: 10:12 AM</t>
         </is>
       </c>
+      <c r="BC5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 11:14 AM</t>
+        </is>
+      </c>
+      <c r="BF5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 11:14 AM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="82">
+  <mergeCells count="92">
     <mergeCell ref="Y4:Z4"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="AN3:AO3"/>
@@ -1676,6 +1782,7 @@
     <mergeCell ref="AE5:AF5"/>
     <mergeCell ref="AT1:AU1"/>
     <mergeCell ref="S4:T4"/>
+    <mergeCell ref="BF1:BG1"/>
     <mergeCell ref="AZ1:BA1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="M1:N1"/>
@@ -1689,12 +1796,14 @@
     <mergeCell ref="AW1:AX1"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="S1:T1"/>
+    <mergeCell ref="BC1:BD1"/>
     <mergeCell ref="AK2:AL2"/>
     <mergeCell ref="P4:Q4"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="Y3:Z3"/>
     <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="BC2:BD2"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="S3:T3"/>
     <mergeCell ref="M2:N2"/>
@@ -1710,21 +1819,26 @@
     <mergeCell ref="AW5:AX5"/>
     <mergeCell ref="AB2:AC2"/>
     <mergeCell ref="AN2:AO2"/>
+    <mergeCell ref="BC5:BD5"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="AQ4:AR4"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="AH2:AI2"/>
     <mergeCell ref="AZ3:BA3"/>
+    <mergeCell ref="BC4:BD4"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="BF5:BG5"/>
+    <mergeCell ref="BF2:BG2"/>
     <mergeCell ref="V3:W3"/>
     <mergeCell ref="AH3:AI3"/>
     <mergeCell ref="AW2:AX2"/>
     <mergeCell ref="AH5:AI5"/>
     <mergeCell ref="AB4:AC4"/>
     <mergeCell ref="V4:W4"/>
+    <mergeCell ref="BF3:BG3"/>
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="AK3:AL3"/>
     <mergeCell ref="AN4:AO4"/>
@@ -1734,6 +1848,8 @@
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="AT4:AU4"/>
     <mergeCell ref="A2:B2"/>
+    <mergeCell ref="BC3:BD3"/>
+    <mergeCell ref="BF4:BG4"/>
     <mergeCell ref="AQ5:AR5"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="G4:H4"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-09 17:12 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -834,6 +834,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -853,6 +856,59 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>60</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="21" name="Image 21" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>63</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="22" name="Image 22" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId22"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1282,7 +1338,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BG5"/>
+  <dimension ref="A1:BM5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1350,6 +1406,12 @@
     <col width="25" customWidth="1" min="58" max="58"/>
     <col width="25" customWidth="1" min="59" max="59"/>
     <col width="3" customWidth="1" min="60" max="60"/>
+    <col width="25" customWidth="1" min="61" max="61"/>
+    <col width="25" customWidth="1" min="62" max="62"/>
+    <col width="3" customWidth="1" min="63" max="63"/>
+    <col width="25" customWidth="1" min="64" max="64"/>
+    <col width="25" customWidth="1" min="65" max="65"/>
+    <col width="3" customWidth="1" min="66" max="66"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1473,6 +1535,18 @@
         </is>
       </c>
       <c r="BG1" s="2" t="n"/>
+      <c r="BI1" s="1" t="inlineStr">
+        <is>
+          <t>MIA @ ORL</t>
+        </is>
+      </c>
+      <c r="BJ1" s="2" t="n"/>
+      <c r="BL1" s="1" t="inlineStr">
+        <is>
+          <t>NYK @ TOR</t>
+        </is>
+      </c>
+      <c r="BM1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -1595,6 +1669,18 @@
         </is>
       </c>
       <c r="BG2" s="2" t="n"/>
+      <c r="BI2" s="3" t="inlineStr">
+        <is>
+          <t>11:00 PM / 2025-12-09</t>
+        </is>
+      </c>
+      <c r="BJ2" s="2" t="n"/>
+      <c r="BL2" s="3" t="inlineStr">
+        <is>
+          <t>1:30 AM / 2025-12-09</t>
+        </is>
+      </c>
+      <c r="BM2" s="2" t="n"/>
     </row>
     <row r="3" ht="112.5" customHeight="1">
       <c r="Y3" s="5" t="inlineStr">
@@ -1657,6 +1743,16 @@
           <t>https://polymarket.com/event/nba-nyk-tor-2025-12-09</t>
         </is>
       </c>
+      <c r="BI3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-mia-orl-2025-12-09</t>
+        </is>
+      </c>
+      <c r="BL3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-nyk-tor-2025-12-09</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="112.5" customHeight="1">
       <c r="A4" s="4" t="inlineStr">
@@ -1761,9 +1857,19 @@
           <t>Captured: 11:14 AM</t>
         </is>
       </c>
+      <c r="BI5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 12:12 PM</t>
+        </is>
+      </c>
+      <c r="BL5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 12:12 PM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="92">
+  <mergeCells count="102">
     <mergeCell ref="Y4:Z4"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="AN3:AO3"/>
@@ -1777,6 +1883,7 @@
     <mergeCell ref="AZ4:BA4"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="AQ2:AR2"/>
+    <mergeCell ref="BL4:BM4"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="AQ1:AR1"/>
     <mergeCell ref="AE5:AF5"/>
@@ -1785,6 +1892,7 @@
     <mergeCell ref="BF1:BG1"/>
     <mergeCell ref="AZ1:BA1"/>
     <mergeCell ref="J1:K1"/>
+    <mergeCell ref="BL1:BM1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="AK4:AL4"/>
     <mergeCell ref="AB3:AC3"/>
@@ -1795,13 +1903,16 @@
     <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="AW1:AX1"/>
     <mergeCell ref="J3:K3"/>
+    <mergeCell ref="BL3:BM3"/>
     <mergeCell ref="S1:T1"/>
     <mergeCell ref="BC1:BD1"/>
     <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="BL5:BM5"/>
     <mergeCell ref="P4:Q4"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="Y3:Z3"/>
+    <mergeCell ref="BI2:BJ2"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="BC2:BD2"/>
     <mergeCell ref="A1:B1"/>
@@ -1830,6 +1941,8 @@
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="BI1:BJ1"/>
+    <mergeCell ref="BL2:BM2"/>
     <mergeCell ref="BF5:BG5"/>
     <mergeCell ref="BF2:BG2"/>
     <mergeCell ref="V3:W3"/>
@@ -1847,12 +1960,15 @@
     <mergeCell ref="AK5:AL5"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="AT4:AU4"/>
+    <mergeCell ref="BI3:BJ3"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="BC3:BD3"/>
     <mergeCell ref="BF4:BG4"/>
     <mergeCell ref="AQ5:AR5"/>
     <mergeCell ref="M3:N3"/>
+    <mergeCell ref="BI5:BJ5"/>
     <mergeCell ref="G4:H4"/>
+    <mergeCell ref="BI4:BJ4"/>
     <mergeCell ref="AZ2:BA2"/>
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="AE4:AF4"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-09 18:16 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -890,6 +890,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -909,6 +912,59 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>66</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="23" name="Image 23" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>69</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="24" name="Image 24" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId24"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1338,7 +1394,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BM5"/>
+  <dimension ref="A1:BS5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1412,6 +1468,12 @@
     <col width="25" customWidth="1" min="64" max="64"/>
     <col width="25" customWidth="1" min="65" max="65"/>
     <col width="3" customWidth="1" min="66" max="66"/>
+    <col width="25" customWidth="1" min="67" max="67"/>
+    <col width="25" customWidth="1" min="68" max="68"/>
+    <col width="3" customWidth="1" min="69" max="69"/>
+    <col width="25" customWidth="1" min="70" max="70"/>
+    <col width="25" customWidth="1" min="71" max="71"/>
+    <col width="3" customWidth="1" min="72" max="72"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1547,6 +1609,18 @@
         </is>
       </c>
       <c r="BM1" s="2" t="n"/>
+      <c r="BO1" s="1" t="inlineStr">
+        <is>
+          <t>MIA @ ORL</t>
+        </is>
+      </c>
+      <c r="BP1" s="2" t="n"/>
+      <c r="BR1" s="1" t="inlineStr">
+        <is>
+          <t>NYK @ TOR</t>
+        </is>
+      </c>
+      <c r="BS1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -1681,6 +1755,18 @@
         </is>
       </c>
       <c r="BM2" s="2" t="n"/>
+      <c r="BO2" s="3" t="inlineStr">
+        <is>
+          <t>11:00 PM / 2025-12-09</t>
+        </is>
+      </c>
+      <c r="BP2" s="2" t="n"/>
+      <c r="BR2" s="3" t="inlineStr">
+        <is>
+          <t>1:30 AM / 2025-12-09</t>
+        </is>
+      </c>
+      <c r="BS2" s="2" t="n"/>
     </row>
     <row r="3" ht="112.5" customHeight="1">
       <c r="Y3" s="5" t="inlineStr">
@@ -1753,6 +1839,16 @@
           <t>https://polymarket.com/event/nba-nyk-tor-2025-12-09</t>
         </is>
       </c>
+      <c r="BO3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-mia-orl-2025-12-09</t>
+        </is>
+      </c>
+      <c r="BR3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-nyk-tor-2025-12-09</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="112.5" customHeight="1">
       <c r="A4" s="4" t="inlineStr">
@@ -1867,13 +1963,25 @@
           <t>Captured: 12:12 PM</t>
         </is>
       </c>
+      <c r="BO5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 01:16 PM</t>
+        </is>
+      </c>
+      <c r="BR5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 01:16 PM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="102">
+  <mergeCells count="112">
+    <mergeCell ref="BO4:BP4"/>
     <mergeCell ref="Y4:Z4"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="AN3:AO3"/>
     <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="BR2:BS2"/>
     <mergeCell ref="AN5:AO5"/>
     <mergeCell ref="AT3:AU3"/>
     <mergeCell ref="AW4:AX4"/>
@@ -1886,6 +1994,7 @@
     <mergeCell ref="BL4:BM4"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="AQ1:AR1"/>
+    <mergeCell ref="BR4:BS4"/>
     <mergeCell ref="AE5:AF5"/>
     <mergeCell ref="AT1:AU1"/>
     <mergeCell ref="S4:T4"/>
@@ -1907,6 +2016,7 @@
     <mergeCell ref="S1:T1"/>
     <mergeCell ref="BC1:BD1"/>
     <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="BO1:BP1"/>
     <mergeCell ref="BL5:BM5"/>
     <mergeCell ref="P4:Q4"/>
     <mergeCell ref="D1:E1"/>
@@ -1916,6 +2026,7 @@
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="BC2:BD2"/>
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="BR1:BS1"/>
     <mergeCell ref="S3:T3"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="AE3:AF3"/>
@@ -1928,11 +2039,13 @@
     <mergeCell ref="AN1:AO1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="AW5:AX5"/>
+    <mergeCell ref="BO3:BP3"/>
     <mergeCell ref="AB2:AC2"/>
     <mergeCell ref="AN2:AO2"/>
     <mergeCell ref="BC5:BD5"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="AQ4:AR4"/>
+    <mergeCell ref="BO5:BP5"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="AH2:AI2"/>
@@ -1946,6 +2059,7 @@
     <mergeCell ref="BF5:BG5"/>
     <mergeCell ref="BF2:BG2"/>
     <mergeCell ref="V3:W3"/>
+    <mergeCell ref="BR5:BS5"/>
     <mergeCell ref="AH3:AI3"/>
     <mergeCell ref="AW2:AX2"/>
     <mergeCell ref="AH5:AI5"/>
@@ -1955,8 +2069,10 @@
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="AK3:AL3"/>
     <mergeCell ref="AN4:AO4"/>
+    <mergeCell ref="BR3:BS3"/>
     <mergeCell ref="AE2:AF2"/>
     <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="BO2:BP2"/>
     <mergeCell ref="AK5:AL5"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="AT4:AU4"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-09 19:11 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -946,6 +946,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -965,6 +968,59 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>72</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="25" name="Image 25" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>75</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="26" name="Image 26" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId26"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1394,7 +1450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BS5"/>
+  <dimension ref="A1:BY5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1474,6 +1530,12 @@
     <col width="25" customWidth="1" min="70" max="70"/>
     <col width="25" customWidth="1" min="71" max="71"/>
     <col width="3" customWidth="1" min="72" max="72"/>
+    <col width="25" customWidth="1" min="73" max="73"/>
+    <col width="25" customWidth="1" min="74" max="74"/>
+    <col width="3" customWidth="1" min="75" max="75"/>
+    <col width="25" customWidth="1" min="76" max="76"/>
+    <col width="25" customWidth="1" min="77" max="77"/>
+    <col width="3" customWidth="1" min="78" max="78"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1621,6 +1683,18 @@
         </is>
       </c>
       <c r="BS1" s="2" t="n"/>
+      <c r="BU1" s="1" t="inlineStr">
+        <is>
+          <t>MIA @ ORL</t>
+        </is>
+      </c>
+      <c r="BV1" s="2" t="n"/>
+      <c r="BX1" s="1" t="inlineStr">
+        <is>
+          <t>NYK @ TOR</t>
+        </is>
+      </c>
+      <c r="BY1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -1767,6 +1841,18 @@
         </is>
       </c>
       <c r="BS2" s="2" t="n"/>
+      <c r="BU2" s="3" t="inlineStr">
+        <is>
+          <t>11:00 PM / 2025-12-09</t>
+        </is>
+      </c>
+      <c r="BV2" s="2" t="n"/>
+      <c r="BX2" s="3" t="inlineStr">
+        <is>
+          <t>1:30 AM / 2025-12-09</t>
+        </is>
+      </c>
+      <c r="BY2" s="2" t="n"/>
     </row>
     <row r="3" ht="112.5" customHeight="1">
       <c r="Y3" s="5" t="inlineStr">
@@ -1849,6 +1935,16 @@
           <t>https://polymarket.com/event/nba-nyk-tor-2025-12-09</t>
         </is>
       </c>
+      <c r="BU3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-mia-orl-2025-12-09</t>
+        </is>
+      </c>
+      <c r="BX3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-nyk-tor-2025-12-09</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="112.5" customHeight="1">
       <c r="A4" s="4" t="inlineStr">
@@ -1973,9 +2069,19 @@
           <t>Captured: 01:16 PM</t>
         </is>
       </c>
+      <c r="BU5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 02:11 PM</t>
+        </is>
+      </c>
+      <c r="BX5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 02:11 PM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="112">
+  <mergeCells count="122">
     <mergeCell ref="BO4:BP4"/>
     <mergeCell ref="Y4:Z4"/>
     <mergeCell ref="V2:W2"/>
@@ -1988,6 +2094,7 @@
     <mergeCell ref="AZ5:BA5"/>
     <mergeCell ref="Y1:Z1"/>
     <mergeCell ref="AT5:AU5"/>
+    <mergeCell ref="BU1:BV1"/>
     <mergeCell ref="AZ4:BA4"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="AQ2:AR2"/>
@@ -2000,6 +2107,7 @@
     <mergeCell ref="S4:T4"/>
     <mergeCell ref="BF1:BG1"/>
     <mergeCell ref="AZ1:BA1"/>
+    <mergeCell ref="BU3:BV3"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="BL1:BM1"/>
     <mergeCell ref="M1:N1"/>
@@ -2009,12 +2117,14 @@
     <mergeCell ref="AH1:AI1"/>
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="AK1:AL1"/>
+    <mergeCell ref="BX2:BY2"/>
     <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="AW1:AX1"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="BL3:BM3"/>
     <mergeCell ref="S1:T1"/>
     <mergeCell ref="BC1:BD1"/>
+    <mergeCell ref="BX3:BY3"/>
     <mergeCell ref="AK2:AL2"/>
     <mergeCell ref="BO1:BP1"/>
     <mergeCell ref="BL5:BM5"/>
@@ -2027,6 +2137,7 @@
     <mergeCell ref="BC2:BD2"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="BR1:BS1"/>
+    <mergeCell ref="BU2:BV2"/>
     <mergeCell ref="S3:T3"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="AE3:AF3"/>
@@ -2037,6 +2148,7 @@
     <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="AQ3:AR3"/>
     <mergeCell ref="AN1:AO1"/>
+    <mergeCell ref="BX1:BY1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="AW5:AX5"/>
     <mergeCell ref="BO3:BP3"/>
@@ -2051,6 +2163,7 @@
     <mergeCell ref="AH2:AI2"/>
     <mergeCell ref="AZ3:BA3"/>
     <mergeCell ref="BC4:BD4"/>
+    <mergeCell ref="BU4:BV4"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="AT2:AU2"/>
@@ -2062,6 +2175,7 @@
     <mergeCell ref="BR5:BS5"/>
     <mergeCell ref="AH3:AI3"/>
     <mergeCell ref="AW2:AX2"/>
+    <mergeCell ref="BX5:BY5"/>
     <mergeCell ref="AH5:AI5"/>
     <mergeCell ref="AB4:AC4"/>
     <mergeCell ref="V4:W4"/>
@@ -2069,6 +2183,7 @@
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="AK3:AL3"/>
     <mergeCell ref="AN4:AO4"/>
+    <mergeCell ref="BX4:BY4"/>
     <mergeCell ref="BR3:BS3"/>
     <mergeCell ref="AE2:AF2"/>
     <mergeCell ref="Y5:Z5"/>
@@ -2083,6 +2198,7 @@
     <mergeCell ref="AQ5:AR5"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="BI5:BJ5"/>
+    <mergeCell ref="BU5:BV5"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="BI4:BJ4"/>
     <mergeCell ref="AZ2:BA2"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-09 20:25 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -1002,6 +1002,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -1021,6 +1024,59 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>78</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="27" name="Image 27" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>81</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="28" name="Image 28" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId28"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1450,7 +1506,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BY5"/>
+  <dimension ref="A1:CE5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1536,6 +1592,12 @@
     <col width="25" customWidth="1" min="76" max="76"/>
     <col width="25" customWidth="1" min="77" max="77"/>
     <col width="3" customWidth="1" min="78" max="78"/>
+    <col width="25" customWidth="1" min="79" max="79"/>
+    <col width="25" customWidth="1" min="80" max="80"/>
+    <col width="3" customWidth="1" min="81" max="81"/>
+    <col width="25" customWidth="1" min="82" max="82"/>
+    <col width="25" customWidth="1" min="83" max="83"/>
+    <col width="3" customWidth="1" min="84" max="84"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1695,6 +1757,18 @@
         </is>
       </c>
       <c r="BY1" s="2" t="n"/>
+      <c r="CA1" s="1" t="inlineStr">
+        <is>
+          <t>MIA @ ORL</t>
+        </is>
+      </c>
+      <c r="CB1" s="2" t="n"/>
+      <c r="CD1" s="1" t="inlineStr">
+        <is>
+          <t>NYK @ TOR</t>
+        </is>
+      </c>
+      <c r="CE1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -1853,6 +1927,18 @@
         </is>
       </c>
       <c r="BY2" s="2" t="n"/>
+      <c r="CA2" s="3" t="inlineStr">
+        <is>
+          <t>11:00 PM / 2025-12-09</t>
+        </is>
+      </c>
+      <c r="CB2" s="2" t="n"/>
+      <c r="CD2" s="3" t="inlineStr">
+        <is>
+          <t>1:30 AM / 2025-12-09</t>
+        </is>
+      </c>
+      <c r="CE2" s="2" t="n"/>
     </row>
     <row r="3" ht="112.5" customHeight="1">
       <c r="Y3" s="5" t="inlineStr">
@@ -1945,6 +2031,16 @@
           <t>https://polymarket.com/event/nba-nyk-tor-2025-12-09</t>
         </is>
       </c>
+      <c r="CA3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-mia-orl-2025-12-09</t>
+        </is>
+      </c>
+      <c r="CD3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-nyk-tor-2025-12-09</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="112.5" customHeight="1">
       <c r="A4" s="4" t="inlineStr">
@@ -2079,15 +2175,27 @@
           <t>Captured: 02:11 PM</t>
         </is>
       </c>
+      <c r="CA5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 03:25 PM</t>
+        </is>
+      </c>
+      <c r="CD5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 03:25 PM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="122">
+  <mergeCells count="132">
     <mergeCell ref="BO4:BP4"/>
     <mergeCell ref="Y4:Z4"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="AN3:AO3"/>
+    <mergeCell ref="CA4:CB4"/>
     <mergeCell ref="AB5:AC5"/>
     <mergeCell ref="BR2:BS2"/>
+    <mergeCell ref="CD5:CE5"/>
     <mergeCell ref="AN5:AO5"/>
     <mergeCell ref="AT3:AU3"/>
     <mergeCell ref="AW4:AX4"/>
@@ -2102,6 +2210,7 @@
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="AQ1:AR1"/>
     <mergeCell ref="BR4:BS4"/>
+    <mergeCell ref="CD4:CE4"/>
     <mergeCell ref="AE5:AF5"/>
     <mergeCell ref="AT1:AU1"/>
     <mergeCell ref="S4:T4"/>
@@ -2111,6 +2220,7 @@
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="BL1:BM1"/>
     <mergeCell ref="M1:N1"/>
+    <mergeCell ref="CD1:CE1"/>
     <mergeCell ref="AK4:AL4"/>
     <mergeCell ref="AB3:AC3"/>
     <mergeCell ref="D2:E2"/>
@@ -2149,10 +2259,12 @@
     <mergeCell ref="AQ3:AR3"/>
     <mergeCell ref="AN1:AO1"/>
     <mergeCell ref="BX1:BY1"/>
+    <mergeCell ref="CA2:CB2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="AW5:AX5"/>
     <mergeCell ref="BO3:BP3"/>
     <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="CD2:CE2"/>
     <mergeCell ref="AN2:AO2"/>
     <mergeCell ref="BC5:BD5"/>
     <mergeCell ref="D3:E3"/>
@@ -2169,12 +2281,14 @@
     <mergeCell ref="AT2:AU2"/>
     <mergeCell ref="BI1:BJ1"/>
     <mergeCell ref="BL2:BM2"/>
+    <mergeCell ref="CD3:CE3"/>
     <mergeCell ref="BF5:BG5"/>
     <mergeCell ref="BF2:BG2"/>
     <mergeCell ref="V3:W3"/>
     <mergeCell ref="BR5:BS5"/>
     <mergeCell ref="AH3:AI3"/>
     <mergeCell ref="AW2:AX2"/>
+    <mergeCell ref="CA1:CB1"/>
     <mergeCell ref="BX5:BY5"/>
     <mergeCell ref="AH5:AI5"/>
     <mergeCell ref="AB4:AC4"/>
@@ -2200,8 +2314,10 @@
     <mergeCell ref="BI5:BJ5"/>
     <mergeCell ref="BU5:BV5"/>
     <mergeCell ref="G4:H4"/>
+    <mergeCell ref="CA3:CB3"/>
     <mergeCell ref="BI4:BJ4"/>
     <mergeCell ref="AZ2:BA2"/>
+    <mergeCell ref="CA5:CB5"/>
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="AE4:AF4"/>
   </mergeCells>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-09 22:34 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -1058,6 +1058,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -1077,6 +1080,59 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>84</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="29" name="Image 29" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>87</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="30" name="Image 30" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId30"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1506,7 +1562,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CE5"/>
+  <dimension ref="A1:CK5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1598,6 +1654,12 @@
     <col width="25" customWidth="1" min="82" max="82"/>
     <col width="25" customWidth="1" min="83" max="83"/>
     <col width="3" customWidth="1" min="84" max="84"/>
+    <col width="25" customWidth="1" min="85" max="85"/>
+    <col width="25" customWidth="1" min="86" max="86"/>
+    <col width="3" customWidth="1" min="87" max="87"/>
+    <col width="25" customWidth="1" min="88" max="88"/>
+    <col width="25" customWidth="1" min="89" max="89"/>
+    <col width="3" customWidth="1" min="90" max="90"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1769,6 +1831,18 @@
         </is>
       </c>
       <c r="CE1" s="2" t="n"/>
+      <c r="CG1" s="1" t="inlineStr">
+        <is>
+          <t>MIA @ ORL</t>
+        </is>
+      </c>
+      <c r="CH1" s="2" t="n"/>
+      <c r="CJ1" s="1" t="inlineStr">
+        <is>
+          <t>NYK @ TOR</t>
+        </is>
+      </c>
+      <c r="CK1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -1939,6 +2013,18 @@
         </is>
       </c>
       <c r="CE2" s="2" t="n"/>
+      <c r="CG2" s="3" t="inlineStr">
+        <is>
+          <t>11:00 PM / 2025-12-09</t>
+        </is>
+      </c>
+      <c r="CH2" s="2" t="n"/>
+      <c r="CJ2" s="3" t="inlineStr">
+        <is>
+          <t>1:30 AM / 2025-12-09</t>
+        </is>
+      </c>
+      <c r="CK2" s="2" t="n"/>
     </row>
     <row r="3" ht="112.5" customHeight="1">
       <c r="Y3" s="5" t="inlineStr">
@@ -2041,6 +2127,16 @@
           <t>https://polymarket.com/event/nba-nyk-tor-2025-12-09</t>
         </is>
       </c>
+      <c r="CG3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-mia-orl-2025-12-09</t>
+        </is>
+      </c>
+      <c r="CJ3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-nyk-tor-2025-12-09</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="112.5" customHeight="1">
       <c r="A4" s="4" t="inlineStr">
@@ -2185,11 +2281,22 @@
           <t>Captured: 03:25 PM</t>
         </is>
       </c>
+      <c r="CG5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 05:34 PM</t>
+        </is>
+      </c>
+      <c r="CJ5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 05:34 PM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="132">
+  <mergeCells count="142">
     <mergeCell ref="BO4:BP4"/>
     <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="CG4:CH4"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="AN3:AO3"/>
     <mergeCell ref="CA4:CB4"/>
@@ -2230,6 +2337,8 @@
     <mergeCell ref="BX2:BY2"/>
     <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="AW1:AX1"/>
+    <mergeCell ref="CG1:CH1"/>
+    <mergeCell ref="CJ2:CK2"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="BL3:BM3"/>
     <mergeCell ref="S1:T1"/>
@@ -2254,6 +2363,8 @@
     <mergeCell ref="AH4:AI4"/>
     <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="AW3:AX3"/>
+    <mergeCell ref="CG3:CH3"/>
+    <mergeCell ref="CJ4:CK4"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="AQ3:AR3"/>
@@ -2262,6 +2373,8 @@
     <mergeCell ref="CA2:CB2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="AW5:AX5"/>
+    <mergeCell ref="CJ1:CK1"/>
+    <mergeCell ref="CG5:CH5"/>
     <mergeCell ref="BO3:BP3"/>
     <mergeCell ref="AB2:AC2"/>
     <mergeCell ref="CD2:CE2"/>
@@ -2287,11 +2400,13 @@
     <mergeCell ref="V3:W3"/>
     <mergeCell ref="BR5:BS5"/>
     <mergeCell ref="AH3:AI3"/>
+    <mergeCell ref="CJ3:CK3"/>
     <mergeCell ref="AW2:AX2"/>
     <mergeCell ref="CA1:CB1"/>
     <mergeCell ref="BX5:BY5"/>
     <mergeCell ref="AH5:AI5"/>
     <mergeCell ref="AB4:AC4"/>
+    <mergeCell ref="CJ5:CK5"/>
     <mergeCell ref="V4:W4"/>
     <mergeCell ref="BF3:BG3"/>
     <mergeCell ref="S2:T2"/>
@@ -2302,6 +2417,7 @@
     <mergeCell ref="AE2:AF2"/>
     <mergeCell ref="Y5:Z5"/>
     <mergeCell ref="BO2:BP2"/>
+    <mergeCell ref="CG2:CH2"/>
     <mergeCell ref="AK5:AL5"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="AT4:AU4"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-09 23:11 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -1114,6 +1114,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -1133,6 +1136,59 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId30"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>90</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="31" name="Image 31" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId31"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>93</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="32" name="Image 32" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId32"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1562,7 +1618,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CK5"/>
+  <dimension ref="A1:CQ5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1660,6 +1716,12 @@
     <col width="25" customWidth="1" min="88" max="88"/>
     <col width="25" customWidth="1" min="89" max="89"/>
     <col width="3" customWidth="1" min="90" max="90"/>
+    <col width="25" customWidth="1" min="91" max="91"/>
+    <col width="25" customWidth="1" min="92" max="92"/>
+    <col width="3" customWidth="1" min="93" max="93"/>
+    <col width="25" customWidth="1" min="94" max="94"/>
+    <col width="25" customWidth="1" min="95" max="95"/>
+    <col width="3" customWidth="1" min="96" max="96"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1843,6 +1905,18 @@
         </is>
       </c>
       <c r="CK1" s="2" t="n"/>
+      <c r="CM1" s="1" t="inlineStr">
+        <is>
+          <t>MIA @ ORL</t>
+        </is>
+      </c>
+      <c r="CN1" s="2" t="n"/>
+      <c r="CP1" s="1" t="inlineStr">
+        <is>
+          <t>NYK @ TOR</t>
+        </is>
+      </c>
+      <c r="CQ1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -2025,6 +2099,18 @@
         </is>
       </c>
       <c r="CK2" s="2" t="n"/>
+      <c r="CM2" s="3" t="inlineStr">
+        <is>
+          <t>11:00 PM / 2025-12-09</t>
+        </is>
+      </c>
+      <c r="CN2" s="2" t="n"/>
+      <c r="CP2" s="3" t="inlineStr">
+        <is>
+          <t>1:30 AM / 2025-12-09</t>
+        </is>
+      </c>
+      <c r="CQ2" s="2" t="n"/>
     </row>
     <row r="3" ht="112.5" customHeight="1">
       <c r="Y3" s="5" t="inlineStr">
@@ -2137,6 +2223,16 @@
           <t>https://polymarket.com/event/nba-nyk-tor-2025-12-09</t>
         </is>
       </c>
+      <c r="CM3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-mia-orl-2025-12-09</t>
+        </is>
+      </c>
+      <c r="CP3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-nyk-tor-2025-12-09</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="112.5" customHeight="1">
       <c r="A4" s="4" t="inlineStr">
@@ -2291,10 +2387,21 @@
           <t>Captured: 05:34 PM</t>
         </is>
       </c>
+      <c r="CM5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 06:11 PM</t>
+        </is>
+      </c>
+      <c r="CP5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 06:11 PM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="142">
+  <mergeCells count="152">
     <mergeCell ref="BO4:BP4"/>
+    <mergeCell ref="CM5:CN5"/>
     <mergeCell ref="Y4:Z4"/>
     <mergeCell ref="CG4:CH4"/>
     <mergeCell ref="V2:W2"/>
@@ -2306,6 +2413,7 @@
     <mergeCell ref="AN5:AO5"/>
     <mergeCell ref="AT3:AU3"/>
     <mergeCell ref="AW4:AX4"/>
+    <mergeCell ref="CP5:CQ5"/>
     <mergeCell ref="AZ5:BA5"/>
     <mergeCell ref="Y1:Z1"/>
     <mergeCell ref="AT5:AU5"/>
@@ -2335,7 +2443,9 @@
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="AK1:AL1"/>
     <mergeCell ref="BX2:BY2"/>
+    <mergeCell ref="CP3:CQ3"/>
     <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="CM1:CN1"/>
     <mergeCell ref="AW1:AX1"/>
     <mergeCell ref="CG1:CH1"/>
     <mergeCell ref="CJ2:CK2"/>
@@ -2348,6 +2458,7 @@
     <mergeCell ref="BO1:BP1"/>
     <mergeCell ref="BL5:BM5"/>
     <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="CP4:CQ4"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="Y3:Z3"/>
@@ -2371,16 +2482,19 @@
     <mergeCell ref="AN1:AO1"/>
     <mergeCell ref="BX1:BY1"/>
     <mergeCell ref="CA2:CB2"/>
+    <mergeCell ref="CP1:CQ1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="AW5:AX5"/>
     <mergeCell ref="CJ1:CK1"/>
     <mergeCell ref="CG5:CH5"/>
+    <mergeCell ref="CM2:CN2"/>
     <mergeCell ref="BO3:BP3"/>
     <mergeCell ref="AB2:AC2"/>
     <mergeCell ref="CD2:CE2"/>
     <mergeCell ref="AN2:AO2"/>
     <mergeCell ref="BC5:BD5"/>
     <mergeCell ref="D3:E3"/>
+    <mergeCell ref="CP2:CQ2"/>
     <mergeCell ref="AQ4:AR4"/>
     <mergeCell ref="BO5:BP5"/>
     <mergeCell ref="A4:B4"/>
@@ -2402,6 +2516,7 @@
     <mergeCell ref="AH3:AI3"/>
     <mergeCell ref="CJ3:CK3"/>
     <mergeCell ref="AW2:AX2"/>
+    <mergeCell ref="CM4:CN4"/>
     <mergeCell ref="CA1:CB1"/>
     <mergeCell ref="BX5:BY5"/>
     <mergeCell ref="AH5:AI5"/>
@@ -2432,6 +2547,7 @@
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="CA3:CB3"/>
     <mergeCell ref="BI4:BJ4"/>
+    <mergeCell ref="CM3:CN3"/>
     <mergeCell ref="AZ2:BA2"/>
     <mergeCell ref="CA5:CB5"/>
     <mergeCell ref="M4:N4"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-10 02:47 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -1170,6 +1170,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -1189,6 +1192,34 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId32"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>96</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="33" name="Image 33" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId33"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1618,7 +1649,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CQ5"/>
+  <dimension ref="A1:CT5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1722,6 +1753,9 @@
     <col width="25" customWidth="1" min="94" max="94"/>
     <col width="25" customWidth="1" min="95" max="95"/>
     <col width="3" customWidth="1" min="96" max="96"/>
+    <col width="25" customWidth="1" min="97" max="97"/>
+    <col width="25" customWidth="1" min="98" max="98"/>
+    <col width="3" customWidth="1" min="99" max="99"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1917,6 +1951,12 @@
         </is>
       </c>
       <c r="CQ1" s="2" t="n"/>
+      <c r="CS1" s="1" t="inlineStr">
+        <is>
+          <t>NYK @ TOR</t>
+        </is>
+      </c>
+      <c r="CT1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -2111,6 +2151,12 @@
         </is>
       </c>
       <c r="CQ2" s="2" t="n"/>
+      <c r="CS2" s="3" t="inlineStr">
+        <is>
+          <t>LIVE / 2025-12-09</t>
+        </is>
+      </c>
+      <c r="CT2" s="2" t="n"/>
     </row>
     <row r="3" ht="112.5" customHeight="1">
       <c r="Y3" s="5" t="inlineStr">
@@ -2233,6 +2279,11 @@
           <t>https://polymarket.com/event/nba-nyk-tor-2025-12-09</t>
         </is>
       </c>
+      <c r="CS3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-nyk-tor-2025-12-09</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="112.5" customHeight="1">
       <c r="A4" s="4" t="inlineStr">
@@ -2397,9 +2448,14 @@
           <t>Captured: 06:11 PM</t>
         </is>
       </c>
+      <c r="CS5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 09:47 PM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="152">
+  <mergeCells count="157">
     <mergeCell ref="BO4:BP4"/>
     <mergeCell ref="CM5:CN5"/>
     <mergeCell ref="Y4:Z4"/>
@@ -2424,6 +2480,7 @@
     <mergeCell ref="BL4:BM4"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="AQ1:AR1"/>
+    <mergeCell ref="CS1:CT1"/>
     <mergeCell ref="BR4:BS4"/>
     <mergeCell ref="CD4:CE4"/>
     <mergeCell ref="AE5:AF5"/>
@@ -2444,6 +2501,7 @@
     <mergeCell ref="AK1:AL1"/>
     <mergeCell ref="BX2:BY2"/>
     <mergeCell ref="CP3:CQ3"/>
+    <mergeCell ref="CS4:CT4"/>
     <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="CM1:CN1"/>
     <mergeCell ref="AW1:AX1"/>
@@ -2482,12 +2540,14 @@
     <mergeCell ref="AN1:AO1"/>
     <mergeCell ref="BX1:BY1"/>
     <mergeCell ref="CA2:CB2"/>
+    <mergeCell ref="CS3:CT3"/>
     <mergeCell ref="CP1:CQ1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="AW5:AX5"/>
     <mergeCell ref="CJ1:CK1"/>
     <mergeCell ref="CG5:CH5"/>
     <mergeCell ref="CM2:CN2"/>
+    <mergeCell ref="CS5:CT5"/>
     <mergeCell ref="BO3:BP3"/>
     <mergeCell ref="AB2:AC2"/>
     <mergeCell ref="CD2:CE2"/>
@@ -2535,6 +2595,7 @@
     <mergeCell ref="CG2:CH2"/>
     <mergeCell ref="AK5:AL5"/>
     <mergeCell ref="G3:H3"/>
+    <mergeCell ref="CS2:CT2"/>
     <mergeCell ref="AT4:AU4"/>
     <mergeCell ref="BI3:BJ3"/>
     <mergeCell ref="A2:B2"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-10 03:51 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -1226,6 +1226,34 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>99</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="34" name="Image 34" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId34"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1649,7 +1677,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CT5"/>
+  <dimension ref="A1:CW5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1756,6 +1784,9 @@
     <col width="25" customWidth="1" min="97" max="97"/>
     <col width="25" customWidth="1" min="98" max="98"/>
     <col width="3" customWidth="1" min="99" max="99"/>
+    <col width="25" customWidth="1" min="100" max="100"/>
+    <col width="25" customWidth="1" min="101" max="101"/>
+    <col width="3" customWidth="1" min="102" max="102"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1957,6 +1988,12 @@
         </is>
       </c>
       <c r="CT1" s="2" t="n"/>
+      <c r="CV1" s="1" t="inlineStr">
+        <is>
+          <t>NYK @ TOR</t>
+        </is>
+      </c>
+      <c r="CW1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -2157,6 +2194,12 @@
         </is>
       </c>
       <c r="CT2" s="2" t="n"/>
+      <c r="CV2" s="3" t="inlineStr">
+        <is>
+          <t>LIVE / 2025-12-09</t>
+        </is>
+      </c>
+      <c r="CW2" s="2" t="n"/>
     </row>
     <row r="3" ht="112.5" customHeight="1">
       <c r="Y3" s="5" t="inlineStr">
@@ -2284,6 +2327,11 @@
           <t>https://polymarket.com/event/nba-nyk-tor-2025-12-09</t>
         </is>
       </c>
+      <c r="CV3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-nyk-tor-2025-12-09</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="112.5" customHeight="1">
       <c r="A4" s="4" t="inlineStr">
@@ -2453,9 +2501,14 @@
           <t>Captured: 09:47 PM</t>
         </is>
       </c>
+      <c r="CV5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 10:51 PM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="157">
+  <mergeCells count="162">
     <mergeCell ref="BO4:BP4"/>
     <mergeCell ref="CM5:CN5"/>
     <mergeCell ref="Y4:Z4"/>
@@ -2473,6 +2526,7 @@
     <mergeCell ref="AZ5:BA5"/>
     <mergeCell ref="Y1:Z1"/>
     <mergeCell ref="AT5:AU5"/>
+    <mergeCell ref="CV5:CW5"/>
     <mergeCell ref="BU1:BV1"/>
     <mergeCell ref="AZ4:BA4"/>
     <mergeCell ref="J4:K4"/>
@@ -2498,6 +2552,7 @@
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="AH1:AI1"/>
     <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="CV1:CW1"/>
     <mergeCell ref="AK1:AL1"/>
     <mergeCell ref="BX2:BY2"/>
     <mergeCell ref="CP3:CQ3"/>
@@ -2570,6 +2625,7 @@
     <mergeCell ref="BL2:BM2"/>
     <mergeCell ref="CD3:CE3"/>
     <mergeCell ref="BF5:BG5"/>
+    <mergeCell ref="CV2:CW2"/>
     <mergeCell ref="BF2:BG2"/>
     <mergeCell ref="V3:W3"/>
     <mergeCell ref="BR5:BS5"/>
@@ -2578,6 +2634,7 @@
     <mergeCell ref="AW2:AX2"/>
     <mergeCell ref="CM4:CN4"/>
     <mergeCell ref="CA1:CB1"/>
+    <mergeCell ref="CV3:CW3"/>
     <mergeCell ref="BX5:BY5"/>
     <mergeCell ref="AH5:AI5"/>
     <mergeCell ref="AB4:AC4"/>
@@ -2599,6 +2656,7 @@
     <mergeCell ref="AT4:AU4"/>
     <mergeCell ref="BI3:BJ3"/>
     <mergeCell ref="A2:B2"/>
+    <mergeCell ref="CV4:CW4"/>
     <mergeCell ref="BC3:BD3"/>
     <mergeCell ref="BF4:BG4"/>
     <mergeCell ref="AQ5:AR5"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-10 07:14 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="2025-12-08" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="2025-12-09" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="2025-12-10" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1254,6 +1255,64 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -2675,4 +2734,97 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="25" customWidth="1" min="1" max="1"/>
+    <col width="25" customWidth="1" min="2" max="2"/>
+    <col width="3" customWidth="1" min="3" max="3"/>
+    <col width="25" customWidth="1" min="4" max="4"/>
+    <col width="25" customWidth="1" min="5" max="5"/>
+    <col width="3" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>PHX @ OKC</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="n"/>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>SAS @ LAL</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>12:30 AM / 2025-12-10</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n"/>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>3:00 AM / 2025-12-10</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-phx-okc-2025-12-10</t>
+        </is>
+      </c>
+      <c r="D3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-sas-lal-2025-12-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="112.5" customHeight="1"/>
+    <row r="5">
+      <c r="A5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 02:14 AM</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 02:14 AM</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A3:B3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update NBA prices - 2025-12-10 08:17 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -1288,6 +1288,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -1307,6 +1310,34 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2742,7 +2773,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2756,6 +2787,9 @@
     <col width="25" customWidth="1" min="4" max="4"/>
     <col width="25" customWidth="1" min="5" max="5"/>
     <col width="3" customWidth="1" min="6" max="6"/>
+    <col width="25" customWidth="1" min="7" max="7"/>
+    <col width="25" customWidth="1" min="8" max="8"/>
+    <col width="3" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2771,6 +2805,12 @@
         </is>
       </c>
       <c r="E1" s="2" t="n"/>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>PHX @ OKC</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -2785,6 +2825,12 @@
         </is>
       </c>
       <c r="E2" s="2" t="n"/>
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>TBD / 2025-12-10</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="5" t="inlineStr">
@@ -2795,6 +2841,11 @@
       <c r="D3" s="5" t="inlineStr">
         <is>
           <t>https://polymarket.com/event/nba-sas-lal-2025-12-10</t>
+        </is>
+      </c>
+      <c r="G3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-phx-okc-2025-12-10</t>
         </is>
       </c>
     </row>
@@ -2810,19 +2861,29 @@
           <t>Captured: 02:14 AM</t>
         </is>
       </c>
+      <c r="G5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 03:17 AM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="15">
     <mergeCell ref="A4:B4"/>
+    <mergeCell ref="G4:H4"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G1:H1"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="A5:B5"/>
+    <mergeCell ref="G5:H5"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="A3:B3"/>
+    <mergeCell ref="G3:H3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-10 09:18 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -1344,6 +1344,59 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="4" name="Image 4" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>12</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="5" name="Image 5" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -2773,7 +2826,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2790,6 +2843,12 @@
     <col width="25" customWidth="1" min="7" max="7"/>
     <col width="25" customWidth="1" min="8" max="8"/>
     <col width="3" customWidth="1" min="9" max="9"/>
+    <col width="25" customWidth="1" min="10" max="10"/>
+    <col width="25" customWidth="1" min="11" max="11"/>
+    <col width="3" customWidth="1" min="12" max="12"/>
+    <col width="25" customWidth="1" min="13" max="13"/>
+    <col width="25" customWidth="1" min="14" max="14"/>
+    <col width="3" customWidth="1" min="15" max="15"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2811,6 +2870,18 @@
         </is>
       </c>
       <c r="H1" s="2" t="n"/>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>PHX @ OKC</t>
+        </is>
+      </c>
+      <c r="K1" s="2" t="n"/>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>SAS @ LAL</t>
+        </is>
+      </c>
+      <c r="N1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -2831,6 +2902,18 @@
         </is>
       </c>
       <c r="H2" s="2" t="n"/>
+      <c r="J2" s="3" t="inlineStr">
+        <is>
+          <t>12:30 AM / 2025-12-10</t>
+        </is>
+      </c>
+      <c r="K2" s="2" t="n"/>
+      <c r="M2" s="3" t="inlineStr">
+        <is>
+          <t>3:00 AM / 2025-12-10</t>
+        </is>
+      </c>
+      <c r="N2" s="2" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="5" t="inlineStr">
@@ -2846,6 +2929,16 @@
       <c r="G3" s="5" t="inlineStr">
         <is>
           <t>https://polymarket.com/event/nba-phx-okc-2025-12-10</t>
+        </is>
+      </c>
+      <c r="J3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-phx-okc-2025-12-10</t>
+        </is>
+      </c>
+      <c r="M3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-sas-lal-2025-12-10</t>
         </is>
       </c>
     </row>
@@ -2866,24 +2959,44 @@
           <t>Captured: 03:17 AM</t>
         </is>
       </c>
+      <c r="J5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 04:18 AM</t>
+        </is>
+      </c>
+      <c r="M5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 04:18 AM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:E2"/>
+  <mergeCells count="25">
+    <mergeCell ref="J5:K5"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="A2:B2"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="D4:E4"/>
-    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="M3:N3"/>
     <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="M4:N4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-10 10:13 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -1372,6 +1372,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -1391,6 +1394,59 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>15</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="6" name="Image 6" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>18</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="7" name="Image 7" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2826,7 +2882,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2849,6 +2905,12 @@
     <col width="25" customWidth="1" min="13" max="13"/>
     <col width="25" customWidth="1" min="14" max="14"/>
     <col width="3" customWidth="1" min="15" max="15"/>
+    <col width="25" customWidth="1" min="16" max="16"/>
+    <col width="25" customWidth="1" min="17" max="17"/>
+    <col width="3" customWidth="1" min="18" max="18"/>
+    <col width="25" customWidth="1" min="19" max="19"/>
+    <col width="25" customWidth="1" min="20" max="20"/>
+    <col width="3" customWidth="1" min="21" max="21"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2882,6 +2944,18 @@
         </is>
       </c>
       <c r="N1" s="2" t="n"/>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>PHX @ OKC</t>
+        </is>
+      </c>
+      <c r="Q1" s="2" t="n"/>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>SAS @ LAL</t>
+        </is>
+      </c>
+      <c r="T1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -2914,6 +2988,18 @@
         </is>
       </c>
       <c r="N2" s="2" t="n"/>
+      <c r="P2" s="3" t="inlineStr">
+        <is>
+          <t>12:30 AM / 2025-12-10</t>
+        </is>
+      </c>
+      <c r="Q2" s="2" t="n"/>
+      <c r="S2" s="3" t="inlineStr">
+        <is>
+          <t>3:00 AM / 2025-12-10</t>
+        </is>
+      </c>
+      <c r="T2" s="2" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="5" t="inlineStr">
@@ -2937,6 +3023,16 @@
         </is>
       </c>
       <c r="M3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-sas-lal-2025-12-10</t>
+        </is>
+      </c>
+      <c r="P3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-phx-okc-2025-12-10</t>
+        </is>
+      </c>
+      <c r="S3" s="5" t="inlineStr">
         <is>
           <t>https://polymarket.com/event/nba-sas-lal-2025-12-10</t>
         </is>
@@ -2969,18 +3065,33 @@
           <t>Captured: 04:18 AM</t>
         </is>
       </c>
+      <c r="P5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 05:13 AM</t>
+        </is>
+      </c>
+      <c r="S5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 05:13 AM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="35">
+    <mergeCell ref="P4:Q4"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="J1:K1"/>
+    <mergeCell ref="P1:Q1"/>
     <mergeCell ref="M5:N5"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="M1:N1"/>
+    <mergeCell ref="S3:T3"/>
     <mergeCell ref="M2:N2"/>
+    <mergeCell ref="S2:T2"/>
     <mergeCell ref="D2:E2"/>
+    <mergeCell ref="P2:Q2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="J4:K4"/>
@@ -2993,10 +3104,15 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="J3:K3"/>
+    <mergeCell ref="P3:Q3"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J2:K2"/>
+    <mergeCell ref="S1:T1"/>
     <mergeCell ref="D5:E5"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="P5:Q5"/>
     <mergeCell ref="M4:N4"/>
+    <mergeCell ref="S4:T4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-10 11:13 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -1428,6 +1428,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -1447,6 +1450,34 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>21</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="8" name="Image 8" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId8"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2882,7 +2913,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T5"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2911,6 +2942,9 @@
     <col width="25" customWidth="1" min="19" max="19"/>
     <col width="25" customWidth="1" min="20" max="20"/>
     <col width="3" customWidth="1" min="21" max="21"/>
+    <col width="25" customWidth="1" min="22" max="22"/>
+    <col width="25" customWidth="1" min="23" max="23"/>
+    <col width="3" customWidth="1" min="24" max="24"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2956,6 +2990,12 @@
         </is>
       </c>
       <c r="T1" s="2" t="n"/>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>SAS @ LAL</t>
+        </is>
+      </c>
+      <c r="W1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -3000,6 +3040,12 @@
         </is>
       </c>
       <c r="T2" s="2" t="n"/>
+      <c r="V2" s="3" t="inlineStr">
+        <is>
+          <t>TBD / 2025-12-10</t>
+        </is>
+      </c>
+      <c r="W2" s="2" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="5" t="inlineStr">
@@ -3033,6 +3079,11 @@
         </is>
       </c>
       <c r="S3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-sas-lal-2025-12-10</t>
+        </is>
+      </c>
+      <c r="V3" s="5" t="inlineStr">
         <is>
           <t>https://polymarket.com/event/nba-sas-lal-2025-12-10</t>
         </is>
@@ -3075,22 +3126,31 @@
           <t>Captured: 05:13 AM</t>
         </is>
       </c>
+      <c r="V5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 06:13 AM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="35">
+  <mergeCells count="40">
     <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="V2:W2"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="V5:W5"/>
     <mergeCell ref="M5:N5"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="S3:T3"/>
+    <mergeCell ref="V4:W4"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="D2:E2"/>
+    <mergeCell ref="V1:W1"/>
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="G3:H3"/>
@@ -3113,6 +3173,7 @@
     <mergeCell ref="P5:Q5"/>
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="S4:T4"/>
+    <mergeCell ref="V3:W3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-10 12:19 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -1484,6 +1484,59 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>24</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="9" name="Image 9" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>27</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="10" name="Image 10" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -2913,7 +2966,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:AC5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2945,6 +2998,12 @@
     <col width="25" customWidth="1" min="22" max="22"/>
     <col width="25" customWidth="1" min="23" max="23"/>
     <col width="3" customWidth="1" min="24" max="24"/>
+    <col width="25" customWidth="1" min="25" max="25"/>
+    <col width="25" customWidth="1" min="26" max="26"/>
+    <col width="3" customWidth="1" min="27" max="27"/>
+    <col width="25" customWidth="1" min="28" max="28"/>
+    <col width="25" customWidth="1" min="29" max="29"/>
+    <col width="3" customWidth="1" min="30" max="30"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2996,6 +3055,18 @@
         </is>
       </c>
       <c r="W1" s="2" t="n"/>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>PHX @ OKC</t>
+        </is>
+      </c>
+      <c r="Z1" s="2" t="n"/>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>SAS @ LAL</t>
+        </is>
+      </c>
+      <c r="AC1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -3046,6 +3117,18 @@
         </is>
       </c>
       <c r="W2" s="2" t="n"/>
+      <c r="Y2" s="3" t="inlineStr">
+        <is>
+          <t>12:30 AM / 2025-12-10</t>
+        </is>
+      </c>
+      <c r="Z2" s="2" t="n"/>
+      <c r="AB2" s="3" t="inlineStr">
+        <is>
+          <t>3:00 AM / 2025-12-10</t>
+        </is>
+      </c>
+      <c r="AC2" s="2" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="5" t="inlineStr">
@@ -3084,6 +3167,16 @@
         </is>
       </c>
       <c r="V3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-sas-lal-2025-12-10</t>
+        </is>
+      </c>
+      <c r="Y3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-phx-okc-2025-12-10</t>
+        </is>
+      </c>
+      <c r="AB3" s="5" t="inlineStr">
         <is>
           <t>https://polymarket.com/event/nba-sas-lal-2025-12-10</t>
         </is>
@@ -3131,31 +3224,50 @@
           <t>Captured: 06:13 AM</t>
         </is>
       </c>
+      <c r="Y5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 07:19 AM</t>
+        </is>
+      </c>
+      <c r="AB5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 07:19 AM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="40">
+  <mergeCells count="50">
     <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="Y4:Z4"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G2:H2"/>
+    <mergeCell ref="Y3:Z3"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="V5:W5"/>
+    <mergeCell ref="AB5:AC5"/>
     <mergeCell ref="M5:N5"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="S3:T3"/>
+    <mergeCell ref="AB4:AC4"/>
     <mergeCell ref="V4:W4"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="S2:T2"/>
+    <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="V1:W1"/>
+    <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="Y1:Z1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="A2:B2"/>
+    <mergeCell ref="AB2:AC2"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="D4:E4"/>
@@ -3174,6 +3286,7 @@
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="S4:T4"/>
     <mergeCell ref="V3:W3"/>
+    <mergeCell ref="AB3:AC3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-10 14:13 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -1512,6 +1512,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -1531,6 +1534,59 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>30</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="11" name="Image 11" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>33</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="12" name="Image 12" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId12"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2966,7 +3022,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC5"/>
+  <dimension ref="A1:AI5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3004,6 +3060,12 @@
     <col width="25" customWidth="1" min="28" max="28"/>
     <col width="25" customWidth="1" min="29" max="29"/>
     <col width="3" customWidth="1" min="30" max="30"/>
+    <col width="25" customWidth="1" min="31" max="31"/>
+    <col width="25" customWidth="1" min="32" max="32"/>
+    <col width="3" customWidth="1" min="33" max="33"/>
+    <col width="25" customWidth="1" min="34" max="34"/>
+    <col width="25" customWidth="1" min="35" max="35"/>
+    <col width="3" customWidth="1" min="36" max="36"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3067,6 +3129,18 @@
         </is>
       </c>
       <c r="AC1" s="2" t="n"/>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>PHX @ OKC</t>
+        </is>
+      </c>
+      <c r="AF1" s="2" t="n"/>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>SAS @ LAL</t>
+        </is>
+      </c>
+      <c r="AI1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -3129,6 +3203,18 @@
         </is>
       </c>
       <c r="AC2" s="2" t="n"/>
+      <c r="AE2" s="3" t="inlineStr">
+        <is>
+          <t>12:30 AM / 2025-12-10</t>
+        </is>
+      </c>
+      <c r="AF2" s="2" t="n"/>
+      <c r="AH2" s="3" t="inlineStr">
+        <is>
+          <t>3:00 AM / 2025-12-10</t>
+        </is>
+      </c>
+      <c r="AI2" s="2" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="5" t="inlineStr">
@@ -3177,6 +3263,16 @@
         </is>
       </c>
       <c r="AB3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-sas-lal-2025-12-10</t>
+        </is>
+      </c>
+      <c r="AE3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-phx-okc-2025-12-10</t>
+        </is>
+      </c>
+      <c r="AH3" s="5" t="inlineStr">
         <is>
           <t>https://polymarket.com/event/nba-sas-lal-2025-12-10</t>
         </is>
@@ -3234,12 +3330,23 @@
           <t>Captured: 07:19 AM</t>
         </is>
       </c>
+      <c r="AE5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 09:13 AM</t>
+        </is>
+      </c>
+      <c r="AH5" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 09:13 AM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="50">
+  <mergeCells count="60">
     <mergeCell ref="P4:Q4"/>
     <mergeCell ref="Y4:Z4"/>
     <mergeCell ref="V2:W2"/>
+    <mergeCell ref="AH3:AI3"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G2:H2"/>
@@ -3251,15 +3358,21 @@
     <mergeCell ref="M5:N5"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="M1:N1"/>
+    <mergeCell ref="AH5:AI5"/>
     <mergeCell ref="S3:T3"/>
     <mergeCell ref="AB4:AC4"/>
     <mergeCell ref="V4:W4"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="S2:T2"/>
+    <mergeCell ref="AE3:AF3"/>
     <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="D2:E2"/>
+    <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="AH4:AI4"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="AE2:AF2"/>
+    <mergeCell ref="AH1:AI1"/>
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="Y5:Z5"/>
     <mergeCell ref="Y1:Z1"/>
@@ -3270,6 +3383,7 @@
     <mergeCell ref="AB2:AC2"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="G5:H5"/>
+    <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="D3:E3"/>
@@ -3277,11 +3391,13 @@
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="AH2:AI2"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="S1:T1"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="S5:T5"/>
+    <mergeCell ref="AE5:AF5"/>
     <mergeCell ref="P5:Q5"/>
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="S4:T4"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-11 03:40 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -19,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -45,6 +45,10 @@
       <color rgb="000066CC"/>
       <sz val="8"/>
       <u val="single"/>
+    </font>
+    <font>
+      <color rgb="00CC6600"/>
+      <sz val="9"/>
     </font>
   </fonts>
   <fills count="3">
@@ -100,7 +104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -113,6 +117,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1568,6 +1575,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -1587,6 +1597,34 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="13" name="Image 13" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId13"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3022,7 +3060,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AI5"/>
+  <dimension ref="A1:AI6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3285,9 +3323,9 @@
           <t>Captured: 02:14 AM</t>
         </is>
       </c>
-      <c r="D5" s="4" t="inlineStr">
-        <is>
-          <t>Captured: 02:14 AM</t>
+      <c r="D5" s="6" t="inlineStr">
+        <is>
+          <t>SAS Low: 0.195</t>
         </is>
       </c>
       <c r="G5" s="4" t="inlineStr">
@@ -3341,12 +3379,13 @@
         </is>
       </c>
     </row>
+    <row r="6"/>
   </sheetData>
   <mergeCells count="60">
     <mergeCell ref="P4:Q4"/>
     <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="AH3:AI3"/>
     <mergeCell ref="V2:W2"/>
-    <mergeCell ref="AH3:AI3"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G2:H2"/>
@@ -3367,8 +3406,8 @@
     <mergeCell ref="AE3:AF3"/>
     <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="D2:E2"/>
+    <mergeCell ref="AH4:AI4"/>
     <mergeCell ref="AE4:AF4"/>
-    <mergeCell ref="AH4:AI4"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="AE2:AF2"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-11 04:22 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -1625,6 +1625,59 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="14" name="Image 14" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="15" name="Image 15" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId15"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3318,14 +3371,14 @@
     </row>
     <row r="4" ht="112.5" customHeight="1"/>
     <row r="5">
-      <c r="A5" s="4" t="inlineStr">
-        <is>
-          <t>Captured: 02:14 AM</t>
+      <c r="A5" s="6" t="inlineStr">
+        <is>
+          <t>PHX Low: 0.001</t>
         </is>
       </c>
       <c r="D5" s="6" t="inlineStr">
         <is>
-          <t>SAS Low: 0.195</t>
+          <t>SAS Low: 0.305</t>
         </is>
       </c>
       <c r="G5" s="4" t="inlineStr">

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-11 05:16 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -10,6 +10,7 @@
     <sheet name="2025-12-08" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="2025-12-09" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="2025-12-10" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="2025-12-11" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1659,6 +1660,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -1678,6 +1682,114 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="4" name="Image 4" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3113,7 +3225,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AI6"/>
+  <dimension ref="A1:AI5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3432,7 +3544,6 @@
         </is>
       </c>
     </row>
-    <row r="6"/>
   </sheetData>
   <mergeCells count="60">
     <mergeCell ref="P4:Q4"/>
@@ -3499,4 +3610,199 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="25" customWidth="1" min="1" max="1"/>
+    <col width="25" customWidth="1" min="2" max="2"/>
+    <col width="3" customWidth="1" min="3" max="3"/>
+    <col width="25" customWidth="1" min="4" max="4"/>
+    <col width="25" customWidth="1" min="5" max="5"/>
+    <col width="3" customWidth="1" min="6" max="6"/>
+    <col width="25" customWidth="1" min="7" max="7"/>
+    <col width="25" customWidth="1" min="8" max="8"/>
+    <col width="3" customWidth="1" min="9" max="9"/>
+    <col width="25" customWidth="1" min="10" max="10"/>
+    <col width="25" customWidth="1" min="11" max="11"/>
+    <col width="3" customWidth="1" min="12" max="12"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>POR @ NOP</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="n"/>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>BOS @ MIL</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="n"/>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>LAC @ HOU</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="n"/>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>DEN @ SAC</t>
+        </is>
+      </c>
+      <c r="K1" s="2" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>1:00 AM / 2025-12-11</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n"/>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>1:00 AM / 2025-12-11</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="n"/>
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>1:00 AM / 2025-12-11</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="n"/>
+      <c r="J2" s="3" t="inlineStr">
+        <is>
+          <t>3:00 AM / 2025-12-11</t>
+        </is>
+      </c>
+      <c r="K2" s="2" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-por-nop-2025-12-11</t>
+        </is>
+      </c>
+      <c r="D3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-bos-mil-2025-12-11</t>
+        </is>
+      </c>
+      <c r="G3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-lac-hou-2025-12-11</t>
+        </is>
+      </c>
+      <c r="J3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-den-sac-2025-12-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="112.5" customHeight="1"/>
+    <row r="5">
+      <c r="A5" s="6" t="inlineStr">
+        <is>
+          <t>POR Low: 0.635</t>
+        </is>
+      </c>
+      <c r="B5" s="6" t="inlineStr">
+        <is>
+          <t>NOP Low: 0.355</t>
+        </is>
+      </c>
+      <c r="D5" s="6" t="inlineStr">
+        <is>
+          <t>BOS Low: 0.765</t>
+        </is>
+      </c>
+      <c r="E5" s="6" t="inlineStr">
+        <is>
+          <t>MIL Low: 0.230</t>
+        </is>
+      </c>
+      <c r="G5" s="6" t="inlineStr">
+        <is>
+          <t>LAC Low: 0.775</t>
+        </is>
+      </c>
+      <c r="H5" s="6" t="inlineStr">
+        <is>
+          <t>HOU Low: 0.215</t>
+        </is>
+      </c>
+      <c r="J5" s="6" t="inlineStr">
+        <is>
+          <t>DEN Low: 0.770</t>
+        </is>
+      </c>
+      <c r="K5" s="6" t="inlineStr">
+        <is>
+          <t>SAC Low: 0.195</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 12:16 AM</t>
+        </is>
+      </c>
+      <c r="D6" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 12:16 AM</t>
+        </is>
+      </c>
+      <c r="G6" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 12:16 AM</t>
+        </is>
+      </c>
+      <c r="J6" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 12:16 AM</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="J2:K2"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update NBA prices - 2025-12-11 07:21 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -1721,6 +1721,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -1746,6 +1749,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -1771,6 +1777,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -1790,6 +1799,34 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>7</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="5" name="Image 5" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3618,7 +3655,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3779,16 +3816,38 @@
         </is>
       </c>
     </row>
+    <row r="8" ht="112.5" customHeight="1"/>
+    <row r="9">
+      <c r="G9" s="6" t="inlineStr">
+        <is>
+          <t>LAC Low: 0.765</t>
+        </is>
+      </c>
+      <c r="H9" s="6" t="inlineStr">
+        <is>
+          <t>HOU Low: 0.215</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="G10" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 02:21 AM</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="22">
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="G8:H8"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="J6:K6"/>
+    <mergeCell ref="G10:H10"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="G3:H3"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-11 08:18 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -1827,6 +1827,109 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>7</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="6" name="Image 6" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>7</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="7" name="Image 7" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>11</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="8" name="Image 8" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>7</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="9" name="Image 9" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId9"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3655,7 +3758,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3818,6 +3921,26 @@
     </row>
     <row r="8" ht="112.5" customHeight="1"/>
     <row r="9">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>POR Low: 0.625</t>
+        </is>
+      </c>
+      <c r="B9" s="6" t="inlineStr">
+        <is>
+          <t>NOP Low: 0.355</t>
+        </is>
+      </c>
+      <c r="D9" s="6" t="inlineStr">
+        <is>
+          <t>BOS Low: 0.765</t>
+        </is>
+      </c>
+      <c r="E9" s="6" t="inlineStr">
+        <is>
+          <t>MIL Low: 0.230</t>
+        </is>
+      </c>
       <c r="G9" s="6" t="inlineStr">
         <is>
           <t>LAC Low: 0.765</t>
@@ -3826,20 +3949,68 @@
       <c r="H9" s="6" t="inlineStr">
         <is>
           <t>HOU Low: 0.215</t>
+        </is>
+      </c>
+      <c r="J9" s="6" t="inlineStr">
+        <is>
+          <t>DEN Low: 0.795</t>
+        </is>
+      </c>
+      <c r="K9" s="6" t="inlineStr">
+        <is>
+          <t>SAC Low: 0.195</t>
         </is>
       </c>
     </row>
     <row r="10">
+      <c r="A10" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 03:18 AM</t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 03:18 AM</t>
+        </is>
+      </c>
       <c r="G10" s="4" t="inlineStr">
         <is>
           <t>Captured: 02:21 AM</t>
+        </is>
+      </c>
+      <c r="J10" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 03:18 AM</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="112.5" customHeight="1"/>
+    <row r="13">
+      <c r="G13" s="6" t="inlineStr">
+        <is>
+          <t>LAC Low: 0.765</t>
+        </is>
+      </c>
+      <c r="H13" s="6" t="inlineStr">
+        <is>
+          <t>HOU Low: 0.215</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="G14" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 03:18 AM</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="30">
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="D10:E10"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J10:K10"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="G8:H8"/>
@@ -3854,12 +4025,17 @@
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D4:E4"/>
+    <mergeCell ref="G14:H14"/>
     <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="J3:K3"/>
+    <mergeCell ref="D8:E8"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J2:K2"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="J8:K8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-11 09:16 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -1861,6 +1861,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -1886,6 +1889,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -1911,6 +1917,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -1930,6 +1939,109 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>11</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="10" name="Image 10" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>11</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="11" name="Image 11" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>15</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="12" name="Image 12" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>11</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="13" name="Image 13" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId13"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3758,7 +3870,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3986,6 +4098,26 @@
     </row>
     <row r="12" ht="112.5" customHeight="1"/>
     <row r="13">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>POR Low: 0.615</t>
+        </is>
+      </c>
+      <c r="B13" s="6" t="inlineStr">
+        <is>
+          <t>NOP Low: 0.355</t>
+        </is>
+      </c>
+      <c r="D13" s="6" t="inlineStr">
+        <is>
+          <t>BOS Low: 0.765</t>
+        </is>
+      </c>
+      <c r="E13" s="6" t="inlineStr">
+        <is>
+          <t>MIL Low: 0.225</t>
+        </is>
+      </c>
       <c r="G13" s="6" t="inlineStr">
         <is>
           <t>LAC Low: 0.765</t>
@@ -3994,22 +4126,68 @@
       <c r="H13" s="6" t="inlineStr">
         <is>
           <t>HOU Low: 0.215</t>
+        </is>
+      </c>
+      <c r="J13" s="6" t="inlineStr">
+        <is>
+          <t>DEN Low: 0.795</t>
+        </is>
+      </c>
+      <c r="K13" s="6" t="inlineStr">
+        <is>
+          <t>SAC Low: 0.195</t>
         </is>
       </c>
     </row>
     <row r="14">
+      <c r="A14" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 04:16 AM</t>
+        </is>
+      </c>
+      <c r="D14" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 04:16 AM</t>
+        </is>
+      </c>
       <c r="G14" s="4" t="inlineStr">
         <is>
           <t>Captured: 03:18 AM</t>
+        </is>
+      </c>
+      <c r="J14" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 04:16 AM</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" ht="112.5" customHeight="1"/>
+    <row r="17">
+      <c r="G17" s="6" t="inlineStr">
+        <is>
+          <t>LAC Low: 0.215</t>
+        </is>
+      </c>
+      <c r="H17" s="6" t="inlineStr">
+        <is>
+          <t>HOU Low: 0.765</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="G18" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 04:16 AM</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="38">
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J14:K14"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="A1:B1"/>
@@ -4020,21 +4198,28 @@
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G18:H18"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="G3:H3"/>
+    <mergeCell ref="A12:B12"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A14:B14"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="A8:B8"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="D8:E8"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="G16:H16"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D14:E14"/>
     <mergeCell ref="J8:K8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-11 11:14 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -1973,6 +1973,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -1998,6 +2001,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -2023,6 +2029,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -2042,6 +2051,109 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>15</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="14" name="Image 14" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>15</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="15" name="Image 15" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>19</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="16" name="Image 16" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>15</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="17" name="Image 17" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId17"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3870,7 +3982,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4163,6 +4275,26 @@
     </row>
     <row r="16" ht="112.5" customHeight="1"/>
     <row r="17">
+      <c r="A17" s="6" t="inlineStr">
+        <is>
+          <t>POR Low: 0.365</t>
+        </is>
+      </c>
+      <c r="B17" s="6" t="inlineStr">
+        <is>
+          <t>NOP Low: 0.615</t>
+        </is>
+      </c>
+      <c r="D17" s="6" t="inlineStr">
+        <is>
+          <t>BOS Low: 0.225</t>
+        </is>
+      </c>
+      <c r="E17" s="6" t="inlineStr">
+        <is>
+          <t>MIL Low: 0.765</t>
+        </is>
+      </c>
       <c r="G17" s="6" t="inlineStr">
         <is>
           <t>LAC Low: 0.215</t>
@@ -4171,18 +4303,63 @@
       <c r="H17" s="6" t="inlineStr">
         <is>
           <t>HOU Low: 0.765</t>
+        </is>
+      </c>
+      <c r="J17" s="6" t="inlineStr">
+        <is>
+          <t>DEN Low: 0.795</t>
+        </is>
+      </c>
+      <c r="K17" s="6" t="inlineStr">
+        <is>
+          <t>SAC Low: 0.195</t>
         </is>
       </c>
     </row>
     <row r="18">
+      <c r="A18" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 06:14 AM</t>
+        </is>
+      </c>
+      <c r="D18" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 06:14 AM</t>
+        </is>
+      </c>
       <c r="G18" s="4" t="inlineStr">
         <is>
           <t>Captured: 04:16 AM</t>
+        </is>
+      </c>
+      <c r="J18" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 06:14 AM</t>
+        </is>
+      </c>
+    </row>
+    <row r="20" ht="112.5" customHeight="1"/>
+    <row r="21">
+      <c r="G21" s="6" t="inlineStr">
+        <is>
+          <t>LAC Low: 0.765</t>
+        </is>
+      </c>
+      <c r="H21" s="6" t="inlineStr">
+        <is>
+          <t>HOU Low: 0.225</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="G22" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 06:14 AM</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="38">
+  <mergeCells count="46">
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D1:E1"/>
@@ -4194,19 +4371,24 @@
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="D6:E6"/>
+    <mergeCell ref="A16:B16"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="G6:H6"/>
+    <mergeCell ref="A18:B18"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="J16:K16"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="G14:H14"/>
+    <mergeCell ref="D18:E18"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="D12:E12"/>
@@ -4214,12 +4396,15 @@
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="D8:E8"/>
+    <mergeCell ref="G20:H20"/>
     <mergeCell ref="J12:K12"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="A10:B10"/>
+    <mergeCell ref="J18:K18"/>
     <mergeCell ref="D14:E14"/>
+    <mergeCell ref="G22:H22"/>
     <mergeCell ref="J8:K8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-11 12:21 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -2085,6 +2085,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -2110,6 +2113,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -2135,6 +2141,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -2154,6 +2163,109 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>19</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="18" name="Image 18" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>19</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="19" name="Image 19" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>23</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="20" name="Image 20" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>19</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="21" name="Image 21" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId21"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3982,7 +4094,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4340,6 +4452,26 @@
     </row>
     <row r="20" ht="112.5" customHeight="1"/>
     <row r="21">
+      <c r="A21" s="6" t="inlineStr">
+        <is>
+          <t>POR Low: 0.615</t>
+        </is>
+      </c>
+      <c r="B21" s="6" t="inlineStr">
+        <is>
+          <t>NOP Low: 0.365</t>
+        </is>
+      </c>
+      <c r="D21" s="6" t="inlineStr">
+        <is>
+          <t>BOS Low: 0.765</t>
+        </is>
+      </c>
+      <c r="E21" s="6" t="inlineStr">
+        <is>
+          <t>MIL Low: 0.225</t>
+        </is>
+      </c>
       <c r="G21" s="6" t="inlineStr">
         <is>
           <t>LAC Low: 0.765</t>
@@ -4348,18 +4480,64 @@
       <c r="H21" s="6" t="inlineStr">
         <is>
           <t>HOU Low: 0.225</t>
+        </is>
+      </c>
+      <c r="J21" s="6" t="inlineStr">
+        <is>
+          <t>DEN Low: 0.795</t>
+        </is>
+      </c>
+      <c r="K21" s="6" t="inlineStr">
+        <is>
+          <t>SAC Low: 0.195</t>
         </is>
       </c>
     </row>
     <row r="22">
+      <c r="A22" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 07:21 AM</t>
+        </is>
+      </c>
+      <c r="D22" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 07:21 AM</t>
+        </is>
+      </c>
       <c r="G22" s="4" t="inlineStr">
         <is>
           <t>Captured: 06:14 AM</t>
+        </is>
+      </c>
+      <c r="J22" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 07:21 AM</t>
+        </is>
+      </c>
+    </row>
+    <row r="24" ht="112.5" customHeight="1"/>
+    <row r="25">
+      <c r="G25" s="6" t="inlineStr">
+        <is>
+          <t>LAC Low: 0.765</t>
+        </is>
+      </c>
+      <c r="H25" s="6" t="inlineStr">
+        <is>
+          <t>HOU Low: 0.225</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="G26" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 07:21 AM</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="46">
+  <mergeCells count="54">
+    <mergeCell ref="D20:E20"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D1:E1"/>
@@ -4367,6 +4545,7 @@
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="J1:K1"/>
+    <mergeCell ref="D22:E22"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="A6:B6"/>
@@ -4384,19 +4563,25 @@
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D16:E16"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="G24:H24"/>
     <mergeCell ref="J16:K16"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="D18:E18"/>
+    <mergeCell ref="J22:K22"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="A8:B8"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="A22:B22"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="G20:H20"/>
+    <mergeCell ref="A20:B20"/>
     <mergeCell ref="J12:K12"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G1:H1"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-11 13:25 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -2197,6 +2197,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -2222,6 +2225,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -2247,6 +2253,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -2266,6 +2275,109 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>23</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="22" name="Image 22" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>27</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="23" name="Image 23" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>23</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="24" name="Image 24" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>23</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="25" name="Image 25" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId25"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4094,7 +4206,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4517,6 +4629,26 @@
     </row>
     <row r="24" ht="112.5" customHeight="1"/>
     <row r="25">
+      <c r="A25" s="6" t="inlineStr">
+        <is>
+          <t>POR Low: 0.615</t>
+        </is>
+      </c>
+      <c r="B25" s="6" t="inlineStr">
+        <is>
+          <t>NOP Low: 0.375</t>
+        </is>
+      </c>
+      <c r="D25" s="6" t="inlineStr">
+        <is>
+          <t>BOS Low: 0.225</t>
+        </is>
+      </c>
+      <c r="E25" s="6" t="inlineStr">
+        <is>
+          <t>MIL Low: 0.765</t>
+        </is>
+      </c>
       <c r="G25" s="6" t="inlineStr">
         <is>
           <t>LAC Low: 0.765</t>
@@ -4525,19 +4657,65 @@
       <c r="H25" s="6" t="inlineStr">
         <is>
           <t>HOU Low: 0.225</t>
+        </is>
+      </c>
+      <c r="J25" s="6" t="inlineStr">
+        <is>
+          <t>DEN Low: 0.195</t>
+        </is>
+      </c>
+      <c r="K25" s="6" t="inlineStr">
+        <is>
+          <t>SAC Low: 0.795</t>
         </is>
       </c>
     </row>
     <row r="26">
+      <c r="A26" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 08:25 AM</t>
+        </is>
+      </c>
+      <c r="D26" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 08:25 AM</t>
+        </is>
+      </c>
       <c r="G26" s="4" t="inlineStr">
         <is>
           <t>Captured: 07:21 AM</t>
+        </is>
+      </c>
+      <c r="J26" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 08:25 AM</t>
+        </is>
+      </c>
+    </row>
+    <row r="28" ht="112.5" customHeight="1"/>
+    <row r="29">
+      <c r="G29" s="6" t="inlineStr">
+        <is>
+          <t>LAC Low: 0.765</t>
+        </is>
+      </c>
+      <c r="H29" s="6" t="inlineStr">
+        <is>
+          <t>HOU Low: 0.225</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="G30" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 08:25 AM</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="54">
+  <mergeCells count="62">
     <mergeCell ref="D20:E20"/>
+    <mergeCell ref="A24:B24"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D1:E1"/>
@@ -4553,18 +4731,24 @@
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J24:K24"/>
     <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G28:H28"/>
     <mergeCell ref="G6:H6"/>
+    <mergeCell ref="D26:E26"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="G3:H3"/>
+    <mergeCell ref="J26:K26"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A26:B26"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="J20:K20"/>
     <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G30:H30"/>
     <mergeCell ref="J16:K16"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="D4:E4"/>
@@ -4583,6 +4767,7 @@
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="J12:K12"/>
+    <mergeCell ref="D24:E24"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J2:K2"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-11 14:16 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -2309,6 +2309,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -2334,6 +2337,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -2359,6 +2365,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -2378,6 +2387,109 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>27</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="26" name="Image 26" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>31</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="27" name="Image 27" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>27</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="28" name="Image 28" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>27</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="29" name="Image 29" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId29"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4206,7 +4318,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4694,6 +4806,26 @@
     </row>
     <row r="28" ht="112.5" customHeight="1"/>
     <row r="29">
+      <c r="A29" s="6" t="inlineStr">
+        <is>
+          <t>POR Low: 0.615</t>
+        </is>
+      </c>
+      <c r="B29" s="6" t="inlineStr">
+        <is>
+          <t>NOP Low: 0.375</t>
+        </is>
+      </c>
+      <c r="D29" s="6" t="inlineStr">
+        <is>
+          <t>BOS Low: 0.225</t>
+        </is>
+      </c>
+      <c r="E29" s="6" t="inlineStr">
+        <is>
+          <t>MIL Low: 0.765</t>
+        </is>
+      </c>
       <c r="G29" s="6" t="inlineStr">
         <is>
           <t>LAC Low: 0.765</t>
@@ -4702,21 +4834,67 @@
       <c r="H29" s="6" t="inlineStr">
         <is>
           <t>HOU Low: 0.225</t>
+        </is>
+      </c>
+      <c r="J29" s="6" t="inlineStr">
+        <is>
+          <t>DEN Low: 0.795</t>
+        </is>
+      </c>
+      <c r="K29" s="6" t="inlineStr">
+        <is>
+          <t>SAC Low: 0.195</t>
         </is>
       </c>
     </row>
     <row r="30">
+      <c r="A30" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 09:16 AM</t>
+        </is>
+      </c>
+      <c r="D30" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 09:16 AM</t>
+        </is>
+      </c>
       <c r="G30" s="4" t="inlineStr">
         <is>
           <t>Captured: 08:25 AM</t>
+        </is>
+      </c>
+      <c r="J30" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 09:16 AM</t>
+        </is>
+      </c>
+    </row>
+    <row r="32" ht="112.5" customHeight="1"/>
+    <row r="33">
+      <c r="G33" s="6" t="inlineStr">
+        <is>
+          <t>LAC Low: 0.765</t>
+        </is>
+      </c>
+      <c r="H33" s="6" t="inlineStr">
+        <is>
+          <t>HOU Low: 0.225</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="G34" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 09:16 AM</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="62">
+  <mergeCells count="70">
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="G12:H12"/>
+    <mergeCell ref="A30:B30"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G2:H2"/>
@@ -4725,9 +4903,11 @@
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="J28:K28"/>
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="D6:E6"/>
+    <mergeCell ref="J30:K30"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="J6:K6"/>
@@ -4747,9 +4927,11 @@
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="J20:K20"/>
+    <mergeCell ref="G34:H34"/>
     <mergeCell ref="G24:H24"/>
     <mergeCell ref="G30:H30"/>
     <mergeCell ref="J16:K16"/>
+    <mergeCell ref="D28:E28"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="G14:H14"/>
@@ -4768,10 +4950,13 @@
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="J12:K12"/>
     <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D30:E30"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J2:K2"/>
+    <mergeCell ref="G32:H32"/>
     <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A28:B28"/>
     <mergeCell ref="J18:K18"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="G22:H22"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-11 15:15 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -2421,6 +2421,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -2446,6 +2449,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -2471,6 +2477,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -2490,6 +2499,109 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>31</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="30" name="Image 30" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId30"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>31</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="31" name="Image 31" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId31"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>35</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="32" name="Image 32" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId32"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>31</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="33" name="Image 33" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId33"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4318,7 +4430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4871,6 +4983,26 @@
     </row>
     <row r="32" ht="112.5" customHeight="1"/>
     <row r="33">
+      <c r="A33" s="6" t="inlineStr">
+        <is>
+          <t>POR Low: 0.615</t>
+        </is>
+      </c>
+      <c r="B33" s="6" t="inlineStr">
+        <is>
+          <t>NOP Low: 0.375</t>
+        </is>
+      </c>
+      <c r="D33" s="6" t="inlineStr">
+        <is>
+          <t>BOS Low: 0.225</t>
+        </is>
+      </c>
+      <c r="E33" s="6" t="inlineStr">
+        <is>
+          <t>MIL Low: 0.770</t>
+        </is>
+      </c>
       <c r="G33" s="6" t="inlineStr">
         <is>
           <t>LAC Low: 0.765</t>
@@ -4879,87 +5011,140 @@
       <c r="H33" s="6" t="inlineStr">
         <is>
           <t>HOU Low: 0.225</t>
+        </is>
+      </c>
+      <c r="J33" s="6" t="inlineStr">
+        <is>
+          <t>DEN Low: 0.195</t>
+        </is>
+      </c>
+      <c r="K33" s="6" t="inlineStr">
+        <is>
+          <t>SAC Low: 0.805</t>
         </is>
       </c>
     </row>
     <row r="34">
+      <c r="A34" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 10:15 AM</t>
+        </is>
+      </c>
+      <c r="D34" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 10:15 AM</t>
+        </is>
+      </c>
       <c r="G34" s="4" t="inlineStr">
         <is>
           <t>Captured: 09:16 AM</t>
+        </is>
+      </c>
+      <c r="J34" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 10:15 AM</t>
+        </is>
+      </c>
+    </row>
+    <row r="36" ht="112.5" customHeight="1"/>
+    <row r="37">
+      <c r="G37" s="6" t="inlineStr">
+        <is>
+          <t>LAC Low: 0.225</t>
+        </is>
+      </c>
+      <c r="H37" s="6" t="inlineStr">
+        <is>
+          <t>HOU Low: 0.765</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="G38" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 10:15 AM</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="70">
+  <mergeCells count="78">
     <mergeCell ref="D20:E20"/>
-    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="A30:B30"/>
     <mergeCell ref="G12:H12"/>
-    <mergeCell ref="A30:B30"/>
     <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A34:B34"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G2:H2"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="D22:E22"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="J6:K6"/>
     <mergeCell ref="J24:K24"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="G18:H18"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="G3:H3"/>
     <mergeCell ref="J26:K26"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G30:H30"/>
     <mergeCell ref="J16:K16"/>
+    <mergeCell ref="A32:B32"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="J22:K22"/>
     <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="A22:B22"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="D24:E24"/>
     <mergeCell ref="D30:E30"/>
-    <mergeCell ref="G16:H16"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="G32:H32"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="A20:B20"/>
     <mergeCell ref="J18:K18"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="G22:H22"/>
     <mergeCell ref="J8:K8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-11 16:17 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -2533,6 +2533,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -2558,6 +2561,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -2583,6 +2589,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -2602,6 +2611,109 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId33"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>35</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="34" name="Image 34" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId34"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>35</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="35" name="Image 35" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId35"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>39</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="36" name="Image 36" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId36"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>35</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="37" name="Image 37" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId37"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4430,7 +4542,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5048,6 +5160,26 @@
     </row>
     <row r="36" ht="112.5" customHeight="1"/>
     <row r="37">
+      <c r="A37" s="6" t="inlineStr">
+        <is>
+          <t>POR Low: 0.375</t>
+        </is>
+      </c>
+      <c r="B37" s="6" t="inlineStr">
+        <is>
+          <t>NOP Low: 0.615</t>
+        </is>
+      </c>
+      <c r="D37" s="6" t="inlineStr">
+        <is>
+          <t>BOS Low: 0.215</t>
+        </is>
+      </c>
+      <c r="E37" s="6" t="inlineStr">
+        <is>
+          <t>MIL Low: 0.770</t>
+        </is>
+      </c>
       <c r="G37" s="6" t="inlineStr">
         <is>
           <t>LAC Low: 0.225</t>
@@ -5056,22 +5188,68 @@
       <c r="H37" s="6" t="inlineStr">
         <is>
           <t>HOU Low: 0.765</t>
+        </is>
+      </c>
+      <c r="J37" s="6" t="inlineStr">
+        <is>
+          <t>DEN Low: 0.195</t>
+        </is>
+      </c>
+      <c r="K37" s="6" t="inlineStr">
+        <is>
+          <t>SAC Low: 0.805</t>
         </is>
       </c>
     </row>
     <row r="38">
+      <c r="A38" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 11:17 AM</t>
+        </is>
+      </c>
+      <c r="D38" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 11:17 AM</t>
+        </is>
+      </c>
       <c r="G38" s="4" t="inlineStr">
         <is>
           <t>Captured: 10:15 AM</t>
+        </is>
+      </c>
+      <c r="J38" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 11:17 AM</t>
+        </is>
+      </c>
+    </row>
+    <row r="40" ht="112.5" customHeight="1"/>
+    <row r="41">
+      <c r="G41" s="6" t="inlineStr">
+        <is>
+          <t>LAC Low: 0.225</t>
+        </is>
+      </c>
+      <c r="H41" s="6" t="inlineStr">
+        <is>
+          <t>HOU Low: 0.765</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="G42" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 11:17 AM</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="78">
+  <mergeCells count="86">
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="J28:K28"/>
+    <mergeCell ref="D36:E36"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="J4:K4"/>
@@ -5091,6 +5269,7 @@
     <mergeCell ref="J34:K34"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="G38:H38"/>
+    <mergeCell ref="J36:K36"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="J20:K20"/>
     <mergeCell ref="G24:H24"/>
@@ -5101,9 +5280,13 @@
     <mergeCell ref="J12:K12"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D38:E38"/>
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="A36:B36"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="J24:K24"/>
     <mergeCell ref="A3:B3"/>
@@ -5116,6 +5299,7 @@
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A38:B38"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J2:K2"/>
@@ -5145,6 +5329,7 @@
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="J18:K18"/>
+    <mergeCell ref="G40:H40"/>
     <mergeCell ref="J8:K8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-11 18:20 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -2645,6 +2645,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -2670,6 +2673,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -2695,6 +2701,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -2714,6 +2723,109 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId37"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>39</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="38" name="Image 38" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId38"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>39</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="39" name="Image 39" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId39"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>43</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="40" name="Image 40" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId40"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>39</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="41" name="Image 41" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId41"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4542,7 +4654,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5225,6 +5337,26 @@
     </row>
     <row r="40" ht="112.5" customHeight="1"/>
     <row r="41">
+      <c r="A41" s="6" t="inlineStr">
+        <is>
+          <t>POR Low: 0.375</t>
+        </is>
+      </c>
+      <c r="B41" s="6" t="inlineStr">
+        <is>
+          <t>NOP Low: 0.605</t>
+        </is>
+      </c>
+      <c r="D41" s="6" t="inlineStr">
+        <is>
+          <t>BOS Low: 0.215</t>
+        </is>
+      </c>
+      <c r="E41" s="6" t="inlineStr">
+        <is>
+          <t>MIL Low: 0.770</t>
+        </is>
+      </c>
       <c r="G41" s="6" t="inlineStr">
         <is>
           <t>LAC Low: 0.225</t>
@@ -5233,18 +5365,63 @@
       <c r="H41" s="6" t="inlineStr">
         <is>
           <t>HOU Low: 0.765</t>
+        </is>
+      </c>
+      <c r="J41" s="6" t="inlineStr">
+        <is>
+          <t>DEN Low: 0.805</t>
+        </is>
+      </c>
+      <c r="K41" s="6" t="inlineStr">
+        <is>
+          <t>SAC Low: 0.195</t>
         </is>
       </c>
     </row>
     <row r="42">
+      <c r="A42" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 01:20 PM</t>
+        </is>
+      </c>
+      <c r="D42" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 01:20 PM</t>
+        </is>
+      </c>
       <c r="G42" s="4" t="inlineStr">
         <is>
           <t>Captured: 11:17 AM</t>
+        </is>
+      </c>
+      <c r="J42" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 01:20 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="44" ht="112.5" customHeight="1"/>
+    <row r="45">
+      <c r="G45" s="6" t="inlineStr">
+        <is>
+          <t>LAC Low: 0.765</t>
+        </is>
+      </c>
+      <c r="H45" s="6" t="inlineStr">
+        <is>
+          <t>HOU Low: 0.225</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="G46" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 01:20 PM</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="86">
+  <mergeCells count="94">
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D22:E22"/>
@@ -5254,11 +5431,13 @@
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="G34:H34"/>
+    <mergeCell ref="A42:B42"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="A28:B28"/>
+    <mergeCell ref="G44:H44"/>
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="A30:B30"/>
@@ -5288,6 +5467,7 @@
     <mergeCell ref="G42:H42"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="J40:K40"/>
     <mergeCell ref="J24:K24"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="J26:K26"/>
@@ -5304,10 +5484,13 @@
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="G32:H32"/>
+    <mergeCell ref="J42:K42"/>
     <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A40:B40"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="G36:H36"/>
+    <mergeCell ref="D40:E40"/>
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="J30:K30"/>
@@ -5328,7 +5511,9 @@
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D42:E42"/>
     <mergeCell ref="J18:K18"/>
+    <mergeCell ref="G46:H46"/>
     <mergeCell ref="G40:H40"/>
     <mergeCell ref="J8:K8"/>
   </mergeCells>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-11 19:15 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -2757,6 +2757,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -2782,6 +2785,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -2807,6 +2813,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -2826,6 +2835,109 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId41"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>43</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="42" name="Image 42" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId42"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>43</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="43" name="Image 43" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId43"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>47</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="44" name="Image 44" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId44"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>43</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="45" name="Image 45" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId45"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4654,7 +4766,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K46"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5402,6 +5514,26 @@
     </row>
     <row r="44" ht="112.5" customHeight="1"/>
     <row r="45">
+      <c r="A45" s="6" t="inlineStr">
+        <is>
+          <t>POR Low: 0.605</t>
+        </is>
+      </c>
+      <c r="B45" s="6" t="inlineStr">
+        <is>
+          <t>NOP Low: 0.375</t>
+        </is>
+      </c>
+      <c r="D45" s="6" t="inlineStr">
+        <is>
+          <t>BOS Low: 0.215</t>
+        </is>
+      </c>
+      <c r="E45" s="6" t="inlineStr">
+        <is>
+          <t>MIL Low: 0.770</t>
+        </is>
+      </c>
       <c r="G45" s="6" t="inlineStr">
         <is>
           <t>LAC Low: 0.765</t>
@@ -5410,18 +5542,63 @@
       <c r="H45" s="6" t="inlineStr">
         <is>
           <t>HOU Low: 0.225</t>
+        </is>
+      </c>
+      <c r="J45" s="6" t="inlineStr">
+        <is>
+          <t>DEN Low: 0.195</t>
+        </is>
+      </c>
+      <c r="K45" s="6" t="inlineStr">
+        <is>
+          <t>SAC Low: 0.795</t>
         </is>
       </c>
     </row>
     <row r="46">
+      <c r="A46" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 02:15 PM</t>
+        </is>
+      </c>
+      <c r="D46" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 02:15 PM</t>
+        </is>
+      </c>
       <c r="G46" s="4" t="inlineStr">
         <is>
           <t>Captured: 01:20 PM</t>
+        </is>
+      </c>
+      <c r="J46" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 02:15 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="48" ht="112.5" customHeight="1"/>
+    <row r="49">
+      <c r="G49" s="6" t="inlineStr">
+        <is>
+          <t>LAC Low: 0.775</t>
+        </is>
+      </c>
+      <c r="H49" s="6" t="inlineStr">
+        <is>
+          <t>HOU Low: 0.215</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="G50" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 02:15 PM</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="94">
+  <mergeCells count="102">
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D22:E22"/>
@@ -5445,9 +5622,11 @@
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="J1:K1"/>
+    <mergeCell ref="G48:H48"/>
     <mergeCell ref="J34:K34"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="G38:H38"/>
+    <mergeCell ref="A46:B46"/>
     <mergeCell ref="J36:K36"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="J20:K20"/>
@@ -5458,6 +5637,7 @@
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="J12:K12"/>
     <mergeCell ref="G16:H16"/>
+    <mergeCell ref="J46:K46"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="D38:E38"/>
     <mergeCell ref="A34:B34"/>
@@ -5486,10 +5666,13 @@
     <mergeCell ref="G32:H32"/>
     <mergeCell ref="J42:K42"/>
     <mergeCell ref="D14:E14"/>
+    <mergeCell ref="G50:H50"/>
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="A24:B24"/>
+    <mergeCell ref="J44:K44"/>
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="G36:H36"/>
+    <mergeCell ref="D46:E46"/>
     <mergeCell ref="D40:E40"/>
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="A6:B6"/>
@@ -5513,9 +5696,11 @@
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="J18:K18"/>
+    <mergeCell ref="A44:B44"/>
     <mergeCell ref="G46:H46"/>
     <mergeCell ref="G40:H40"/>
     <mergeCell ref="J8:K8"/>
+    <mergeCell ref="D44:E44"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-11 20:15 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -2869,6 +2869,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -2894,6 +2897,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -2919,6 +2925,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -2938,6 +2947,109 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId45"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>47</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="46" name="Image 46" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId46"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>47</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="47" name="Image 47" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId47"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>51</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="48" name="Image 48" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId48"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>47</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="49" name="Image 49" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId49"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4766,7 +4878,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5579,6 +5691,26 @@
     </row>
     <row r="48" ht="112.5" customHeight="1"/>
     <row r="49">
+      <c r="A49" s="6" t="inlineStr">
+        <is>
+          <t>POR Low: 0.375</t>
+        </is>
+      </c>
+      <c r="B49" s="6" t="inlineStr">
+        <is>
+          <t>NOP Low: 0.605</t>
+        </is>
+      </c>
+      <c r="D49" s="6" t="inlineStr">
+        <is>
+          <t>BOS Low: 0.215</t>
+        </is>
+      </c>
+      <c r="E49" s="6" t="inlineStr">
+        <is>
+          <t>MIL Low: 0.770</t>
+        </is>
+      </c>
       <c r="G49" s="6" t="inlineStr">
         <is>
           <t>LAC Low: 0.775</t>
@@ -5587,25 +5719,72 @@
       <c r="H49" s="6" t="inlineStr">
         <is>
           <t>HOU Low: 0.215</t>
+        </is>
+      </c>
+      <c r="J49" s="6" t="inlineStr">
+        <is>
+          <t>DEN Low: 0.195</t>
+        </is>
+      </c>
+      <c r="K49" s="6" t="inlineStr">
+        <is>
+          <t>SAC Low: 0.795</t>
         </is>
       </c>
     </row>
     <row r="50">
+      <c r="A50" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 03:15 PM</t>
+        </is>
+      </c>
+      <c r="D50" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 03:15 PM</t>
+        </is>
+      </c>
       <c r="G50" s="4" t="inlineStr">
         <is>
           <t>Captured: 02:15 PM</t>
+        </is>
+      </c>
+      <c r="J50" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 03:15 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="52" ht="112.5" customHeight="1"/>
+    <row r="53">
+      <c r="G53" s="6" t="inlineStr">
+        <is>
+          <t>LAC Low: 0.775</t>
+        </is>
+      </c>
+      <c r="H53" s="6" t="inlineStr">
+        <is>
+          <t>HOU Low: 0.215</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="G54" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 03:15 PM</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="102">
+  <mergeCells count="110">
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="J28:K28"/>
     <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D50:E50"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="G18:H18"/>
+    <mergeCell ref="D48:E48"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="G34:H34"/>
     <mergeCell ref="A42:B42"/>
@@ -5617,6 +5796,7 @@
     <mergeCell ref="G44:H44"/>
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="D26:E26"/>
+    <mergeCell ref="A48:B48"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="D10:E10"/>
@@ -5640,6 +5820,7 @@
     <mergeCell ref="J46:K46"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="D38:E38"/>
+    <mergeCell ref="J48:K48"/>
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G2:H2"/>
@@ -5661,6 +5842,8 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="D30:E30"/>
+    <mergeCell ref="J50:K50"/>
+    <mergeCell ref="G54:H54"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="G32:H32"/>
@@ -5670,6 +5853,7 @@
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="J44:K44"/>
+    <mergeCell ref="G52:H52"/>
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="G36:H36"/>
     <mergeCell ref="D46:E46"/>
@@ -5685,6 +5869,7 @@
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="G3:H3"/>
+    <mergeCell ref="A50:B50"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="G30:H30"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-11 21:14 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -2981,6 +2981,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -3006,6 +3009,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -3031,6 +3037,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -3050,6 +3059,109 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId49"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>51</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="50" name="Image 50" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId50"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>55</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="51" name="Image 51" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId51"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>51</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="52" name="Image 52" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId52"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>51</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="53" name="Image 53" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId53"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4878,7 +4990,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K54"/>
+  <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5756,6 +5868,26 @@
     </row>
     <row r="52" ht="112.5" customHeight="1"/>
     <row r="53">
+      <c r="A53" s="6" t="inlineStr">
+        <is>
+          <t>POR Low: 0.605</t>
+        </is>
+      </c>
+      <c r="B53" s="6" t="inlineStr">
+        <is>
+          <t>NOP Low: 0.375</t>
+        </is>
+      </c>
+      <c r="D53" s="6" t="inlineStr">
+        <is>
+          <t>BOS Low: 0.215</t>
+        </is>
+      </c>
+      <c r="E53" s="6" t="inlineStr">
+        <is>
+          <t>MIL Low: 0.775</t>
+        </is>
+      </c>
       <c r="G53" s="6" t="inlineStr">
         <is>
           <t>LAC Low: 0.775</t>
@@ -5764,18 +5896,63 @@
       <c r="H53" s="6" t="inlineStr">
         <is>
           <t>HOU Low: 0.215</t>
+        </is>
+      </c>
+      <c r="J53" s="6" t="inlineStr">
+        <is>
+          <t>DEN Low: 0.795</t>
+        </is>
+      </c>
+      <c r="K53" s="6" t="inlineStr">
+        <is>
+          <t>SAC Low: 0.195</t>
         </is>
       </c>
     </row>
     <row r="54">
+      <c r="A54" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 04:14 PM</t>
+        </is>
+      </c>
+      <c r="D54" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 04:14 PM</t>
+        </is>
+      </c>
       <c r="G54" s="4" t="inlineStr">
         <is>
           <t>Captured: 03:15 PM</t>
+        </is>
+      </c>
+      <c r="J54" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 04:14 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="56" ht="112.5" customHeight="1"/>
+    <row r="57">
+      <c r="G57" s="6" t="inlineStr">
+        <is>
+          <t>LAC Low: 0.775</t>
+        </is>
+      </c>
+      <c r="H57" s="6" t="inlineStr">
+        <is>
+          <t>HOU Low: 0.215</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="G58" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 04:14 PM</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="110">
+  <mergeCells count="118">
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D22:E22"/>
@@ -5783,11 +5960,13 @@
     <mergeCell ref="D36:E36"/>
     <mergeCell ref="D50:E50"/>
     <mergeCell ref="D6:E6"/>
+    <mergeCell ref="A54:B54"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="D48:E48"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="G34:H34"/>
     <mergeCell ref="A42:B42"/>
+    <mergeCell ref="G58:H58"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="G20:H20"/>
@@ -5816,6 +5995,7 @@
     <mergeCell ref="G26:H26"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="J12:K12"/>
+    <mergeCell ref="A52:B52"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="J46:K46"/>
     <mergeCell ref="A10:B10"/>
@@ -5829,6 +6009,7 @@
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="J40:K40"/>
+    <mergeCell ref="D52:E52"/>
     <mergeCell ref="J24:K24"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="J26:K26"/>
@@ -5850,7 +6031,10 @@
     <mergeCell ref="J42:K42"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="G50:H50"/>
+    <mergeCell ref="D54:E54"/>
     <mergeCell ref="A40:B40"/>
+    <mergeCell ref="J52:K52"/>
+    <mergeCell ref="G56:H56"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="J44:K44"/>
     <mergeCell ref="G52:H52"/>
@@ -5873,6 +6057,7 @@
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="G30:H30"/>
+    <mergeCell ref="J54:K54"/>
     <mergeCell ref="J32:K32"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="D18:E18"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-11 22:13 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -3093,6 +3093,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -3118,6 +3121,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -3143,6 +3149,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -3162,6 +3171,109 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId53"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>55</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="54" name="Image 54" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId54"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>55</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="55" name="Image 55" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId55"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>59</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="56" name="Image 56" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId56"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>55</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="57" name="Image 57" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId57"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4990,7 +5102,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K58"/>
+  <dimension ref="A1:K62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5933,6 +6045,26 @@
     </row>
     <row r="56" ht="112.5" customHeight="1"/>
     <row r="57">
+      <c r="A57" s="6" t="inlineStr">
+        <is>
+          <t>POR Low: 0.605</t>
+        </is>
+      </c>
+      <c r="B57" s="6" t="inlineStr">
+        <is>
+          <t>NOP Low: 0.380</t>
+        </is>
+      </c>
+      <c r="D57" s="6" t="inlineStr">
+        <is>
+          <t>BOS Low: 0.215</t>
+        </is>
+      </c>
+      <c r="E57" s="6" t="inlineStr">
+        <is>
+          <t>MIL Low: 0.775</t>
+        </is>
+      </c>
       <c r="G57" s="6" t="inlineStr">
         <is>
           <t>LAC Low: 0.775</t>
@@ -5941,18 +6073,63 @@
       <c r="H57" s="6" t="inlineStr">
         <is>
           <t>HOU Low: 0.215</t>
+        </is>
+      </c>
+      <c r="J57" s="6" t="inlineStr">
+        <is>
+          <t>DEN Low: 0.195</t>
+        </is>
+      </c>
+      <c r="K57" s="6" t="inlineStr">
+        <is>
+          <t>SAC Low: 0.795</t>
         </is>
       </c>
     </row>
     <row r="58">
+      <c r="A58" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 05:13 PM</t>
+        </is>
+      </c>
+      <c r="D58" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 05:13 PM</t>
+        </is>
+      </c>
       <c r="G58" s="4" t="inlineStr">
         <is>
           <t>Captured: 04:14 PM</t>
+        </is>
+      </c>
+      <c r="J58" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 05:13 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="60" ht="112.5" customHeight="1"/>
+    <row r="61">
+      <c r="G61" s="6" t="inlineStr">
+        <is>
+          <t>LAC Low: 0.775</t>
+        </is>
+      </c>
+      <c r="H61" s="6" t="inlineStr">
+        <is>
+          <t>HOU Low: 0.215</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="G62" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 05:13 PM</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="118">
+  <mergeCells count="126">
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D22:E22"/>
@@ -5961,6 +6138,7 @@
     <mergeCell ref="D50:E50"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A56:B56"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="D48:E48"/>
     <mergeCell ref="J4:K4"/>
@@ -5968,12 +6146,14 @@
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="G58:H58"/>
     <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D56:E56"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="G44:H44"/>
     <mergeCell ref="G22:H22"/>
+    <mergeCell ref="J58:K58"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="A48:B48"/>
     <mergeCell ref="A30:B30"/>
@@ -5986,6 +6166,7 @@
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="G38:H38"/>
     <mergeCell ref="A46:B46"/>
+    <mergeCell ref="G62:H62"/>
     <mergeCell ref="J36:K36"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="J20:K20"/>
@@ -6000,6 +6181,7 @@
     <mergeCell ref="J46:K46"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="D38:E38"/>
+    <mergeCell ref="G60:H60"/>
     <mergeCell ref="J48:K48"/>
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="D1:E1"/>
@@ -6061,6 +6243,8 @@
     <mergeCell ref="J32:K32"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="J56:K56"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="A20:B20"/>
@@ -6071,6 +6255,7 @@
     <mergeCell ref="G40:H40"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="D44:E44"/>
+    <mergeCell ref="A58:B58"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-11 23:14 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -3205,6 +3205,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -3230,6 +3233,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -3255,6 +3261,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -3274,6 +3283,109 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId57"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>59</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="58" name="Image 58" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId58"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>59</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="59" name="Image 59" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId59"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>63</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="60" name="Image 60" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId60"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>59</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="61" name="Image 61" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId61"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -5102,7 +5214,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K62"/>
+  <dimension ref="A1:K66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6110,6 +6222,26 @@
     </row>
     <row r="60" ht="112.5" customHeight="1"/>
     <row r="61">
+      <c r="A61" s="6" t="inlineStr">
+        <is>
+          <t>POR Low: 0.385</t>
+        </is>
+      </c>
+      <c r="B61" s="6" t="inlineStr">
+        <is>
+          <t>NOP Low: 0.605</t>
+        </is>
+      </c>
+      <c r="D61" s="6" t="inlineStr">
+        <is>
+          <t>BOS Low: 0.775</t>
+        </is>
+      </c>
+      <c r="E61" s="6" t="inlineStr">
+        <is>
+          <t>MIL Low: 0.215</t>
+        </is>
+      </c>
       <c r="G61" s="6" t="inlineStr">
         <is>
           <t>LAC Low: 0.775</t>
@@ -6118,26 +6250,74 @@
       <c r="H61" s="6" t="inlineStr">
         <is>
           <t>HOU Low: 0.215</t>
+        </is>
+      </c>
+      <c r="J61" s="6" t="inlineStr">
+        <is>
+          <t>DEN Low: 0.195</t>
+        </is>
+      </c>
+      <c r="K61" s="6" t="inlineStr">
+        <is>
+          <t>SAC Low: 0.795</t>
         </is>
       </c>
     </row>
     <row r="62">
+      <c r="A62" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 06:14 PM</t>
+        </is>
+      </c>
+      <c r="D62" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 06:14 PM</t>
+        </is>
+      </c>
       <c r="G62" s="4" t="inlineStr">
         <is>
           <t>Captured: 05:13 PM</t>
+        </is>
+      </c>
+      <c r="J62" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 06:14 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="64" ht="112.5" customHeight="1"/>
+    <row r="65">
+      <c r="G65" s="6" t="inlineStr">
+        <is>
+          <t>LAC Low: 0.775</t>
+        </is>
+      </c>
+      <c r="H65" s="6" t="inlineStr">
+        <is>
+          <t>HOU Low: 0.215</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="G66" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 06:14 PM</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="126">
+  <mergeCells count="134">
     <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D60:E60"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="J28:K28"/>
     <mergeCell ref="D36:E36"/>
     <mergeCell ref="D50:E50"/>
+    <mergeCell ref="J60:K60"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="A54:B54"/>
+    <mergeCell ref="G66:H66"/>
     <mergeCell ref="A56:B56"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="D48:E48"/>
@@ -6146,10 +6326,13 @@
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="G58:H58"/>
     <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D62:E62"/>
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A62:B62"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="D24:E24"/>
+    <mergeCell ref="J62:K62"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="G44:H44"/>
     <mergeCell ref="G22:H22"/>
@@ -6201,6 +6384,7 @@
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="D3:E3"/>
+    <mergeCell ref="G64:H64"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A38:B38"/>
@@ -6220,6 +6404,7 @@
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="J44:K44"/>
     <mergeCell ref="G52:H52"/>
+    <mergeCell ref="A60:B60"/>
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="G36:H36"/>
     <mergeCell ref="D46:E46"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-12 00:43 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -3317,6 +3317,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -3342,6 +3345,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -3367,6 +3373,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -3386,6 +3395,109 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId61"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>63</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="62" name="Image 62" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId62"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>67</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="63" name="Image 63" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId63"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>63</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="64" name="Image 64" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId64"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>63</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="65" name="Image 65" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId65"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -5214,7 +5326,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K66"/>
+  <dimension ref="A1:K70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6287,6 +6399,26 @@
     </row>
     <row r="64" ht="112.5" customHeight="1"/>
     <row r="65">
+      <c r="A65" s="6" t="inlineStr">
+        <is>
+          <t>POR Low: 0.605</t>
+        </is>
+      </c>
+      <c r="B65" s="6" t="inlineStr">
+        <is>
+          <t>NOP Low: 0.385</t>
+        </is>
+      </c>
+      <c r="D65" s="6" t="inlineStr">
+        <is>
+          <t>BOS Low: 0.775</t>
+        </is>
+      </c>
+      <c r="E65" s="6" t="inlineStr">
+        <is>
+          <t>MIL Low: 0.205</t>
+        </is>
+      </c>
       <c r="G65" s="6" t="inlineStr">
         <is>
           <t>LAC Low: 0.775</t>
@@ -6295,20 +6427,66 @@
       <c r="H65" s="6" t="inlineStr">
         <is>
           <t>HOU Low: 0.215</t>
+        </is>
+      </c>
+      <c r="J65" s="6" t="inlineStr">
+        <is>
+          <t>DEN Low: 0.195</t>
+        </is>
+      </c>
+      <c r="K65" s="6" t="inlineStr">
+        <is>
+          <t>SAC Low: 0.795</t>
         </is>
       </c>
     </row>
     <row r="66">
+      <c r="A66" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 07:43 PM</t>
+        </is>
+      </c>
+      <c r="D66" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 07:43 PM</t>
+        </is>
+      </c>
       <c r="G66" s="4" t="inlineStr">
         <is>
           <t>Captured: 06:14 PM</t>
+        </is>
+      </c>
+      <c r="J66" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 07:43 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="68" ht="112.5" customHeight="1"/>
+    <row r="69">
+      <c r="G69" s="6" t="inlineStr">
+        <is>
+          <t>LAC Low: 0.765</t>
+        </is>
+      </c>
+      <c r="H69" s="6" t="inlineStr">
+        <is>
+          <t>HOU Low: 0.215</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="G70" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 07:43 PM</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="134">
+  <mergeCells count="142">
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D60:E60"/>
+    <mergeCell ref="A64:B64"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="J28:K28"/>
@@ -6323,6 +6501,7 @@
     <mergeCell ref="D48:E48"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G68:H68"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="G58:H58"/>
     <mergeCell ref="D4:E4"/>
@@ -6332,6 +6511,7 @@
     <mergeCell ref="A62:B62"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D64:E64"/>
     <mergeCell ref="J62:K62"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="G44:H44"/>
@@ -6339,11 +6519,13 @@
     <mergeCell ref="J58:K58"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="A48:B48"/>
+    <mergeCell ref="J64:K64"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="J1:K1"/>
+    <mergeCell ref="G70:H70"/>
     <mergeCell ref="G48:H48"/>
     <mergeCell ref="J34:K34"/>
     <mergeCell ref="D2:E2"/>
@@ -6351,6 +6533,7 @@
     <mergeCell ref="A46:B46"/>
     <mergeCell ref="G62:H62"/>
     <mergeCell ref="J36:K36"/>
+    <mergeCell ref="D66:E66"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="J20:K20"/>
     <mergeCell ref="G24:H24"/>
@@ -6384,6 +6567,7 @@
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="D3:E3"/>
+    <mergeCell ref="J66:K66"/>
     <mergeCell ref="G64:H64"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A4:B4"/>
@@ -6417,6 +6601,7 @@
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="D32:E32"/>
     <mergeCell ref="G28:H28"/>
+    <mergeCell ref="A66:B66"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="G3:H3"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-12 01:41 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -3429,6 +3429,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -3454,6 +3457,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -3479,6 +3485,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -3498,6 +3507,109 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId65"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>67</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="66" name="Image 66" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId66"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>67</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="67" name="Image 67" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId67"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>71</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="68" name="Image 68" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId68"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>67</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="69" name="Image 69" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId69"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -5326,7 +5438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K70"/>
+  <dimension ref="A1:K74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6464,6 +6576,26 @@
     </row>
     <row r="68" ht="112.5" customHeight="1"/>
     <row r="69">
+      <c r="A69" s="6" t="inlineStr">
+        <is>
+          <t>POR Low: 0.435</t>
+        </is>
+      </c>
+      <c r="B69" s="6" t="inlineStr">
+        <is>
+          <t>NOP Low: 0.385</t>
+        </is>
+      </c>
+      <c r="D69" s="6" t="inlineStr">
+        <is>
+          <t>BOS Low: 0.775</t>
+        </is>
+      </c>
+      <c r="E69" s="6" t="inlineStr">
+        <is>
+          <t>MIL Low: 0.085</t>
+        </is>
+      </c>
       <c r="G69" s="6" t="inlineStr">
         <is>
           <t>LAC Low: 0.765</t>
@@ -6472,18 +6604,63 @@
       <c r="H69" s="6" t="inlineStr">
         <is>
           <t>HOU Low: 0.215</t>
+        </is>
+      </c>
+      <c r="J69" s="6" t="inlineStr">
+        <is>
+          <t>DEN Low: 0.795</t>
+        </is>
+      </c>
+      <c r="K69" s="6" t="inlineStr">
+        <is>
+          <t>SAC Low: 0.195</t>
         </is>
       </c>
     </row>
     <row r="70">
+      <c r="A70" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 08:41 PM</t>
+        </is>
+      </c>
+      <c r="D70" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 08:41 PM</t>
+        </is>
+      </c>
       <c r="G70" s="4" t="inlineStr">
         <is>
           <t>Captured: 07:43 PM</t>
+        </is>
+      </c>
+      <c r="J70" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 08:41 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="72" ht="112.5" customHeight="1"/>
+    <row r="73">
+      <c r="G73" s="6" t="inlineStr">
+        <is>
+          <t>LAC Low: 0.145</t>
+        </is>
+      </c>
+      <c r="H73" s="6" t="inlineStr">
+        <is>
+          <t>HOU Low: 0.745</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="G74" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 08:41 PM</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="142">
+  <mergeCells count="150">
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D60:E60"/>
     <mergeCell ref="A64:B64"/>
@@ -6492,10 +6669,13 @@
     <mergeCell ref="J28:K28"/>
     <mergeCell ref="D36:E36"/>
     <mergeCell ref="D50:E50"/>
+    <mergeCell ref="A70:B70"/>
     <mergeCell ref="J60:K60"/>
     <mergeCell ref="D6:E6"/>
+    <mergeCell ref="J68:K68"/>
     <mergeCell ref="A54:B54"/>
     <mergeCell ref="G66:H66"/>
+    <mergeCell ref="D70:E70"/>
     <mergeCell ref="A56:B56"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="D48:E48"/>
@@ -6512,6 +6692,7 @@
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="D64:E64"/>
+    <mergeCell ref="A68:B68"/>
     <mergeCell ref="J62:K62"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="G44:H44"/>
@@ -6605,7 +6786,9 @@
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G74:H74"/>
     <mergeCell ref="A50:B50"/>
+    <mergeCell ref="J70:K70"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="G30:H30"/>
@@ -6618,6 +6801,7 @@
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D68:E68"/>
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="J18:K18"/>
     <mergeCell ref="A44:B44"/>
@@ -6626,6 +6810,7 @@
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="D44:E44"/>
     <mergeCell ref="A58:B58"/>
+    <mergeCell ref="G72:H72"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-12 02:48 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -3541,6 +3541,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -3566,6 +3569,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -3591,6 +3597,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -3610,6 +3619,109 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId69"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>71</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="70" name="Image 70" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId70"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>71</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="71" name="Image 71" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId71"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>75</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="72" name="Image 72" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId72"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>71</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="73" name="Image 73" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId73"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -5438,7 +5550,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K74"/>
+  <dimension ref="A1:K78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6641,6 +6753,26 @@
     </row>
     <row r="72" ht="112.5" customHeight="1"/>
     <row r="73">
+      <c r="A73" s="6" t="inlineStr">
+        <is>
+          <t>POR Low: 0.435</t>
+        </is>
+      </c>
+      <c r="B73" s="6" t="inlineStr">
+        <is>
+          <t>NOP Low: 0.385</t>
+        </is>
+      </c>
+      <c r="D73" s="6" t="inlineStr">
+        <is>
+          <t>BOS Low: 0.685</t>
+        </is>
+      </c>
+      <c r="E73" s="6" t="inlineStr">
+        <is>
+          <t>MIL Low: 0.075</t>
+        </is>
+      </c>
       <c r="G73" s="6" t="inlineStr">
         <is>
           <t>LAC Low: 0.145</t>
@@ -6649,38 +6781,85 @@
       <c r="H73" s="6" t="inlineStr">
         <is>
           <t>HOU Low: 0.745</t>
+        </is>
+      </c>
+      <c r="J73" s="6" t="inlineStr">
+        <is>
+          <t>DEN Low: 0.795</t>
+        </is>
+      </c>
+      <c r="K73" s="6" t="inlineStr">
+        <is>
+          <t>SAC Low: 0.195</t>
         </is>
       </c>
     </row>
     <row r="74">
+      <c r="A74" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 09:48 PM</t>
+        </is>
+      </c>
+      <c r="D74" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 09:48 PM</t>
+        </is>
+      </c>
       <c r="G74" s="4" t="inlineStr">
         <is>
           <t>Captured: 08:41 PM</t>
+        </is>
+      </c>
+      <c r="J74" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 09:48 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="76" ht="112.5" customHeight="1"/>
+    <row r="77">
+      <c r="G77" s="6" t="inlineStr">
+        <is>
+          <t>LAC Low: 0.505</t>
+        </is>
+      </c>
+      <c r="H77" s="6" t="inlineStr">
+        <is>
+          <t>HOU Low: 0.145</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="G78" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 09:48 PM</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="150">
+  <mergeCells count="158">
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D60:E60"/>
     <mergeCell ref="A64:B64"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="J28:K28"/>
+    <mergeCell ref="A70:B70"/>
     <mergeCell ref="D36:E36"/>
     <mergeCell ref="D50:E50"/>
-    <mergeCell ref="A70:B70"/>
     <mergeCell ref="J60:K60"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="J68:K68"/>
     <mergeCell ref="A54:B54"/>
     <mergeCell ref="G66:H66"/>
+    <mergeCell ref="A74:B74"/>
     <mergeCell ref="D70:E70"/>
     <mergeCell ref="A56:B56"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="D48:E48"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="G34:H34"/>
+    <mergeCell ref="D72:E72"/>
     <mergeCell ref="G68:H68"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="G58:H58"/>
@@ -6726,6 +6905,7 @@
     <mergeCell ref="A52:B52"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="J46:K46"/>
+    <mergeCell ref="G76:H76"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="D38:E38"/>
     <mergeCell ref="G60:H60"/>
@@ -6740,7 +6920,9 @@
     <mergeCell ref="J40:K40"/>
     <mergeCell ref="D52:E52"/>
     <mergeCell ref="J24:K24"/>
+    <mergeCell ref="J74:K74"/>
     <mergeCell ref="A3:B3"/>
+    <mergeCell ref="G78:H78"/>
     <mergeCell ref="J26:K26"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="J16:K16"/>
@@ -6771,6 +6953,7 @@
     <mergeCell ref="G52:H52"/>
     <mergeCell ref="A60:B60"/>
     <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J72:K72"/>
     <mergeCell ref="G36:H36"/>
     <mergeCell ref="D46:E46"/>
     <mergeCell ref="D40:E40"/>
@@ -6801,6 +6984,8 @@
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="A72:B72"/>
     <mergeCell ref="D68:E68"/>
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="J18:K18"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-12 03:42 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -20,7 +20,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -49,6 +49,12 @@
     </font>
     <font>
       <color rgb="00CC6600"/>
+      <sz val="9"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="1"/>
+      <color rgb="00008000"/>
       <sz val="9"/>
     </font>
   </fonts>
@@ -105,7 +111,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -121,6 +127,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3653,6 +3662,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -3678,6 +3690,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -3703,6 +3718,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -3722,6 +3740,84 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId73"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>79</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="74" name="Image 74" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId74"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>75</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="75" name="Image 75" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId75"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>75</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="76" name="Image 76" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId76"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -5550,7 +5646,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K78"/>
+  <dimension ref="A1:K82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6818,6 +6914,16 @@
     </row>
     <row r="76" ht="112.5" customHeight="1"/>
     <row r="77">
+      <c r="D77" s="6" t="inlineStr">
+        <is>
+          <t>BOS Low: 0.075</t>
+        </is>
+      </c>
+      <c r="E77" s="6" t="inlineStr">
+        <is>
+          <t>MIL Low: 0.000</t>
+        </is>
+      </c>
       <c r="G77" s="6" t="inlineStr">
         <is>
           <t>LAC Low: 0.505</t>
@@ -6826,18 +6932,58 @@
       <c r="H77" s="6" t="inlineStr">
         <is>
           <t>HOU Low: 0.145</t>
+        </is>
+      </c>
+      <c r="J77" s="6" t="inlineStr">
+        <is>
+          <t>DEN Low: 0.060</t>
+        </is>
+      </c>
+      <c r="K77" s="6" t="inlineStr">
+        <is>
+          <t>SAC Low: 0.795</t>
         </is>
       </c>
     </row>
     <row r="78">
+      <c r="D78" s="7" t="inlineStr">
+        <is>
+          <t>Captured: 10:41 PM - FINAL</t>
+        </is>
+      </c>
       <c r="G78" s="4" t="inlineStr">
         <is>
           <t>Captured: 09:48 PM</t>
+        </is>
+      </c>
+      <c r="J78" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 10:41 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="80" ht="112.5" customHeight="1"/>
+    <row r="81">
+      <c r="G81" s="6" t="inlineStr">
+        <is>
+          <t>LAC Low: 0.005</t>
+        </is>
+      </c>
+      <c r="H81" s="6" t="inlineStr">
+        <is>
+          <t>HOU Low: 0.485</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="G82" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 10:41 PM</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="158">
+  <mergeCells count="164">
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D60:E60"/>
     <mergeCell ref="A64:B64"/>
@@ -6861,6 +7007,7 @@
     <mergeCell ref="G34:H34"/>
     <mergeCell ref="D72:E72"/>
     <mergeCell ref="G68:H68"/>
+    <mergeCell ref="D78:E78"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="G58:H58"/>
     <mergeCell ref="D4:E4"/>
@@ -6890,6 +7037,7 @@
     <mergeCell ref="J34:K34"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="G38:H38"/>
+    <mergeCell ref="D76:E76"/>
     <mergeCell ref="A46:B46"/>
     <mergeCell ref="G62:H62"/>
     <mergeCell ref="J36:K36"/>
@@ -6926,6 +7074,7 @@
     <mergeCell ref="J26:K26"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="J16:K16"/>
+    <mergeCell ref="G80:H80"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="A14:B14"/>
@@ -6959,6 +7108,8 @@
     <mergeCell ref="D40:E40"/>
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="A6:B6"/>
+    <mergeCell ref="J78:K78"/>
+    <mergeCell ref="G82:H82"/>
     <mergeCell ref="J30:K30"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="J6:K6"/>
@@ -6989,6 +7140,7 @@
     <mergeCell ref="D68:E68"/>
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J76:K76"/>
     <mergeCell ref="A44:B44"/>
     <mergeCell ref="G46:H46"/>
     <mergeCell ref="G40:H40"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-12 04:25 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -3774,6 +3774,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -3799,6 +3802,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -3818,6 +3824,59 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId76"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>83</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="77" name="Image 77" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId77"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>79</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="78" name="Image 78" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId78"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -5646,7 +5705,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K82"/>
+  <dimension ref="A1:K86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6974,6 +7033,16 @@
           <t>HOU Low: 0.485</t>
         </is>
       </c>
+      <c r="J81" s="6" t="inlineStr">
+        <is>
+          <t>DEN Low: 0.795</t>
+        </is>
+      </c>
+      <c r="K81" s="6" t="inlineStr">
+        <is>
+          <t>SAC Low: 0.014</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="G82" s="4" t="inlineStr">
@@ -6981,11 +7050,37 @@
           <t>Captured: 10:41 PM</t>
         </is>
       </c>
+      <c r="J82" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 11:25 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="84" ht="112.5" customHeight="1"/>
+    <row r="85">
+      <c r="G85" s="6" t="inlineStr">
+        <is>
+          <t>LAC Low: 0.485</t>
+        </is>
+      </c>
+      <c r="H85" s="6" t="inlineStr">
+        <is>
+          <t>HOU Low: 0.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="G86" s="7" t="inlineStr">
+        <is>
+          <t>Captured: 11:25 PM - FINAL</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="164">
+  <mergeCells count="168">
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D60:E60"/>
+    <mergeCell ref="J82:K82"/>
     <mergeCell ref="A64:B64"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D22:E22"/>
@@ -7022,6 +7117,7 @@
     <mergeCell ref="J62:K62"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="G44:H44"/>
+    <mergeCell ref="G84:H84"/>
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="J58:K58"/>
     <mergeCell ref="D26:E26"/>
@@ -7030,6 +7126,7 @@
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="D10:E10"/>
+    <mergeCell ref="G86:H86"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="G70:H70"/>
@@ -7114,6 +7211,7 @@
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="G10:H10"/>
+    <mergeCell ref="J80:K80"/>
     <mergeCell ref="D32:E32"/>
     <mergeCell ref="G28:H28"/>
     <mergeCell ref="A66:B66"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-12 05:15 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -11,6 +11,7 @@
     <sheet name="2025-12-09" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="2025-12-10" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="2025-12-11" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="2025-12-12" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -3858,6 +3859,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -3877,6 +3881,114 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId78"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="4" name="Image 4" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -7250,4 +7362,199 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="25" customWidth="1" min="1" max="1"/>
+    <col width="25" customWidth="1" min="2" max="2"/>
+    <col width="3" customWidth="1" min="3" max="3"/>
+    <col width="25" customWidth="1" min="4" max="4"/>
+    <col width="25" customWidth="1" min="5" max="5"/>
+    <col width="3" customWidth="1" min="6" max="6"/>
+    <col width="25" customWidth="1" min="7" max="7"/>
+    <col width="25" customWidth="1" min="8" max="8"/>
+    <col width="3" customWidth="1" min="9" max="9"/>
+    <col width="25" customWidth="1" min="10" max="10"/>
+    <col width="25" customWidth="1" min="11" max="11"/>
+    <col width="3" customWidth="1" min="12" max="12"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>CHI @ CHA</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="n"/>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>IND @ PHI</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="n"/>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>CLE @ WAS</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="n"/>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>ATL @ DET</t>
+        </is>
+      </c>
+      <c r="K1" s="2" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>12:00 AM / 2025-12-12</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n"/>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>12:00 AM / 2025-12-12</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="n"/>
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>12:00 AM / 2025-12-12</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="n"/>
+      <c r="J2" s="3" t="inlineStr">
+        <is>
+          <t>12:00 AM / 2025-12-12</t>
+        </is>
+      </c>
+      <c r="K2" s="2" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-chi-cha-2025-12-12</t>
+        </is>
+      </c>
+      <c r="D3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-ind-phi-2025-12-12</t>
+        </is>
+      </c>
+      <c r="G3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-cle-was-2025-12-12</t>
+        </is>
+      </c>
+      <c r="J3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-atl-det-2025-12-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="112.5" customHeight="1"/>
+    <row r="5">
+      <c r="A5" s="6" t="inlineStr">
+        <is>
+          <t>CHI Low: 0.555</t>
+        </is>
+      </c>
+      <c r="B5" s="6" t="inlineStr">
+        <is>
+          <t>CHA Low: 0.375</t>
+        </is>
+      </c>
+      <c r="D5" s="6" t="inlineStr">
+        <is>
+          <t>IND Low: 0.265</t>
+        </is>
+      </c>
+      <c r="E5" s="6" t="inlineStr">
+        <is>
+          <t>PHI Low: 0.715</t>
+        </is>
+      </c>
+      <c r="G5" s="6" t="inlineStr">
+        <is>
+          <t>CLE Low: 0.105</t>
+        </is>
+      </c>
+      <c r="H5" s="6" t="inlineStr">
+        <is>
+          <t>WAS Low: 0.875</t>
+        </is>
+      </c>
+      <c r="J5" s="6" t="inlineStr">
+        <is>
+          <t>ATL Low: 0.275</t>
+        </is>
+      </c>
+      <c r="K5" s="6" t="inlineStr">
+        <is>
+          <t>DET Low: 0.695</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 12:15 AM</t>
+        </is>
+      </c>
+      <c r="D6" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 12:15 AM</t>
+        </is>
+      </c>
+      <c r="G6" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 12:15 AM</t>
+        </is>
+      </c>
+      <c r="J6" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 12:15 AM</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="J2:K2"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update NBA prices - 2025-12-12 06:19 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -3920,6 +3920,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -3945,6 +3948,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -3970,6 +3976,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -3989,6 +3998,134 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>7</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="5" name="Image 5" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>7</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="6" name="Image 6" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>7</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="7" name="Image 7" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>7</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="8" name="Image 8" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>12</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="9" name="Image 9" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId9"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -7370,7 +7507,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7390,6 +7527,9 @@
     <col width="25" customWidth="1" min="10" max="10"/>
     <col width="25" customWidth="1" min="11" max="11"/>
     <col width="3" customWidth="1" min="12" max="12"/>
+    <col width="25" customWidth="1" min="13" max="13"/>
+    <col width="25" customWidth="1" min="14" max="14"/>
+    <col width="3" customWidth="1" min="15" max="15"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -7417,6 +7557,12 @@
         </is>
       </c>
       <c r="K1" s="2" t="n"/>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>UTA @ MEM</t>
+        </is>
+      </c>
+      <c r="N1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -7443,6 +7589,12 @@
         </is>
       </c>
       <c r="K2" s="2" t="n"/>
+      <c r="M2" s="3" t="inlineStr">
+        <is>
+          <t>1:00 AM / 2025-12-12</t>
+        </is>
+      </c>
+      <c r="N2" s="2" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="5" t="inlineStr">
@@ -7463,6 +7615,11 @@
       <c r="J3" s="5" t="inlineStr">
         <is>
           <t>https://polymarket.com/event/nba-atl-det-2025-12-12</t>
+        </is>
+      </c>
+      <c r="M3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-uta-mem-2025-12-12</t>
         </is>
       </c>
     </row>
@@ -7508,6 +7665,16 @@
           <t>DET Low: 0.695</t>
         </is>
       </c>
+      <c r="M5" s="6" t="inlineStr">
+        <is>
+          <t>UTA Low: 0.665</t>
+        </is>
+      </c>
+      <c r="N5" s="6" t="inlineStr">
+        <is>
+          <t>MEM Low: 0.295</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="inlineStr">
@@ -7530,29 +7697,112 @@
           <t>Captured: 12:15 AM</t>
         </is>
       </c>
+      <c r="M6" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 01:19 AM</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="112.5" customHeight="1"/>
+    <row r="9">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>CHI Low: 0.555</t>
+        </is>
+      </c>
+      <c r="B9" s="6" t="inlineStr">
+        <is>
+          <t>CHA Low: 0.375</t>
+        </is>
+      </c>
+      <c r="D9" s="6" t="inlineStr">
+        <is>
+          <t>IND Low: 0.715</t>
+        </is>
+      </c>
+      <c r="E9" s="6" t="inlineStr">
+        <is>
+          <t>PHI Low: 0.265</t>
+        </is>
+      </c>
+      <c r="G9" s="6" t="inlineStr">
+        <is>
+          <t>CLE Low: 0.880</t>
+        </is>
+      </c>
+      <c r="H9" s="6" t="inlineStr">
+        <is>
+          <t>WAS Low: 0.105</t>
+        </is>
+      </c>
+      <c r="J9" s="6" t="inlineStr">
+        <is>
+          <t>ATL Low: 0.275</t>
+        </is>
+      </c>
+      <c r="K9" s="6" t="inlineStr">
+        <is>
+          <t>DET Low: 0.695</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 01:19 AM</t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 01:19 AM</t>
+        </is>
+      </c>
+      <c r="G10" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 01:19 AM</t>
+        </is>
+      </c>
+      <c r="J10" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 01:19 AM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="33">
+    <mergeCell ref="D10:E10"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J10:K10"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="M1:N1"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="D6:E6"/>
+    <mergeCell ref="M2:N2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="J6:K6"/>
+    <mergeCell ref="G10:H10"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="A2:B2"/>
+    <mergeCell ref="M6:N6"/>
     <mergeCell ref="D4:E4"/>
+    <mergeCell ref="M3:N3"/>
     <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="J3:K3"/>
+    <mergeCell ref="D8:E8"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J2:K2"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="M4:N4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-12 07:17 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -4032,6 +4032,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -4057,6 +4060,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -4082,6 +4088,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -4107,6 +4116,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -4126,6 +4138,134 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>11</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="10" name="Image 10" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>11</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="11" name="Image 11" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>11</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="12" name="Image 12" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>11</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="13" name="Image 13" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>12</col>
+      <colOff>0</colOff>
+      <row>7</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="14" name="Image 14" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId14"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -7507,7 +7647,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7745,6 +7885,16 @@
           <t>DET Low: 0.695</t>
         </is>
       </c>
+      <c r="M9" s="6" t="inlineStr">
+        <is>
+          <t>UTA Low: 0.665</t>
+        </is>
+      </c>
+      <c r="N9" s="6" t="inlineStr">
+        <is>
+          <t>MEM Low: 0.295</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="inlineStr">
@@ -7767,12 +7917,84 @@
           <t>Captured: 01:19 AM</t>
         </is>
       </c>
+      <c r="M10" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 02:17 AM</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="112.5" customHeight="1"/>
+    <row r="13">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>CHI Low: 0.555</t>
+        </is>
+      </c>
+      <c r="B13" s="6" t="inlineStr">
+        <is>
+          <t>CHA Low: 0.395</t>
+        </is>
+      </c>
+      <c r="D13" s="6" t="inlineStr">
+        <is>
+          <t>IND Low: 0.265</t>
+        </is>
+      </c>
+      <c r="E13" s="6" t="inlineStr">
+        <is>
+          <t>PHI Low: 0.710</t>
+        </is>
+      </c>
+      <c r="G13" s="6" t="inlineStr">
+        <is>
+          <t>CLE Low: 0.105</t>
+        </is>
+      </c>
+      <c r="H13" s="6" t="inlineStr">
+        <is>
+          <t>WAS Low: 0.885</t>
+        </is>
+      </c>
+      <c r="J13" s="6" t="inlineStr">
+        <is>
+          <t>ATL Low: 0.275</t>
+        </is>
+      </c>
+      <c r="K13" s="6" t="inlineStr">
+        <is>
+          <t>DET Low: 0.695</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 02:17 AM</t>
+        </is>
+      </c>
+      <c r="D14" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 02:17 AM</t>
+        </is>
+      </c>
+      <c r="G14" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 02:17 AM</t>
+        </is>
+      </c>
+      <c r="J14" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 02:17 AM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="43">
+    <mergeCell ref="G12:H12"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J14:K14"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="A1:B1"/>
@@ -7784,23 +8006,31 @@
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="G10:H10"/>
+    <mergeCell ref="M10:N10"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="G3:H3"/>
+    <mergeCell ref="A12:B12"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="M6:N6"/>
+    <mergeCell ref="A14:B14"/>
     <mergeCell ref="D4:E4"/>
+    <mergeCell ref="G14:H14"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="A8:B8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="D8:E8"/>
+    <mergeCell ref="J12:K12"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D14:E14"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="M4:N4"/>
   </mergeCells>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-12 08:19 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -4172,6 +4172,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -4197,6 +4200,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -4222,6 +4228,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -4247,6 +4256,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -4266,6 +4278,134 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>15</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="15" name="Image 15" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>15</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="16" name="Image 16" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>15</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="17" name="Image 17" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>15</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="18" name="Image 18" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>12</col>
+      <colOff>0</colOff>
+      <row>11</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="19" name="Image 19" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId19"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -7647,7 +7787,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7965,6 +8105,16 @@
           <t>DET Low: 0.695</t>
         </is>
       </c>
+      <c r="M13" s="6" t="inlineStr">
+        <is>
+          <t>UTA Low: 0.295</t>
+        </is>
+      </c>
+      <c r="N13" s="6" t="inlineStr">
+        <is>
+          <t>MEM Low: 0.665</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="inlineStr">
@@ -7987,9 +8137,79 @@
           <t>Captured: 02:17 AM</t>
         </is>
       </c>
+      <c r="M14" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 03:19 AM</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" ht="112.5" customHeight="1"/>
+    <row r="17">
+      <c r="A17" s="6" t="inlineStr">
+        <is>
+          <t>CHI Low: 0.555</t>
+        </is>
+      </c>
+      <c r="B17" s="6" t="inlineStr">
+        <is>
+          <t>CHA Low: 0.405</t>
+        </is>
+      </c>
+      <c r="D17" s="6" t="inlineStr">
+        <is>
+          <t>IND Low: 0.265</t>
+        </is>
+      </c>
+      <c r="E17" s="6" t="inlineStr">
+        <is>
+          <t>PHI Low: 0.710</t>
+        </is>
+      </c>
+      <c r="G17" s="6" t="inlineStr">
+        <is>
+          <t>CLE Low: 0.105</t>
+        </is>
+      </c>
+      <c r="H17" s="6" t="inlineStr">
+        <is>
+          <t>WAS Low: 0.885</t>
+        </is>
+      </c>
+      <c r="J17" s="6" t="inlineStr">
+        <is>
+          <t>ATL Low: 0.695</t>
+        </is>
+      </c>
+      <c r="K17" s="6" t="inlineStr">
+        <is>
+          <t>DET Low: 0.275</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 03:19 AM</t>
+        </is>
+      </c>
+      <c r="D18" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 03:19 AM</t>
+        </is>
+      </c>
+      <c r="G18" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 03:19 AM</t>
+        </is>
+      </c>
+      <c r="J18" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 03:19 AM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="43">
+  <mergeCells count="53">
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D1:E1"/>
@@ -8003,21 +8223,28 @@
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A16:B16"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="M10:N10"/>
     <mergeCell ref="G6:H6"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="G18:H18"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D16:E16"/>
     <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="J16:K16"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="M3:N3"/>
+    <mergeCell ref="D18:E18"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="M8:N8"/>
@@ -8027,9 +8254,12 @@
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="J12:K12"/>
+    <mergeCell ref="G16:H16"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="A10:B10"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="J18:K18"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="M4:N4"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-12 09:16 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -4312,6 +4312,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -4337,6 +4340,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -4362,6 +4368,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -4387,6 +4396,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -4406,6 +4418,134 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>19</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="20" name="Image 20" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>19</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="21" name="Image 21" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>19</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="22" name="Image 22" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>19</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="23" name="Image 23" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>12</col>
+      <colOff>0</colOff>
+      <row>15</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="24" name="Image 24" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId24"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -7787,7 +7927,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8185,6 +8325,16 @@
           <t>DET Low: 0.275</t>
         </is>
       </c>
+      <c r="M17" s="6" t="inlineStr">
+        <is>
+          <t>UTA Low: 0.295</t>
+        </is>
+      </c>
+      <c r="N17" s="6" t="inlineStr">
+        <is>
+          <t>MEM Low: 0.695</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="inlineStr">
@@ -8207,9 +8357,80 @@
           <t>Captured: 03:19 AM</t>
         </is>
       </c>
+      <c r="M18" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 04:16 AM</t>
+        </is>
+      </c>
+    </row>
+    <row r="20" ht="112.5" customHeight="1"/>
+    <row r="21">
+      <c r="A21" s="6" t="inlineStr">
+        <is>
+          <t>CHI Low: 0.420</t>
+        </is>
+      </c>
+      <c r="B21" s="6" t="inlineStr">
+        <is>
+          <t>CHA Low: 0.565</t>
+        </is>
+      </c>
+      <c r="D21" s="6" t="inlineStr">
+        <is>
+          <t>IND Low: 0.265</t>
+        </is>
+      </c>
+      <c r="E21" s="6" t="inlineStr">
+        <is>
+          <t>PHI Low: 0.710</t>
+        </is>
+      </c>
+      <c r="G21" s="6" t="inlineStr">
+        <is>
+          <t>CLE Low: 0.105</t>
+        </is>
+      </c>
+      <c r="H21" s="6" t="inlineStr">
+        <is>
+          <t>WAS Low: 0.885</t>
+        </is>
+      </c>
+      <c r="J21" s="6" t="inlineStr">
+        <is>
+          <t>ATL Low: 0.275</t>
+        </is>
+      </c>
+      <c r="K21" s="6" t="inlineStr">
+        <is>
+          <t>DET Low: 0.705</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 04:16 AM</t>
+        </is>
+      </c>
+      <c r="D22" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 04:16 AM</t>
+        </is>
+      </c>
+      <c r="G22" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 04:16 AM</t>
+        </is>
+      </c>
+      <c r="J22" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 04:16 AM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="53">
+  <mergeCells count="63">
+    <mergeCell ref="D20:E20"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D1:E1"/>
@@ -8217,6 +8438,7 @@
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="J1:K1"/>
+    <mergeCell ref="D22:E22"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="M1:N1"/>
@@ -8234,9 +8456,11 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="M16:N16"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D16:E16"/>
+    <mergeCell ref="J20:K20"/>
     <mergeCell ref="M6:N6"/>
     <mergeCell ref="M12:N12"/>
     <mergeCell ref="J16:K16"/>
@@ -8245,14 +8469,19 @@
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="D18:E18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="J22:K22"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="M8:N8"/>
+    <mergeCell ref="A22:B22"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="D8:E8"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="G20:H20"/>
     <mergeCell ref="J12:K12"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G1:H1"/>
@@ -8261,6 +8490,7 @@
     <mergeCell ref="M14:N14"/>
     <mergeCell ref="J18:K18"/>
     <mergeCell ref="D14:E14"/>
+    <mergeCell ref="G22:H22"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="M4:N4"/>
   </mergeCells>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-12 10:15 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -4452,6 +4452,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -4477,6 +4480,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -4502,6 +4508,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -4527,6 +4536,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -4546,6 +4558,134 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>23</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="25" name="Image 25" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>23</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="26" name="Image 26" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>23</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="27" name="Image 27" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>23</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="28" name="Image 28" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>12</col>
+      <colOff>0</colOff>
+      <row>19</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="29" name="Image 29" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId29"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -7927,7 +8067,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8405,6 +8545,16 @@
           <t>DET Low: 0.705</t>
         </is>
       </c>
+      <c r="M21" s="6" t="inlineStr">
+        <is>
+          <t>UTA Low: 0.295</t>
+        </is>
+      </c>
+      <c r="N21" s="6" t="inlineStr">
+        <is>
+          <t>MEM Low: 0.695</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="4" t="inlineStr">
@@ -8427,10 +8577,81 @@
           <t>Captured: 04:16 AM</t>
         </is>
       </c>
+      <c r="M22" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 05:15 AM</t>
+        </is>
+      </c>
+    </row>
+    <row r="24" ht="112.5" customHeight="1"/>
+    <row r="25">
+      <c r="A25" s="6" t="inlineStr">
+        <is>
+          <t>CHI Low: 0.565</t>
+        </is>
+      </c>
+      <c r="B25" s="6" t="inlineStr">
+        <is>
+          <t>CHA Low: 0.425</t>
+        </is>
+      </c>
+      <c r="D25" s="6" t="inlineStr">
+        <is>
+          <t>IND Low: 0.710</t>
+        </is>
+      </c>
+      <c r="E25" s="6" t="inlineStr">
+        <is>
+          <t>PHI Low: 0.265</t>
+        </is>
+      </c>
+      <c r="G25" s="6" t="inlineStr">
+        <is>
+          <t>CLE Low: 0.885</t>
+        </is>
+      </c>
+      <c r="H25" s="6" t="inlineStr">
+        <is>
+          <t>WAS Low: 0.105</t>
+        </is>
+      </c>
+      <c r="J25" s="6" t="inlineStr">
+        <is>
+          <t>ATL Low: 0.715</t>
+        </is>
+      </c>
+      <c r="K25" s="6" t="inlineStr">
+        <is>
+          <t>DET Low: 0.275</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 05:15 AM</t>
+        </is>
+      </c>
+      <c r="D26" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 05:15 AM</t>
+        </is>
+      </c>
+      <c r="G26" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 05:15 AM</t>
+        </is>
+      </c>
+      <c r="J26" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 05:15 AM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="63">
+  <mergeCells count="73">
     <mergeCell ref="D20:E20"/>
+    <mergeCell ref="A24:B24"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D1:E1"/>
@@ -8447,22 +8668,29 @@
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="D2:E2"/>
+    <mergeCell ref="M20:N20"/>
     <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J24:K24"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="M10:N10"/>
     <mergeCell ref="G6:H6"/>
+    <mergeCell ref="D26:E26"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="G3:H3"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="J26:K26"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="M16:N16"/>
+    <mergeCell ref="A26:B26"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="J20:K20"/>
     <mergeCell ref="M6:N6"/>
     <mergeCell ref="M12:N12"/>
+    <mergeCell ref="G24:H24"/>
     <mergeCell ref="J16:K16"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="D4:E4"/>
@@ -8476,6 +8704,7 @@
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="D12:E12"/>
+    <mergeCell ref="G26:H26"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="J3:K3"/>
@@ -8483,6 +8712,7 @@
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="J12:K12"/>
+    <mergeCell ref="D24:E24"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J2:K2"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-12 11:15 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -4592,6 +4592,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -4617,6 +4620,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -4642,6 +4648,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -4667,6 +4676,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -4686,6 +4698,134 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>27</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="30" name="Image 30" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId30"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>27</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="31" name="Image 31" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId31"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>27</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="32" name="Image 32" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId32"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>27</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="33" name="Image 33" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId33"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>12</col>
+      <colOff>0</colOff>
+      <row>23</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="34" name="Image 34" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId34"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -8067,7 +8207,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8625,6 +8765,16 @@
           <t>DET Low: 0.275</t>
         </is>
       </c>
+      <c r="M25" s="6" t="inlineStr">
+        <is>
+          <t>UTA Low: 0.695</t>
+        </is>
+      </c>
+      <c r="N25" s="6" t="inlineStr">
+        <is>
+          <t>MEM Low: 0.285</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="4" t="inlineStr">
@@ -8647,80 +8797,160 @@
           <t>Captured: 05:15 AM</t>
         </is>
       </c>
+      <c r="M26" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 06:15 AM</t>
+        </is>
+      </c>
+    </row>
+    <row r="28" ht="112.5" customHeight="1"/>
+    <row r="29">
+      <c r="A29" s="6" t="inlineStr">
+        <is>
+          <t>CHI Low: 0.565</t>
+        </is>
+      </c>
+      <c r="B29" s="6" t="inlineStr">
+        <is>
+          <t>CHA Low: 0.425</t>
+        </is>
+      </c>
+      <c r="D29" s="6" t="inlineStr">
+        <is>
+          <t>IND Low: 0.710</t>
+        </is>
+      </c>
+      <c r="E29" s="6" t="inlineStr">
+        <is>
+          <t>PHI Low: 0.275</t>
+        </is>
+      </c>
+      <c r="G29" s="6" t="inlineStr">
+        <is>
+          <t>CLE Low: 0.105</t>
+        </is>
+      </c>
+      <c r="H29" s="6" t="inlineStr">
+        <is>
+          <t>WAS Low: 0.885</t>
+        </is>
+      </c>
+      <c r="J29" s="6" t="inlineStr">
+        <is>
+          <t>ATL Low: 0.725</t>
+        </is>
+      </c>
+      <c r="K29" s="6" t="inlineStr">
+        <is>
+          <t>DET Low: 0.275</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 06:15 AM</t>
+        </is>
+      </c>
+      <c r="D30" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 06:15 AM</t>
+        </is>
+      </c>
+      <c r="G30" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 06:15 AM</t>
+        </is>
+      </c>
+      <c r="J30" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 06:15 AM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="73">
+  <mergeCells count="83">
     <mergeCell ref="D20:E20"/>
-    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="A30:B30"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="D10:E10"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="A10:B10"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A24:B24"/>
     <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="A1:B1"/>
     <mergeCell ref="G8:H8"/>
-    <mergeCell ref="M1:N1"/>
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="J30:K30"/>
     <mergeCell ref="A16:B16"/>
-    <mergeCell ref="D2:E2"/>
     <mergeCell ref="M20:N20"/>
     <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J24:K24"/>
     <mergeCell ref="G10:H10"/>
-    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="G28:H28"/>
     <mergeCell ref="G6:H6"/>
-    <mergeCell ref="D26:E26"/>
     <mergeCell ref="A18:B18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="A3:B3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="M22:N22"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="D16:E16"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="J20:K20"/>
     <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="G30:H30"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="D18:E18"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D8:E8"/>
     <mergeCell ref="G4:H4"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="D8:E8"/>
     <mergeCell ref="A20:B20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="A10:B10"/>
     <mergeCell ref="M14:N14"/>
     <mergeCell ref="J18:K18"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="G22:H22"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="M4:N4"/>
   </mergeCells>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-12 12:21 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -4732,6 +4732,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -4757,6 +4760,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -4782,6 +4788,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -4807,6 +4816,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -4826,6 +4838,134 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId34"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>31</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="35" name="Image 35" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId35"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>31</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="36" name="Image 36" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId36"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>31</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="37" name="Image 37" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId37"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>31</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="38" name="Image 38" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId38"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>12</col>
+      <colOff>0</colOff>
+      <row>27</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="39" name="Image 39" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId39"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -8207,7 +8347,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8845,6 +8985,16 @@
           <t>DET Low: 0.275</t>
         </is>
       </c>
+      <c r="M29" s="6" t="inlineStr">
+        <is>
+          <t>UTA Low: 0.285</t>
+        </is>
+      </c>
+      <c r="N29" s="6" t="inlineStr">
+        <is>
+          <t>MEM Low: 0.695</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="4" t="inlineStr">
@@ -8867,9 +9017,79 @@
           <t>Captured: 06:15 AM</t>
         </is>
       </c>
+      <c r="M30" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 07:21 AM</t>
+        </is>
+      </c>
+    </row>
+    <row r="32" ht="112.5" customHeight="1"/>
+    <row r="33">
+      <c r="A33" s="6" t="inlineStr">
+        <is>
+          <t>CHI Low: 0.565</t>
+        </is>
+      </c>
+      <c r="B33" s="6" t="inlineStr">
+        <is>
+          <t>CHA Low: 0.425</t>
+        </is>
+      </c>
+      <c r="D33" s="6" t="inlineStr">
+        <is>
+          <t>IND Low: 0.265</t>
+        </is>
+      </c>
+      <c r="E33" s="6" t="inlineStr">
+        <is>
+          <t>PHI Low: 0.710</t>
+        </is>
+      </c>
+      <c r="G33" s="6" t="inlineStr">
+        <is>
+          <t>CLE Low: 0.885</t>
+        </is>
+      </c>
+      <c r="H33" s="6" t="inlineStr">
+        <is>
+          <t>WAS Low: 0.105</t>
+        </is>
+      </c>
+      <c r="J33" s="6" t="inlineStr">
+        <is>
+          <t>ATL Low: 0.275</t>
+        </is>
+      </c>
+      <c r="K33" s="6" t="inlineStr">
+        <is>
+          <t>DET Low: 0.725</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 07:21 AM</t>
+        </is>
+      </c>
+      <c r="D34" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 07:21 AM</t>
+        </is>
+      </c>
+      <c r="G34" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 07:21 AM</t>
+        </is>
+      </c>
+      <c r="J34" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 07:21 AM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="83">
+  <mergeCells count="93">
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D22:E22"/>
@@ -8879,6 +9099,7 @@
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="M16:N16"/>
     <mergeCell ref="J4:K4"/>
+    <mergeCell ref="G34:H34"/>
     <mergeCell ref="M18:N18"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="M8:N8"/>
@@ -8891,8 +9112,10 @@
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D34:E34"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="M1:N1"/>
+    <mergeCell ref="J34:K34"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="J20:K20"/>
@@ -8905,6 +9128,7 @@
     <mergeCell ref="J12:K12"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A34:B34"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="A1:B1"/>
@@ -8915,6 +9139,7 @@
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="M12:N12"/>
     <mergeCell ref="J16:K16"/>
+    <mergeCell ref="A32:B32"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="D3:E3"/>
@@ -8924,6 +9149,7 @@
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J2:K2"/>
+    <mergeCell ref="G32:H32"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="J14:K14"/>
@@ -8934,15 +9160,19 @@
     <mergeCell ref="M20:N20"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="G10:H10"/>
+    <mergeCell ref="D32:E32"/>
     <mergeCell ref="G28:H28"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="M22:N22"/>
+    <mergeCell ref="M30:N30"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="M6:N6"/>
     <mergeCell ref="G30:H30"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="M28:N28"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="D18:E18"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-12 13:24 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -4872,6 +4872,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -4897,6 +4900,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -4922,6 +4928,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -4947,6 +4956,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -4966,6 +4978,134 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId39"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>35</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="40" name="Image 40" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId40"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>35</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="41" name="Image 41" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId41"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>35</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="42" name="Image 42" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId42"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>35</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="43" name="Image 43" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId43"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>12</col>
+      <colOff>0</colOff>
+      <row>31</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="44" name="Image 44" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId44"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -8347,7 +8487,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9065,6 +9205,16 @@
           <t>DET Low: 0.725</t>
         </is>
       </c>
+      <c r="M33" s="6" t="inlineStr">
+        <is>
+          <t>UTA Low: 0.285</t>
+        </is>
+      </c>
+      <c r="N33" s="6" t="inlineStr">
+        <is>
+          <t>MEM Low: 0.695</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="4" t="inlineStr">
@@ -9087,13 +9237,84 @@
           <t>Captured: 07:21 AM</t>
         </is>
       </c>
+      <c r="M34" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 08:24 AM</t>
+        </is>
+      </c>
+    </row>
+    <row r="36" ht="112.5" customHeight="1"/>
+    <row r="37">
+      <c r="A37" s="6" t="inlineStr">
+        <is>
+          <t>CHI Low: 0.425</t>
+        </is>
+      </c>
+      <c r="B37" s="6" t="inlineStr">
+        <is>
+          <t>CHA Low: 0.565</t>
+        </is>
+      </c>
+      <c r="D37" s="6" t="inlineStr">
+        <is>
+          <t>IND Low: 0.710</t>
+        </is>
+      </c>
+      <c r="E37" s="6" t="inlineStr">
+        <is>
+          <t>PHI Low: 0.265</t>
+        </is>
+      </c>
+      <c r="G37" s="6" t="inlineStr">
+        <is>
+          <t>CLE Low: 0.105</t>
+        </is>
+      </c>
+      <c r="H37" s="6" t="inlineStr">
+        <is>
+          <t>WAS Low: 0.885</t>
+        </is>
+      </c>
+      <c r="J37" s="6" t="inlineStr">
+        <is>
+          <t>ATL Low: 0.275</t>
+        </is>
+      </c>
+      <c r="K37" s="6" t="inlineStr">
+        <is>
+          <t>DET Low: 0.725</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 08:24 AM</t>
+        </is>
+      </c>
+      <c r="D38" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 08:24 AM</t>
+        </is>
+      </c>
+      <c r="G38" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 08:24 AM</t>
+        </is>
+      </c>
+      <c r="J38" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 08:24 AM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="93">
+  <mergeCells count="103">
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="J28:K28"/>
+    <mergeCell ref="D36:E36"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="M10:N10"/>
     <mergeCell ref="G18:H18"/>
@@ -9117,6 +9338,8 @@
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="J34:K34"/>
     <mergeCell ref="D2:E2"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="J36:K36"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="J20:K20"/>
     <mergeCell ref="G24:H24"/>
@@ -9128,9 +9351,13 @@
     <mergeCell ref="J12:K12"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D38:E38"/>
     <mergeCell ref="A34:B34"/>
+    <mergeCell ref="M34:N34"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="A36:B36"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="J24:K24"/>
@@ -9146,6 +9373,7 @@
     <mergeCell ref="M26:N26"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A38:B38"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J2:K2"/>
@@ -9153,6 +9381,7 @@
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="J14:K14"/>
+    <mergeCell ref="G36:H36"/>
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="J30:K30"/>
@@ -9179,6 +9408,7 @@
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="A20:B20"/>
+    <mergeCell ref="M32:N32"/>
     <mergeCell ref="M14:N14"/>
     <mergeCell ref="J18:K18"/>
     <mergeCell ref="J8:K8"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-12 14:19 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -5012,6 +5012,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -5037,6 +5040,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -5062,6 +5068,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -5087,6 +5096,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -5106,6 +5118,84 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId44"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>39</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="45" name="Image 45" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId45"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>39</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="46" name="Image 46" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId46"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>12</col>
+      <colOff>0</colOff>
+      <row>35</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="47" name="Image 47" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId47"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -8487,7 +8577,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N38"/>
+  <dimension ref="A1:N42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9285,6 +9375,16 @@
           <t>DET Low: 0.725</t>
         </is>
       </c>
+      <c r="M37" s="6" t="inlineStr">
+        <is>
+          <t>UTA Low: 0.285</t>
+        </is>
+      </c>
+      <c r="N37" s="6" t="inlineStr">
+        <is>
+          <t>MEM Low: 0.695</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="4" t="inlineStr">
@@ -9307,9 +9407,49 @@
           <t>Captured: 08:24 AM</t>
         </is>
       </c>
+      <c r="M38" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 09:19 AM</t>
+        </is>
+      </c>
+    </row>
+    <row r="40" ht="112.5" customHeight="1"/>
+    <row r="41">
+      <c r="D41" s="6" t="inlineStr">
+        <is>
+          <t>IND Low: 0.710</t>
+        </is>
+      </c>
+      <c r="E41" s="6" t="inlineStr">
+        <is>
+          <t>PHI Low: 0.265</t>
+        </is>
+      </c>
+      <c r="J41" s="6" t="inlineStr">
+        <is>
+          <t>ATL Low: 0.725</t>
+        </is>
+      </c>
+      <c r="K41" s="6" t="inlineStr">
+        <is>
+          <t>DET Low: 0.275</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="D42" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 09:19 AM</t>
+        </is>
+      </c>
+      <c r="J42" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 09:19 AM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="103">
+  <mergeCells count="109">
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D22:E22"/>
@@ -9321,6 +9461,7 @@
     <mergeCell ref="M16:N16"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="G34:H34"/>
+    <mergeCell ref="M36:N36"/>
     <mergeCell ref="M18:N18"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="M8:N8"/>
@@ -9359,6 +9500,7 @@
     <mergeCell ref="J38:K38"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="J40:K40"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="J24:K24"/>
     <mergeCell ref="A3:B3"/>
@@ -9378,10 +9520,13 @@
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="G32:H32"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="J42:K42"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="G36:H36"/>
+    <mergeCell ref="D40:E40"/>
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="J30:K30"/>
@@ -9408,6 +9553,7 @@
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D42:E42"/>
     <mergeCell ref="M32:N32"/>
     <mergeCell ref="M14:N14"/>
     <mergeCell ref="J18:K18"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-12 15:15 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -5152,6 +5152,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -5177,6 +5180,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -5196,6 +5202,134 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId47"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>43</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="48" name="Image 48" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId48"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>39</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="49" name="Image 49" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId49"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>39</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="50" name="Image 50" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId50"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>43</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="51" name="Image 51" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId51"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>12</col>
+      <colOff>0</colOff>
+      <row>39</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="52" name="Image 52" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId52"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -8577,7 +8711,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N42"/>
+  <dimension ref="A1:N46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9415,6 +9549,16 @@
     </row>
     <row r="40" ht="112.5" customHeight="1"/>
     <row r="41">
+      <c r="A41" s="6" t="inlineStr">
+        <is>
+          <t>CHI Low: 0.565</t>
+        </is>
+      </c>
+      <c r="B41" s="6" t="inlineStr">
+        <is>
+          <t>CHA Low: 0.415</t>
+        </is>
+      </c>
       <c r="D41" s="6" t="inlineStr">
         <is>
           <t>IND Low: 0.710</t>
@@ -9425,6 +9569,16 @@
           <t>PHI Low: 0.265</t>
         </is>
       </c>
+      <c r="G41" s="6" t="inlineStr">
+        <is>
+          <t>CLE Low: 0.105</t>
+        </is>
+      </c>
+      <c r="H41" s="6" t="inlineStr">
+        <is>
+          <t>WAS Low: 0.885</t>
+        </is>
+      </c>
       <c r="J41" s="6" t="inlineStr">
         <is>
           <t>ATL Low: 0.725</t>
@@ -9433,34 +9587,96 @@
       <c r="K41" s="6" t="inlineStr">
         <is>
           <t>DET Low: 0.275</t>
+        </is>
+      </c>
+      <c r="M41" s="6" t="inlineStr">
+        <is>
+          <t>UTA Low: 0.695</t>
+        </is>
+      </c>
+      <c r="N41" s="6" t="inlineStr">
+        <is>
+          <t>MEM Low: 0.285</t>
         </is>
       </c>
     </row>
     <row r="42">
+      <c r="A42" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 10:15 AM</t>
+        </is>
+      </c>
       <c r="D42" s="4" t="inlineStr">
         <is>
           <t>Captured: 09:19 AM</t>
         </is>
       </c>
+      <c r="G42" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 10:15 AM</t>
+        </is>
+      </c>
       <c r="J42" s="4" t="inlineStr">
         <is>
           <t>Captured: 09:19 AM</t>
+        </is>
+      </c>
+      <c r="M42" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 10:15 AM</t>
+        </is>
+      </c>
+    </row>
+    <row r="44" ht="112.5" customHeight="1"/>
+    <row r="45">
+      <c r="D45" s="6" t="inlineStr">
+        <is>
+          <t>IND Low: 0.265</t>
+        </is>
+      </c>
+      <c r="E45" s="6" t="inlineStr">
+        <is>
+          <t>PHI Low: 0.685</t>
+        </is>
+      </c>
+      <c r="J45" s="6" t="inlineStr">
+        <is>
+          <t>ATL Low: 0.725</t>
+        </is>
+      </c>
+      <c r="K45" s="6" t="inlineStr">
+        <is>
+          <t>DET Low: 0.275</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="D46" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 10:15 AM</t>
+        </is>
+      </c>
+      <c r="J46" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 10:15 AM</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="109">
+  <mergeCells count="119">
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="J28:K28"/>
     <mergeCell ref="D36:E36"/>
     <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D44:E44"/>
     <mergeCell ref="M10:N10"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="M16:N16"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="G34:H34"/>
+    <mergeCell ref="A42:B42"/>
     <mergeCell ref="M36:N36"/>
     <mergeCell ref="M18:N18"/>
     <mergeCell ref="D4:E4"/>
@@ -9491,6 +9707,7 @@
     <mergeCell ref="M24:N24"/>
     <mergeCell ref="J12:K12"/>
     <mergeCell ref="G16:H16"/>
+    <mergeCell ref="J46:K46"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="D38:E38"/>
     <mergeCell ref="A34:B34"/>
@@ -9498,12 +9715,14 @@
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="J38:K38"/>
+    <mergeCell ref="G42:H42"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="J40:K40"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="J24:K24"/>
     <mergeCell ref="A3:B3"/>
+    <mergeCell ref="M40:N40"/>
     <mergeCell ref="J26:K26"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="M12:N12"/>
@@ -9523,9 +9742,12 @@
     <mergeCell ref="M38:N38"/>
     <mergeCell ref="J42:K42"/>
     <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A40:B40"/>
     <mergeCell ref="A24:B24"/>
+    <mergeCell ref="J44:K44"/>
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="G36:H36"/>
+    <mergeCell ref="D46:E46"/>
     <mergeCell ref="D40:E40"/>
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="A6:B6"/>
@@ -9547,6 +9769,7 @@
     <mergeCell ref="G30:H30"/>
     <mergeCell ref="J32:K32"/>
     <mergeCell ref="M28:N28"/>
+    <mergeCell ref="M42:N42"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="D18:E18"/>
@@ -9557,6 +9780,7 @@
     <mergeCell ref="M32:N32"/>
     <mergeCell ref="M14:N14"/>
     <mergeCell ref="J18:K18"/>
+    <mergeCell ref="G40:H40"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="M4:N4"/>
   </mergeCells>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-12 16:21 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -5236,6 +5236,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -5261,6 +5264,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -5286,6 +5292,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -5311,6 +5320,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -5330,6 +5342,84 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId52"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>43</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="53" name="Image 53" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId53"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>47</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="54" name="Image 54" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId54"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>43</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="55" name="Image 55" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId55"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -8711,7 +8801,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N46"/>
+  <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9629,6 +9719,16 @@
     </row>
     <row r="44" ht="112.5" customHeight="1"/>
     <row r="45">
+      <c r="A45" s="6" t="inlineStr">
+        <is>
+          <t>CHI Low: 0.415</t>
+        </is>
+      </c>
+      <c r="B45" s="6" t="inlineStr">
+        <is>
+          <t>CHA Low: 0.565</t>
+        </is>
+      </c>
       <c r="D45" s="6" t="inlineStr">
         <is>
           <t>IND Low: 0.265</t>
@@ -9637,6 +9737,16 @@
       <c r="E45" s="6" t="inlineStr">
         <is>
           <t>PHI Low: 0.685</t>
+        </is>
+      </c>
+      <c r="G45" s="6" t="inlineStr">
+        <is>
+          <t>CLE Low: 0.105</t>
+        </is>
+      </c>
+      <c r="H45" s="6" t="inlineStr">
+        <is>
+          <t>WAS Low: 0.885</t>
         </is>
       </c>
       <c r="J45" s="6" t="inlineStr">
@@ -9651,28 +9761,60 @@
       </c>
     </row>
     <row r="46">
+      <c r="A46" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 11:21 AM</t>
+        </is>
+      </c>
       <c r="D46" s="4" t="inlineStr">
         <is>
           <t>Captured: 10:15 AM</t>
         </is>
       </c>
+      <c r="G46" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 11:21 AM</t>
+        </is>
+      </c>
       <c r="J46" s="4" t="inlineStr">
         <is>
           <t>Captured: 10:15 AM</t>
+        </is>
+      </c>
+    </row>
+    <row r="48" ht="112.5" customHeight="1"/>
+    <row r="49">
+      <c r="D49" s="6" t="inlineStr">
+        <is>
+          <t>IND Low: 0.265</t>
+        </is>
+      </c>
+      <c r="E49" s="6" t="inlineStr">
+        <is>
+          <t>PHI Low: 0.685</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="D50" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 11:21 AM</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="119">
+  <mergeCells count="125">
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="J28:K28"/>
     <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D50:E50"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D44:E44"/>
     <mergeCell ref="M10:N10"/>
     <mergeCell ref="G18:H18"/>
+    <mergeCell ref="D48:E48"/>
     <mergeCell ref="M16:N16"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="G34:H34"/>
@@ -9685,6 +9827,7 @@
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="A28:B28"/>
+    <mergeCell ref="G44:H44"/>
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="A30:B30"/>
@@ -9696,6 +9839,7 @@
     <mergeCell ref="J34:K34"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="G38:H38"/>
+    <mergeCell ref="A46:B46"/>
     <mergeCell ref="J36:K36"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="J20:K20"/>
@@ -9780,6 +9924,8 @@
     <mergeCell ref="M32:N32"/>
     <mergeCell ref="M14:N14"/>
     <mergeCell ref="J18:K18"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="G46:H46"/>
     <mergeCell ref="G40:H40"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="M4:N4"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-12 17:14 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -5376,6 +5376,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -5401,6 +5404,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -5420,6 +5426,134 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId55"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>51</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="56" name="Image 56" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId56"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>47</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="57" name="Image 57" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId57"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>47</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="58" name="Image 58" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId58"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>47</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="59" name="Image 59" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId59"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>12</col>
+      <colOff>0</colOff>
+      <row>43</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="60" name="Image 60" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId60"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -8801,7 +8935,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N50"/>
+  <dimension ref="A1:N54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9759,6 +9893,16 @@
           <t>DET Low: 0.275</t>
         </is>
       </c>
+      <c r="M45" s="6" t="inlineStr">
+        <is>
+          <t>UTA Low: 0.275</t>
+        </is>
+      </c>
+      <c r="N45" s="6" t="inlineStr">
+        <is>
+          <t>MEM Low: 0.700</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="4" t="inlineStr">
@@ -9781,9 +9925,24 @@
           <t>Captured: 10:15 AM</t>
         </is>
       </c>
+      <c r="M46" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 12:14 PM</t>
+        </is>
+      </c>
     </row>
     <row r="48" ht="112.5" customHeight="1"/>
     <row r="49">
+      <c r="A49" s="6" t="inlineStr">
+        <is>
+          <t>CHI Low: 0.415</t>
+        </is>
+      </c>
+      <c r="B49" s="6" t="inlineStr">
+        <is>
+          <t>CHA Low: 0.565</t>
+        </is>
+      </c>
       <c r="D49" s="6" t="inlineStr">
         <is>
           <t>IND Low: 0.265</t>
@@ -9792,18 +9951,73 @@
       <c r="E49" s="6" t="inlineStr">
         <is>
           <t>PHI Low: 0.685</t>
+        </is>
+      </c>
+      <c r="G49" s="6" t="inlineStr">
+        <is>
+          <t>CLE Low: 0.885</t>
+        </is>
+      </c>
+      <c r="H49" s="6" t="inlineStr">
+        <is>
+          <t>WAS Low: 0.105</t>
+        </is>
+      </c>
+      <c r="J49" s="6" t="inlineStr">
+        <is>
+          <t>ATL Low: 0.725</t>
+        </is>
+      </c>
+      <c r="K49" s="6" t="inlineStr">
+        <is>
+          <t>DET Low: 0.275</t>
         </is>
       </c>
     </row>
     <row r="50">
+      <c r="A50" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 12:14 PM</t>
+        </is>
+      </c>
       <c r="D50" s="4" t="inlineStr">
         <is>
           <t>Captured: 11:21 AM</t>
+        </is>
+      </c>
+      <c r="G50" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 12:14 PM</t>
+        </is>
+      </c>
+      <c r="J50" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 12:14 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="52" ht="112.5" customHeight="1"/>
+    <row r="53">
+      <c r="D53" s="6" t="inlineStr">
+        <is>
+          <t>IND Low: 0.685</t>
+        </is>
+      </c>
+      <c r="E53" s="6" t="inlineStr">
+        <is>
+          <t>PHI Low: 0.265</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="D54" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 12:14 PM</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="125">
+  <mergeCells count="135">
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D22:E22"/>
@@ -9830,12 +10044,15 @@
     <mergeCell ref="G44:H44"/>
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="D26:E26"/>
+    <mergeCell ref="A48:B48"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D34:E34"/>
+    <mergeCell ref="M44:N44"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="M1:N1"/>
+    <mergeCell ref="G48:H48"/>
     <mergeCell ref="J34:K34"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="G38:H38"/>
@@ -9854,6 +10071,7 @@
     <mergeCell ref="J46:K46"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="D38:E38"/>
+    <mergeCell ref="J48:K48"/>
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="M34:N34"/>
     <mergeCell ref="D1:E1"/>
@@ -9864,6 +10082,7 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="J40:K40"/>
     <mergeCell ref="M2:N2"/>
+    <mergeCell ref="D52:E52"/>
     <mergeCell ref="J24:K24"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="M40:N40"/>
@@ -9880,12 +10099,15 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="D30:E30"/>
+    <mergeCell ref="J50:K50"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="G32:H32"/>
     <mergeCell ref="M38:N38"/>
     <mergeCell ref="J42:K42"/>
     <mergeCell ref="D14:E14"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="D54:E54"/>
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="J44:K44"/>
@@ -9906,11 +10128,13 @@
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="M22:N22"/>
+    <mergeCell ref="A50:B50"/>
     <mergeCell ref="M30:N30"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="M6:N6"/>
     <mergeCell ref="G30:H30"/>
+    <mergeCell ref="M46:N46"/>
     <mergeCell ref="J32:K32"/>
     <mergeCell ref="M28:N28"/>
     <mergeCell ref="M42:N42"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-12 18:19 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -5460,6 +5460,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -5485,6 +5488,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -5510,6 +5516,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -5535,6 +5544,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -5554,6 +5566,134 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId60"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>55</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="61" name="Image 61" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId61"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>51</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="62" name="Image 62" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId62"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>51</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="63" name="Image 63" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId63"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>51</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="64" name="Image 64" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId64"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>12</col>
+      <colOff>0</colOff>
+      <row>47</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="65" name="Image 65" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId65"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -8935,7 +9075,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N54"/>
+  <dimension ref="A1:N58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9973,6 +10113,16 @@
           <t>DET Low: 0.275</t>
         </is>
       </c>
+      <c r="M49" s="6" t="inlineStr">
+        <is>
+          <t>UTA Low: 0.275</t>
+        </is>
+      </c>
+      <c r="N49" s="6" t="inlineStr">
+        <is>
+          <t>MEM Low: 0.705</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="4" t="inlineStr">
@@ -9995,9 +10145,24 @@
           <t>Captured: 12:14 PM</t>
         </is>
       </c>
+      <c r="M50" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 01:19 PM</t>
+        </is>
+      </c>
     </row>
     <row r="52" ht="112.5" customHeight="1"/>
     <row r="53">
+      <c r="A53" s="6" t="inlineStr">
+        <is>
+          <t>CHI Low: 0.415</t>
+        </is>
+      </c>
+      <c r="B53" s="6" t="inlineStr">
+        <is>
+          <t>CHA Low: 0.565</t>
+        </is>
+      </c>
       <c r="D53" s="6" t="inlineStr">
         <is>
           <t>IND Low: 0.685</t>
@@ -10006,18 +10171,73 @@
       <c r="E53" s="6" t="inlineStr">
         <is>
           <t>PHI Low: 0.265</t>
+        </is>
+      </c>
+      <c r="G53" s="6" t="inlineStr">
+        <is>
+          <t>CLE Low: 0.105</t>
+        </is>
+      </c>
+      <c r="H53" s="6" t="inlineStr">
+        <is>
+          <t>WAS Low: 0.885</t>
+        </is>
+      </c>
+      <c r="J53" s="6" t="inlineStr">
+        <is>
+          <t>ATL Low: 0.275</t>
+        </is>
+      </c>
+      <c r="K53" s="6" t="inlineStr">
+        <is>
+          <t>DET Low: 0.725</t>
         </is>
       </c>
     </row>
     <row r="54">
+      <c r="A54" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 01:19 PM</t>
+        </is>
+      </c>
       <c r="D54" s="4" t="inlineStr">
         <is>
           <t>Captured: 12:14 PM</t>
+        </is>
+      </c>
+      <c r="G54" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 01:19 PM</t>
+        </is>
+      </c>
+      <c r="J54" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 01:19 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="56" ht="112.5" customHeight="1"/>
+    <row r="57">
+      <c r="D57" s="6" t="inlineStr">
+        <is>
+          <t>IND Low: 0.685</t>
+        </is>
+      </c>
+      <c r="E57" s="6" t="inlineStr">
+        <is>
+          <t>PHI Low: 0.265</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="D58" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 01:19 PM</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="135">
+  <mergeCells count="145">
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D22:E22"/>
@@ -10025,6 +10245,7 @@
     <mergeCell ref="D36:E36"/>
     <mergeCell ref="D50:E50"/>
     <mergeCell ref="D6:E6"/>
+    <mergeCell ref="A54:B54"/>
     <mergeCell ref="D44:E44"/>
     <mergeCell ref="M10:N10"/>
     <mergeCell ref="G18:H18"/>
@@ -10036,11 +10257,13 @@
     <mergeCell ref="M36:N36"/>
     <mergeCell ref="M18:N18"/>
     <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D56:E56"/>
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="A28:B28"/>
+    <mergeCell ref="M50:N50"/>
     <mergeCell ref="G44:H44"/>
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="D26:E26"/>
@@ -10067,6 +10290,7 @@
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="M24:N24"/>
     <mergeCell ref="J12:K12"/>
+    <mergeCell ref="A52:B52"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="J46:K46"/>
     <mergeCell ref="A10:B10"/>
@@ -10080,6 +10304,7 @@
     <mergeCell ref="G42:H42"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="M48:N48"/>
     <mergeCell ref="J40:K40"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="D52:E52"/>
@@ -10100,6 +10325,7 @@
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="J50:K50"/>
+    <mergeCell ref="G54:H54"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="G32:H32"/>
@@ -10109,8 +10335,10 @@
     <mergeCell ref="G50:H50"/>
     <mergeCell ref="D54:E54"/>
     <mergeCell ref="A40:B40"/>
+    <mergeCell ref="J52:K52"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="J44:K44"/>
+    <mergeCell ref="G52:H52"/>
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="G36:H36"/>
     <mergeCell ref="D46:E46"/>
@@ -10134,6 +10362,7 @@
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="M6:N6"/>
     <mergeCell ref="G30:H30"/>
+    <mergeCell ref="J54:K54"/>
     <mergeCell ref="M46:N46"/>
     <mergeCell ref="J32:K32"/>
     <mergeCell ref="M28:N28"/>
@@ -10141,6 +10370,7 @@
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D58:E58"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="A20:B20"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-12 19:16 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -5600,6 +5600,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -5625,6 +5628,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -5650,6 +5656,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -5675,6 +5684,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -5694,6 +5706,134 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId65"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>55</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="66" name="Image 66" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId66"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>59</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="67" name="Image 67" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId67"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>55</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="68" name="Image 68" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId68"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>55</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="69" name="Image 69" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId69"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>12</col>
+      <colOff>0</colOff>
+      <row>51</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="70" name="Image 70" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId70"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -9075,7 +9215,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N58"/>
+  <dimension ref="A1:N62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10193,6 +10333,16 @@
           <t>DET Low: 0.725</t>
         </is>
       </c>
+      <c r="M53" s="6" t="inlineStr">
+        <is>
+          <t>UTA Low: 0.695</t>
+        </is>
+      </c>
+      <c r="N53" s="6" t="inlineStr">
+        <is>
+          <t>MEM Low: 0.275</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="4" t="inlineStr">
@@ -10215,9 +10365,24 @@
           <t>Captured: 01:19 PM</t>
         </is>
       </c>
+      <c r="M54" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 02:16 PM</t>
+        </is>
+      </c>
     </row>
     <row r="56" ht="112.5" customHeight="1"/>
     <row r="57">
+      <c r="A57" s="6" t="inlineStr">
+        <is>
+          <t>CHI Low: 0.415</t>
+        </is>
+      </c>
+      <c r="B57" s="6" t="inlineStr">
+        <is>
+          <t>CHA Low: 0.565</t>
+        </is>
+      </c>
       <c r="D57" s="6" t="inlineStr">
         <is>
           <t>IND Low: 0.685</t>
@@ -10226,19 +10391,75 @@
       <c r="E57" s="6" t="inlineStr">
         <is>
           <t>PHI Low: 0.265</t>
+        </is>
+      </c>
+      <c r="G57" s="6" t="inlineStr">
+        <is>
+          <t>CLE Low: 0.105</t>
+        </is>
+      </c>
+      <c r="H57" s="6" t="inlineStr">
+        <is>
+          <t>WAS Low: 0.885</t>
+        </is>
+      </c>
+      <c r="J57" s="6" t="inlineStr">
+        <is>
+          <t>ATL Low: 0.725</t>
+        </is>
+      </c>
+      <c r="K57" s="6" t="inlineStr">
+        <is>
+          <t>DET Low: 0.275</t>
         </is>
       </c>
     </row>
     <row r="58">
+      <c r="A58" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 02:16 PM</t>
+        </is>
+      </c>
       <c r="D58" s="4" t="inlineStr">
         <is>
           <t>Captured: 01:19 PM</t>
+        </is>
+      </c>
+      <c r="G58" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 02:16 PM</t>
+        </is>
+      </c>
+      <c r="J58" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 02:16 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="60" ht="112.5" customHeight="1"/>
+    <row r="61">
+      <c r="D61" s="6" t="inlineStr">
+        <is>
+          <t>IND Low: 0.265</t>
+        </is>
+      </c>
+      <c r="E61" s="6" t="inlineStr">
+        <is>
+          <t>PHI Low: 0.685</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="D62" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 02:16 PM</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="145">
+  <mergeCells count="155">
     <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D60:E60"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="J28:K28"/>
@@ -10248,6 +10469,8 @@
     <mergeCell ref="A54:B54"/>
     <mergeCell ref="D44:E44"/>
     <mergeCell ref="M10:N10"/>
+    <mergeCell ref="M54:N54"/>
+    <mergeCell ref="A56:B56"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="D48:E48"/>
     <mergeCell ref="M16:N16"/>
@@ -10255,8 +10478,10 @@
     <mergeCell ref="G34:H34"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="M36:N36"/>
+    <mergeCell ref="G58:H58"/>
     <mergeCell ref="M18:N18"/>
     <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D62:E62"/>
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="A22:B22"/>
@@ -10266,6 +10491,7 @@
     <mergeCell ref="M50:N50"/>
     <mergeCell ref="G44:H44"/>
     <mergeCell ref="G22:H22"/>
+    <mergeCell ref="J58:K58"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="A48:B48"/>
     <mergeCell ref="A30:B30"/>
@@ -10303,6 +10529,7 @@
     <mergeCell ref="J38:K38"/>
     <mergeCell ref="G42:H42"/>
     <mergeCell ref="A36:B36"/>
+    <mergeCell ref="M52:N52"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="M48:N48"/>
     <mergeCell ref="J40:K40"/>
@@ -10336,6 +10563,7 @@
     <mergeCell ref="D54:E54"/>
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="J52:K52"/>
+    <mergeCell ref="G56:H56"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="J44:K44"/>
     <mergeCell ref="G52:H52"/>
@@ -10371,6 +10599,7 @@
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="D58:E58"/>
+    <mergeCell ref="J56:K56"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="A20:B20"/>
@@ -10383,6 +10612,7 @@
     <mergeCell ref="G40:H40"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="M4:N4"/>
+    <mergeCell ref="A58:B58"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-12 20:15 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -5740,6 +5740,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -5765,6 +5768,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -5790,6 +5796,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -5815,6 +5824,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -5834,6 +5846,134 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId70"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>63</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="71" name="Image 71" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId71"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>59</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="72" name="Image 72" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId72"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>59</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="73" name="Image 73" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId73"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>59</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="74" name="Image 74" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId74"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>12</col>
+      <colOff>0</colOff>
+      <row>55</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="75" name="Image 75" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId75"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -9215,7 +9355,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N62"/>
+  <dimension ref="A1:N66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10413,6 +10553,16 @@
           <t>DET Low: 0.275</t>
         </is>
       </c>
+      <c r="M57" s="6" t="inlineStr">
+        <is>
+          <t>UTA Low: 0.695</t>
+        </is>
+      </c>
+      <c r="N57" s="6" t="inlineStr">
+        <is>
+          <t>MEM Low: 0.275</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="4" t="inlineStr">
@@ -10435,9 +10585,24 @@
           <t>Captured: 02:16 PM</t>
         </is>
       </c>
+      <c r="M58" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 03:15 PM</t>
+        </is>
+      </c>
     </row>
     <row r="60" ht="112.5" customHeight="1"/>
     <row r="61">
+      <c r="A61" s="6" t="inlineStr">
+        <is>
+          <t>CHI Low: 0.575</t>
+        </is>
+      </c>
+      <c r="B61" s="6" t="inlineStr">
+        <is>
+          <t>CHA Low: 0.415</t>
+        </is>
+      </c>
       <c r="D61" s="6" t="inlineStr">
         <is>
           <t>IND Low: 0.265</t>
@@ -10446,18 +10611,73 @@
       <c r="E61" s="6" t="inlineStr">
         <is>
           <t>PHI Low: 0.685</t>
+        </is>
+      </c>
+      <c r="G61" s="6" t="inlineStr">
+        <is>
+          <t>CLE Low: 0.105</t>
+        </is>
+      </c>
+      <c r="H61" s="6" t="inlineStr">
+        <is>
+          <t>WAS Low: 0.885</t>
+        </is>
+      </c>
+      <c r="J61" s="6" t="inlineStr">
+        <is>
+          <t>ATL Low: 0.725</t>
+        </is>
+      </c>
+      <c r="K61" s="6" t="inlineStr">
+        <is>
+          <t>DET Low: 0.265</t>
         </is>
       </c>
     </row>
     <row r="62">
+      <c r="A62" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 03:15 PM</t>
+        </is>
+      </c>
       <c r="D62" s="4" t="inlineStr">
         <is>
           <t>Captured: 02:16 PM</t>
+        </is>
+      </c>
+      <c r="G62" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 03:15 PM</t>
+        </is>
+      </c>
+      <c r="J62" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 03:15 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="64" ht="112.5" customHeight="1"/>
+    <row r="65">
+      <c r="D65" s="6" t="inlineStr">
+        <is>
+          <t>IND Low: 0.685</t>
+        </is>
+      </c>
+      <c r="E65" s="6" t="inlineStr">
+        <is>
+          <t>PHI Low: 0.265</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="D66" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 03:15 PM</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="155">
+  <mergeCells count="165">
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D60:E60"/>
     <mergeCell ref="J10:K10"/>
@@ -10465,6 +10685,7 @@
     <mergeCell ref="J28:K28"/>
     <mergeCell ref="D36:E36"/>
     <mergeCell ref="D50:E50"/>
+    <mergeCell ref="J60:K60"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="A54:B54"/>
     <mergeCell ref="D44:E44"/>
@@ -10485,8 +10706,11 @@
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A62:B62"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="J62:K62"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="M50:N50"/>
     <mergeCell ref="G44:H44"/>
@@ -10506,7 +10730,9 @@
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="G38:H38"/>
     <mergeCell ref="A46:B46"/>
+    <mergeCell ref="G62:H62"/>
     <mergeCell ref="J36:K36"/>
+    <mergeCell ref="D66:E66"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="J20:K20"/>
     <mergeCell ref="G24:H24"/>
@@ -10521,6 +10747,7 @@
     <mergeCell ref="J46:K46"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="D38:E38"/>
+    <mergeCell ref="G60:H60"/>
     <mergeCell ref="J48:K48"/>
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="M34:N34"/>
@@ -10564,9 +10791,11 @@
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="J52:K52"/>
     <mergeCell ref="G56:H56"/>
+    <mergeCell ref="M58:N58"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="J44:K44"/>
     <mergeCell ref="G52:H52"/>
+    <mergeCell ref="A60:B60"/>
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="G36:H36"/>
     <mergeCell ref="D46:E46"/>
@@ -10613,6 +10842,7 @@
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="A58:B58"/>
+    <mergeCell ref="M56:N56"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-12 21:13 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -5880,6 +5880,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -5905,6 +5908,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -5930,6 +5936,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -5955,6 +5964,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -5974,6 +5986,134 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId75"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>67</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="76" name="Image 76" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId76"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>63</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="77" name="Image 77" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId77"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>63</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="78" name="Image 78" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId78"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>63</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="79" name="Image 79" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId79"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>12</col>
+      <colOff>0</colOff>
+      <row>59</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="80" name="Image 80" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId80"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -9355,7 +9495,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N66"/>
+  <dimension ref="A1:N70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10633,6 +10773,16 @@
           <t>DET Low: 0.265</t>
         </is>
       </c>
+      <c r="M61" s="6" t="inlineStr">
+        <is>
+          <t>UTA Low: 0.275</t>
+        </is>
+      </c>
+      <c r="N61" s="6" t="inlineStr">
+        <is>
+          <t>MEM Low: 0.695</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="4" t="inlineStr">
@@ -10655,9 +10805,24 @@
           <t>Captured: 03:15 PM</t>
         </is>
       </c>
+      <c r="M62" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 04:13 PM</t>
+        </is>
+      </c>
     </row>
     <row r="64" ht="112.5" customHeight="1"/>
     <row r="65">
+      <c r="A65" s="6" t="inlineStr">
+        <is>
+          <t>CHI Low: 0.415</t>
+        </is>
+      </c>
+      <c r="B65" s="6" t="inlineStr">
+        <is>
+          <t>CHA Low: 0.575</t>
+        </is>
+      </c>
       <c r="D65" s="6" t="inlineStr">
         <is>
           <t>IND Low: 0.685</t>
@@ -10666,20 +10831,76 @@
       <c r="E65" s="6" t="inlineStr">
         <is>
           <t>PHI Low: 0.265</t>
+        </is>
+      </c>
+      <c r="G65" s="6" t="inlineStr">
+        <is>
+          <t>CLE Low: 0.105</t>
+        </is>
+      </c>
+      <c r="H65" s="6" t="inlineStr">
+        <is>
+          <t>WAS Low: 0.885</t>
+        </is>
+      </c>
+      <c r="J65" s="6" t="inlineStr">
+        <is>
+          <t>ATL Low: 0.265</t>
+        </is>
+      </c>
+      <c r="K65" s="6" t="inlineStr">
+        <is>
+          <t>DET Low: 0.715</t>
         </is>
       </c>
     </row>
     <row r="66">
+      <c r="A66" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 04:13 PM</t>
+        </is>
+      </c>
       <c r="D66" s="4" t="inlineStr">
         <is>
           <t>Captured: 03:15 PM</t>
+        </is>
+      </c>
+      <c r="G66" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 04:13 PM</t>
+        </is>
+      </c>
+      <c r="J66" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 04:13 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="68" ht="112.5" customHeight="1"/>
+    <row r="69">
+      <c r="D69" s="6" t="inlineStr">
+        <is>
+          <t>IND Low: 0.285</t>
+        </is>
+      </c>
+      <c r="E69" s="6" t="inlineStr">
+        <is>
+          <t>PHI Low: 0.705</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="D70" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 04:13 PM</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="165">
+  <mergeCells count="175">
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D60:E60"/>
+    <mergeCell ref="A64:B64"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="J28:K28"/>
@@ -10688,9 +10909,12 @@
     <mergeCell ref="J60:K60"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="A54:B54"/>
+    <mergeCell ref="M60:N60"/>
     <mergeCell ref="D44:E44"/>
     <mergeCell ref="M10:N10"/>
     <mergeCell ref="M54:N54"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="D70:E70"/>
     <mergeCell ref="A56:B56"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="D48:E48"/>
@@ -10710,6 +10934,7 @@
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="D64:E64"/>
+    <mergeCell ref="M62:N62"/>
     <mergeCell ref="J62:K62"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="M50:N50"/>
@@ -10718,6 +10943,7 @@
     <mergeCell ref="J58:K58"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="A48:B48"/>
+    <mergeCell ref="J64:K64"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="D10:E10"/>
@@ -10773,6 +10999,8 @@
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="D3:E3"/>
+    <mergeCell ref="J66:K66"/>
+    <mergeCell ref="G64:H64"/>
     <mergeCell ref="M26:N26"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A4:B4"/>
@@ -10809,6 +11037,7 @@
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="D32:E32"/>
     <mergeCell ref="G28:H28"/>
+    <mergeCell ref="A66:B66"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="G3:H3"/>
@@ -10832,6 +11061,7 @@
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D68:E68"/>
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="M32:N32"/>
     <mergeCell ref="M14:N14"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-12 22:15 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -6020,6 +6020,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -6045,6 +6048,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -6070,6 +6076,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -6095,6 +6104,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -6114,6 +6126,134 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId80"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>71</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="81" name="Image 81" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId81"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>67</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="82" name="Image 82" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId82"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>67</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="83" name="Image 83" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId83"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>67</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="84" name="Image 84" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId84"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>12</col>
+      <colOff>0</colOff>
+      <row>63</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="85" name="Image 85" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId85"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -9495,7 +9635,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N70"/>
+  <dimension ref="A1:N74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10853,6 +10993,16 @@
           <t>DET Low: 0.715</t>
         </is>
       </c>
+      <c r="M65" s="6" t="inlineStr">
+        <is>
+          <t>UTA Low: 0.275</t>
+        </is>
+      </c>
+      <c r="N65" s="6" t="inlineStr">
+        <is>
+          <t>MEM Low: 0.695</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="4" t="inlineStr">
@@ -10875,9 +11025,24 @@
           <t>Captured: 04:13 PM</t>
         </is>
       </c>
+      <c r="M66" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 05:15 PM</t>
+        </is>
+      </c>
     </row>
     <row r="68" ht="112.5" customHeight="1"/>
     <row r="69">
+      <c r="A69" s="6" t="inlineStr">
+        <is>
+          <t>CHI Low: 0.565</t>
+        </is>
+      </c>
+      <c r="B69" s="6" t="inlineStr">
+        <is>
+          <t>CHA Low: 0.415</t>
+        </is>
+      </c>
       <c r="D69" s="6" t="inlineStr">
         <is>
           <t>IND Low: 0.285</t>
@@ -10886,18 +11051,73 @@
       <c r="E69" s="6" t="inlineStr">
         <is>
           <t>PHI Low: 0.705</t>
+        </is>
+      </c>
+      <c r="G69" s="6" t="inlineStr">
+        <is>
+          <t>CLE Low: 0.895</t>
+        </is>
+      </c>
+      <c r="H69" s="6" t="inlineStr">
+        <is>
+          <t>WAS Low: 0.095</t>
+        </is>
+      </c>
+      <c r="J69" s="6" t="inlineStr">
+        <is>
+          <t>ATL Low: 0.715</t>
+        </is>
+      </c>
+      <c r="K69" s="6" t="inlineStr">
+        <is>
+          <t>DET Low: 0.265</t>
         </is>
       </c>
     </row>
     <row r="70">
+      <c r="A70" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 05:15 PM</t>
+        </is>
+      </c>
       <c r="D70" s="4" t="inlineStr">
         <is>
           <t>Captured: 04:13 PM</t>
+        </is>
+      </c>
+      <c r="G70" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 05:15 PM</t>
+        </is>
+      </c>
+      <c r="J70" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 05:15 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="72" ht="112.5" customHeight="1"/>
+    <row r="73">
+      <c r="D73" s="6" t="inlineStr">
+        <is>
+          <t>IND Low: 0.715</t>
+        </is>
+      </c>
+      <c r="E73" s="6" t="inlineStr">
+        <is>
+          <t>PHI Low: 0.275</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="D74" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 05:15 PM</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="175">
+  <mergeCells count="185">
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D60:E60"/>
     <mergeCell ref="A64:B64"/>
@@ -10906,8 +11126,10 @@
     <mergeCell ref="J28:K28"/>
     <mergeCell ref="D36:E36"/>
     <mergeCell ref="D50:E50"/>
+    <mergeCell ref="A70:B70"/>
     <mergeCell ref="J60:K60"/>
     <mergeCell ref="D6:E6"/>
+    <mergeCell ref="J68:K68"/>
     <mergeCell ref="A54:B54"/>
     <mergeCell ref="M60:N60"/>
     <mergeCell ref="D44:E44"/>
@@ -10921,6 +11143,8 @@
     <mergeCell ref="M16:N16"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="G34:H34"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="G68:H68"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="M36:N36"/>
     <mergeCell ref="G58:H58"/>
@@ -10935,6 +11159,7 @@
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="D64:E64"/>
     <mergeCell ref="M62:N62"/>
+    <mergeCell ref="A68:B68"/>
     <mergeCell ref="J62:K62"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="M50:N50"/>
@@ -10951,7 +11176,9 @@
     <mergeCell ref="M44:N44"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="M1:N1"/>
+    <mergeCell ref="G70:H70"/>
     <mergeCell ref="G48:H48"/>
+    <mergeCell ref="M64:N64"/>
     <mergeCell ref="J34:K34"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="G38:H38"/>
@@ -10973,6 +11200,7 @@
     <mergeCell ref="J46:K46"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="D38:E38"/>
+    <mergeCell ref="M66:N66"/>
     <mergeCell ref="G60:H60"/>
     <mergeCell ref="J48:K48"/>
     <mergeCell ref="A34:B34"/>
@@ -11043,6 +11271,7 @@
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="M22:N22"/>
     <mergeCell ref="A50:B50"/>
+    <mergeCell ref="J70:K70"/>
     <mergeCell ref="M30:N30"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="A2:B2"/>
@@ -11061,6 +11290,7 @@
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D74:E74"/>
     <mergeCell ref="D68:E68"/>
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="M32:N32"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-12 23:14 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -6160,6 +6160,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -6185,6 +6188,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -6210,6 +6216,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -6235,6 +6244,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -6254,6 +6266,134 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId85"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>75</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="86" name="Image 86" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId86"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>71</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="87" name="Image 87" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId87"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>71</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="88" name="Image 88" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId88"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>71</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="89" name="Image 89" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId89"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>12</col>
+      <colOff>0</colOff>
+      <row>67</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="90" name="Image 90" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId90"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -9635,7 +9775,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N74"/>
+  <dimension ref="A1:N78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11073,6 +11213,16 @@
           <t>DET Low: 0.265</t>
         </is>
       </c>
+      <c r="M69" s="6" t="inlineStr">
+        <is>
+          <t>UTA Low: 0.695</t>
+        </is>
+      </c>
+      <c r="N69" s="6" t="inlineStr">
+        <is>
+          <t>MEM Low: 0.295</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="4" t="inlineStr">
@@ -11095,9 +11245,24 @@
           <t>Captured: 05:15 PM</t>
         </is>
       </c>
+      <c r="M70" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 06:14 PM</t>
+        </is>
+      </c>
     </row>
     <row r="72" ht="112.5" customHeight="1"/>
     <row r="73">
+      <c r="A73" s="6" t="inlineStr">
+        <is>
+          <t>CHI Low: 0.565</t>
+        </is>
+      </c>
+      <c r="B73" s="6" t="inlineStr">
+        <is>
+          <t>CHA Low: 0.415</t>
+        </is>
+      </c>
       <c r="D73" s="6" t="inlineStr">
         <is>
           <t>IND Low: 0.715</t>
@@ -11106,29 +11271,85 @@
       <c r="E73" s="6" t="inlineStr">
         <is>
           <t>PHI Low: 0.275</t>
+        </is>
+      </c>
+      <c r="G73" s="6" t="inlineStr">
+        <is>
+          <t>CLE Low: 0.095</t>
+        </is>
+      </c>
+      <c r="H73" s="6" t="inlineStr">
+        <is>
+          <t>WAS Low: 0.895</t>
+        </is>
+      </c>
+      <c r="J73" s="6" t="inlineStr">
+        <is>
+          <t>ATL Low: 0.715</t>
+        </is>
+      </c>
+      <c r="K73" s="6" t="inlineStr">
+        <is>
+          <t>DET Low: 0.265</t>
         </is>
       </c>
     </row>
     <row r="74">
+      <c r="A74" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 06:14 PM</t>
+        </is>
+      </c>
       <c r="D74" s="4" t="inlineStr">
         <is>
           <t>Captured: 05:15 PM</t>
+        </is>
+      </c>
+      <c r="G74" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 06:14 PM</t>
+        </is>
+      </c>
+      <c r="J74" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 06:14 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="76" ht="112.5" customHeight="1"/>
+    <row r="77">
+      <c r="D77" s="6" t="inlineStr">
+        <is>
+          <t>IND Low: 0.275</t>
+        </is>
+      </c>
+      <c r="E77" s="6" t="inlineStr">
+        <is>
+          <t>PHI Low: 0.675</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="D78" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 06:14 PM</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="185">
+  <mergeCells count="195">
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D60:E60"/>
     <mergeCell ref="A64:B64"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="J28:K28"/>
+    <mergeCell ref="A70:B70"/>
     <mergeCell ref="D36:E36"/>
     <mergeCell ref="D50:E50"/>
-    <mergeCell ref="A70:B70"/>
     <mergeCell ref="J60:K60"/>
     <mergeCell ref="D6:E6"/>
+    <mergeCell ref="M70:N70"/>
     <mergeCell ref="J68:K68"/>
     <mergeCell ref="A54:B54"/>
     <mergeCell ref="M60:N60"/>
@@ -11136,6 +11357,7 @@
     <mergeCell ref="M10:N10"/>
     <mergeCell ref="M54:N54"/>
     <mergeCell ref="G66:H66"/>
+    <mergeCell ref="A74:B74"/>
     <mergeCell ref="D70:E70"/>
     <mergeCell ref="A56:B56"/>
     <mergeCell ref="G18:H18"/>
@@ -11145,6 +11367,7 @@
     <mergeCell ref="G34:H34"/>
     <mergeCell ref="D72:E72"/>
     <mergeCell ref="G68:H68"/>
+    <mergeCell ref="D78:E78"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="M36:N36"/>
     <mergeCell ref="G58:H58"/>
@@ -11182,6 +11405,7 @@
     <mergeCell ref="J34:K34"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="G38:H38"/>
+    <mergeCell ref="D76:E76"/>
     <mergeCell ref="A46:B46"/>
     <mergeCell ref="G62:H62"/>
     <mergeCell ref="J36:K36"/>
@@ -11204,6 +11428,7 @@
     <mergeCell ref="G60:H60"/>
     <mergeCell ref="J48:K48"/>
     <mergeCell ref="A34:B34"/>
+    <mergeCell ref="M68:N68"/>
     <mergeCell ref="M34:N34"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G2:H2"/>
@@ -11217,6 +11442,7 @@
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="D52:E52"/>
     <mergeCell ref="J24:K24"/>
+    <mergeCell ref="J74:K74"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="M40:N40"/>
     <mergeCell ref="J26:K26"/>
@@ -11253,6 +11479,7 @@
     <mergeCell ref="G52:H52"/>
     <mergeCell ref="A60:B60"/>
     <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J72:K72"/>
     <mergeCell ref="G36:H36"/>
     <mergeCell ref="D46:E46"/>
     <mergeCell ref="D40:E40"/>
@@ -11270,6 +11497,7 @@
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="M22:N22"/>
+    <mergeCell ref="G74:H74"/>
     <mergeCell ref="A50:B50"/>
     <mergeCell ref="J70:K70"/>
     <mergeCell ref="M30:N30"/>
@@ -11291,6 +11519,7 @@
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="D74:E74"/>
+    <mergeCell ref="A72:B72"/>
     <mergeCell ref="D68:E68"/>
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="M32:N32"/>
@@ -11303,6 +11532,7 @@
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="A58:B58"/>
     <mergeCell ref="M56:N56"/>
+    <mergeCell ref="G72:H72"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-13 00:42 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -6300,6 +6300,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -6325,6 +6328,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -6350,6 +6356,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -6375,6 +6384,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -6394,6 +6406,134 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId90"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>75</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="91" name="Image 91" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId91"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>75</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="92" name="Image 92" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId92"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>75</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="93" name="Image 93" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId93"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>79</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="94" name="Image 94" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId94"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>12</col>
+      <colOff>0</colOff>
+      <row>71</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="95" name="Image 95" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId95"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -9775,7 +9915,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N78"/>
+  <dimension ref="A1:N82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11293,6 +11433,16 @@
           <t>DET Low: 0.265</t>
         </is>
       </c>
+      <c r="M73" s="6" t="inlineStr">
+        <is>
+          <t>UTA Low: 0.695</t>
+        </is>
+      </c>
+      <c r="N73" s="6" t="inlineStr">
+        <is>
+          <t>MEM Low: 0.295</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="4" t="inlineStr">
@@ -11315,9 +11465,24 @@
           <t>Captured: 06:14 PM</t>
         </is>
       </c>
+      <c r="M74" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 07:42 PM</t>
+        </is>
+      </c>
     </row>
     <row r="76" ht="112.5" customHeight="1"/>
     <row r="77">
+      <c r="A77" s="6" t="inlineStr">
+        <is>
+          <t>CHI Low: 0.345</t>
+        </is>
+      </c>
+      <c r="B77" s="6" t="inlineStr">
+        <is>
+          <t>CHA Low: 0.530</t>
+        </is>
+      </c>
       <c r="D77" s="6" t="inlineStr">
         <is>
           <t>IND Low: 0.275</t>
@@ -11326,18 +11491,73 @@
       <c r="E77" s="6" t="inlineStr">
         <is>
           <t>PHI Low: 0.675</t>
+        </is>
+      </c>
+      <c r="G77" s="6" t="inlineStr">
+        <is>
+          <t>CLE Low: 0.880</t>
+        </is>
+      </c>
+      <c r="H77" s="6" t="inlineStr">
+        <is>
+          <t>WAS Low: 0.045</t>
+        </is>
+      </c>
+      <c r="J77" s="6" t="inlineStr">
+        <is>
+          <t>ATL Low: 0.255</t>
+        </is>
+      </c>
+      <c r="K77" s="6" t="inlineStr">
+        <is>
+          <t>DET Low: 0.685</t>
         </is>
       </c>
     </row>
     <row r="78">
+      <c r="A78" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 07:42 PM</t>
+        </is>
+      </c>
       <c r="D78" s="4" t="inlineStr">
         <is>
           <t>Captured: 06:14 PM</t>
+        </is>
+      </c>
+      <c r="G78" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 07:42 PM</t>
+        </is>
+      </c>
+      <c r="J78" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 07:42 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="80" ht="112.5" customHeight="1"/>
+    <row r="81">
+      <c r="D81" s="6" t="inlineStr">
+        <is>
+          <t>IND Low: 0.645</t>
+        </is>
+      </c>
+      <c r="E81" s="6" t="inlineStr">
+        <is>
+          <t>PHI Low: 0.235</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="D82" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 07:42 PM</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="195">
+  <mergeCells count="205">
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D60:E60"/>
     <mergeCell ref="A64:B64"/>
@@ -11363,11 +11583,13 @@
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="D48:E48"/>
     <mergeCell ref="M16:N16"/>
+    <mergeCell ref="M74:N74"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="G34:H34"/>
     <mergeCell ref="D72:E72"/>
     <mergeCell ref="G68:H68"/>
     <mergeCell ref="D78:E78"/>
+    <mergeCell ref="A76:B76"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="M36:N36"/>
     <mergeCell ref="G58:H58"/>
@@ -11422,6 +11644,7 @@
     <mergeCell ref="A52:B52"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="J46:K46"/>
+    <mergeCell ref="G76:H76"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="D38:E38"/>
     <mergeCell ref="M66:N66"/>
@@ -11439,11 +11662,13 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="M48:N48"/>
     <mergeCell ref="J40:K40"/>
+    <mergeCell ref="A78:B78"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="D52:E52"/>
     <mergeCell ref="J24:K24"/>
     <mergeCell ref="J74:K74"/>
     <mergeCell ref="A3:B3"/>
+    <mergeCell ref="G78:H78"/>
     <mergeCell ref="M40:N40"/>
     <mergeCell ref="J26:K26"/>
     <mergeCell ref="A12:B12"/>
@@ -11484,7 +11709,9 @@
     <mergeCell ref="D46:E46"/>
     <mergeCell ref="D40:E40"/>
     <mergeCell ref="G8:H8"/>
+    <mergeCell ref="D80:E80"/>
     <mergeCell ref="A6:B6"/>
+    <mergeCell ref="J78:K78"/>
     <mergeCell ref="J30:K30"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="M20:N20"/>
@@ -11522,9 +11749,12 @@
     <mergeCell ref="A72:B72"/>
     <mergeCell ref="D68:E68"/>
     <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D82:E82"/>
     <mergeCell ref="M32:N32"/>
     <mergeCell ref="M14:N14"/>
+    <mergeCell ref="M72:N72"/>
     <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J76:K76"/>
     <mergeCell ref="A44:B44"/>
     <mergeCell ref="G46:H46"/>
     <mergeCell ref="G40:H40"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-13 01:42 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -6440,6 +6440,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -6465,6 +6468,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -6490,6 +6496,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -6515,6 +6524,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -6534,6 +6546,134 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId95"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>79</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="96" name="Image 96" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId96"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>79</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="97" name="Image 97" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId97"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>79</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="98" name="Image 98" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId98"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>83</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="99" name="Image 99" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId99"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>12</col>
+      <colOff>0</colOff>
+      <row>75</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="100" name="Image 100" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId100"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -9915,7 +10055,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N82"/>
+  <dimension ref="A1:N86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11513,6 +11653,16 @@
           <t>DET Low: 0.685</t>
         </is>
       </c>
+      <c r="M77" s="6" t="inlineStr">
+        <is>
+          <t>UTA Low: 0.265</t>
+        </is>
+      </c>
+      <c r="N77" s="6" t="inlineStr">
+        <is>
+          <t>MEM Low: 0.555</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="4" t="inlineStr">
@@ -11535,9 +11685,24 @@
           <t>Captured: 07:42 PM</t>
         </is>
       </c>
+      <c r="M78" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 08:42 PM</t>
+        </is>
+      </c>
     </row>
     <row r="80" ht="112.5" customHeight="1"/>
     <row r="81">
+      <c r="A81" s="6" t="inlineStr">
+        <is>
+          <t>CHI Low: 0.345</t>
+        </is>
+      </c>
+      <c r="B81" s="6" t="inlineStr">
+        <is>
+          <t>CHA Low: 0.185</t>
+        </is>
+      </c>
       <c r="D81" s="6" t="inlineStr">
         <is>
           <t>IND Low: 0.645</t>
@@ -11546,22 +11711,79 @@
       <c r="E81" s="6" t="inlineStr">
         <is>
           <t>PHI Low: 0.235</t>
+        </is>
+      </c>
+      <c r="G81" s="6" t="inlineStr">
+        <is>
+          <t>CLE Low: 0.465</t>
+        </is>
+      </c>
+      <c r="H81" s="6" t="inlineStr">
+        <is>
+          <t>WAS Low: 0.045</t>
+        </is>
+      </c>
+      <c r="J81" s="6" t="inlineStr">
+        <is>
+          <t>ATL Low: 0.070</t>
+        </is>
+      </c>
+      <c r="K81" s="6" t="inlineStr">
+        <is>
+          <t>DET Low: 0.685</t>
         </is>
       </c>
     </row>
     <row r="82">
+      <c r="A82" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 08:42 PM</t>
+        </is>
+      </c>
       <c r="D82" s="4" t="inlineStr">
         <is>
           <t>Captured: 07:42 PM</t>
+        </is>
+      </c>
+      <c r="G82" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 08:42 PM</t>
+        </is>
+      </c>
+      <c r="J82" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 08:42 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="84" ht="112.5" customHeight="1"/>
+    <row r="85">
+      <c r="D85" s="6" t="inlineStr">
+        <is>
+          <t>IND Low: 0.555</t>
+        </is>
+      </c>
+      <c r="E85" s="6" t="inlineStr">
+        <is>
+          <t>PHI Low: 0.175</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="D86" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 08:42 PM</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="205">
+  <mergeCells count="215">
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D60:E60"/>
+    <mergeCell ref="J82:K82"/>
     <mergeCell ref="A64:B64"/>
     <mergeCell ref="J10:K10"/>
+    <mergeCell ref="D84:E84"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="J28:K28"/>
     <mergeCell ref="A70:B70"/>
@@ -11574,6 +11796,7 @@
     <mergeCell ref="A54:B54"/>
     <mergeCell ref="M60:N60"/>
     <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D86:E86"/>
     <mergeCell ref="M10:N10"/>
     <mergeCell ref="M54:N54"/>
     <mergeCell ref="G66:H66"/>
@@ -11640,6 +11863,7 @@
     <mergeCell ref="G26:H26"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="M24:N24"/>
+    <mergeCell ref="M76:N76"/>
     <mergeCell ref="J12:K12"/>
     <mergeCell ref="A52:B52"/>
     <mergeCell ref="G16:H16"/>
@@ -11666,6 +11890,8 @@
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="D52:E52"/>
     <mergeCell ref="J24:K24"/>
+    <mergeCell ref="M78:N78"/>
+    <mergeCell ref="A80:B80"/>
     <mergeCell ref="J74:K74"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="G78:H78"/>
@@ -11674,6 +11900,7 @@
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="M12:N12"/>
     <mergeCell ref="J16:K16"/>
+    <mergeCell ref="G80:H80"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="A14:B14"/>
@@ -11702,6 +11929,7 @@
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="J44:K44"/>
     <mergeCell ref="G52:H52"/>
+    <mergeCell ref="A82:B82"/>
     <mergeCell ref="A60:B60"/>
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="J72:K72"/>
@@ -11712,11 +11940,13 @@
     <mergeCell ref="D80:E80"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="J78:K78"/>
+    <mergeCell ref="G82:H82"/>
     <mergeCell ref="J30:K30"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="M20:N20"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="G10:H10"/>
+    <mergeCell ref="J80:K80"/>
     <mergeCell ref="D32:E32"/>
     <mergeCell ref="G28:H28"/>
     <mergeCell ref="A66:B66"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-13 02:50 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -6580,6 +6580,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -6605,6 +6608,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -6630,6 +6636,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -6655,6 +6664,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -6674,6 +6686,109 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId100"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>12</col>
+      <colOff>0</colOff>
+      <row>79</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="101" name="Image 101" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId101"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>15</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="102" name="Image 102" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId102"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>18</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="103" name="Image 103" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId103"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>83</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="104" name="Image 104" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId104"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -10055,7 +10170,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N86"/>
+  <dimension ref="A1:T86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10078,6 +10193,12 @@
     <col width="25" customWidth="1" min="13" max="13"/>
     <col width="25" customWidth="1" min="14" max="14"/>
     <col width="3" customWidth="1" min="15" max="15"/>
+    <col width="25" customWidth="1" min="16" max="16"/>
+    <col width="25" customWidth="1" min="17" max="17"/>
+    <col width="3" customWidth="1" min="18" max="18"/>
+    <col width="25" customWidth="1" min="19" max="19"/>
+    <col width="25" customWidth="1" min="20" max="20"/>
+    <col width="3" customWidth="1" min="21" max="21"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -10111,6 +10232,18 @@
         </is>
       </c>
       <c r="N1" s="2" t="n"/>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>BKN @ DAL</t>
+        </is>
+      </c>
+      <c r="Q1" s="2" t="n"/>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>MIN @ GSW</t>
+        </is>
+      </c>
+      <c r="T1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -10143,6 +10276,18 @@
         </is>
       </c>
       <c r="N2" s="2" t="n"/>
+      <c r="P2" s="3" t="inlineStr">
+        <is>
+          <t>LIVE / 2025-12-12</t>
+        </is>
+      </c>
+      <c r="Q2" s="2" t="n"/>
+      <c r="S2" s="3" t="inlineStr">
+        <is>
+          <t>3:00 AM / 2025-12-12</t>
+        </is>
+      </c>
+      <c r="T2" s="2" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="5" t="inlineStr">
@@ -10168,6 +10313,16 @@
       <c r="M3" s="5" t="inlineStr">
         <is>
           <t>https://polymarket.com/event/nba-uta-mem-2025-12-12</t>
+        </is>
+      </c>
+      <c r="P3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-bkn-dal-2025-12-12</t>
+        </is>
+      </c>
+      <c r="S3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-min-gsw-2025-12-12</t>
         </is>
       </c>
     </row>
@@ -10223,6 +10378,26 @@
           <t>MEM Low: 0.295</t>
         </is>
       </c>
+      <c r="P5" s="6" t="inlineStr">
+        <is>
+          <t>BKN Low: 0.220</t>
+        </is>
+      </c>
+      <c r="Q5" s="6" t="inlineStr">
+        <is>
+          <t>DAL Low: 0.615</t>
+        </is>
+      </c>
+      <c r="S5" s="6" t="inlineStr">
+        <is>
+          <t>MIN Low: 0.525</t>
+        </is>
+      </c>
+      <c r="T5" s="6" t="inlineStr">
+        <is>
+          <t>GSW Low: 0.365</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="inlineStr">
@@ -10248,6 +10423,16 @@
       <c r="M6" s="4" t="inlineStr">
         <is>
           <t>Captured: 01:19 AM</t>
+        </is>
+      </c>
+      <c r="P6" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 09:50 PM</t>
+        </is>
+      </c>
+      <c r="S6" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 09:50 PM</t>
         </is>
       </c>
     </row>
@@ -11733,6 +11918,16 @@
           <t>DET Low: 0.685</t>
         </is>
       </c>
+      <c r="M81" s="6" t="inlineStr">
+        <is>
+          <t>UTA Low: 0.155</t>
+        </is>
+      </c>
+      <c r="N81" s="6" t="inlineStr">
+        <is>
+          <t>MEM Low: 0.555</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="4" t="inlineStr">
@@ -11755,9 +11950,24 @@
           <t>Captured: 08:42 PM</t>
         </is>
       </c>
+      <c r="M82" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 09:50 PM</t>
+        </is>
+      </c>
     </row>
     <row r="84" ht="112.5" customHeight="1"/>
     <row r="85">
+      <c r="A85" s="6" t="inlineStr">
+        <is>
+          <t>CHI Low: 0.185</t>
+        </is>
+      </c>
+      <c r="B85" s="6" t="inlineStr">
+        <is>
+          <t>CHA Low: 0.000</t>
+        </is>
+      </c>
       <c r="D85" s="6" t="inlineStr">
         <is>
           <t>IND Low: 0.555</t>
@@ -11770,6 +11980,11 @@
       </c>
     </row>
     <row r="86">
+      <c r="A86" s="7" t="inlineStr">
+        <is>
+          <t>Captured: 09:50 PM - FINAL</t>
+        </is>
+      </c>
       <c r="D86" s="4" t="inlineStr">
         <is>
           <t>Captured: 08:42 PM</t>
@@ -11777,7 +11992,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="215">
+  <mergeCells count="229">
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D60:E60"/>
     <mergeCell ref="J82:K82"/>
@@ -11795,8 +12010,10 @@
     <mergeCell ref="J68:K68"/>
     <mergeCell ref="A54:B54"/>
     <mergeCell ref="M60:N60"/>
+    <mergeCell ref="M82:N82"/>
+    <mergeCell ref="D86:E86"/>
     <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="P6:Q6"/>
     <mergeCell ref="M10:N10"/>
     <mergeCell ref="M54:N54"/>
     <mergeCell ref="G66:H66"/>
@@ -11835,6 +12052,7 @@
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="J58:K58"/>
     <mergeCell ref="D26:E26"/>
+    <mergeCell ref="S4:T4"/>
     <mergeCell ref="A48:B48"/>
     <mergeCell ref="J64:K64"/>
     <mergeCell ref="A30:B30"/>
@@ -11852,6 +12070,7 @@
     <mergeCell ref="G38:H38"/>
     <mergeCell ref="D76:E76"/>
     <mergeCell ref="A46:B46"/>
+    <mergeCell ref="P2:Q2"/>
     <mergeCell ref="G62:H62"/>
     <mergeCell ref="J36:K36"/>
     <mergeCell ref="D66:E66"/>
@@ -11869,12 +12088,14 @@
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="J46:K46"/>
     <mergeCell ref="G76:H76"/>
+    <mergeCell ref="S1:T1"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="D38:E38"/>
     <mergeCell ref="M66:N66"/>
     <mergeCell ref="G60:H60"/>
     <mergeCell ref="J48:K48"/>
     <mergeCell ref="A34:B34"/>
+    <mergeCell ref="P4:Q4"/>
     <mergeCell ref="M68:N68"/>
     <mergeCell ref="M34:N34"/>
     <mergeCell ref="D1:E1"/>
@@ -11883,7 +12104,9 @@
     <mergeCell ref="G42:H42"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="M52:N52"/>
+    <mergeCell ref="P1:Q1"/>
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="S3:T3"/>
     <mergeCell ref="M48:N48"/>
     <mergeCell ref="J40:K40"/>
     <mergeCell ref="A78:B78"/>
@@ -11904,6 +12127,7 @@
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="A14:B14"/>
+    <mergeCell ref="S6:T6"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="J66:K66"/>
     <mergeCell ref="G64:H64"/>
@@ -11911,6 +12135,7 @@
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A38:B38"/>
+    <mergeCell ref="P3:Q3"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="J50:K50"/>
     <mergeCell ref="G54:H54"/>
@@ -11943,9 +12168,11 @@
     <mergeCell ref="G82:H82"/>
     <mergeCell ref="J30:K30"/>
     <mergeCell ref="A16:B16"/>
+    <mergeCell ref="S2:T2"/>
     <mergeCell ref="M20:N20"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="G10:H10"/>
+    <mergeCell ref="A84:B84"/>
     <mergeCell ref="J80:K80"/>
     <mergeCell ref="D32:E32"/>
     <mergeCell ref="G28:H28"/>
@@ -11960,6 +12187,7 @@
     <mergeCell ref="M30:N30"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A86:B86"/>
     <mergeCell ref="M6:N6"/>
     <mergeCell ref="G30:H30"/>
     <mergeCell ref="J54:K54"/>
@@ -11967,6 +12195,7 @@
     <mergeCell ref="J32:K32"/>
     <mergeCell ref="M28:N28"/>
     <mergeCell ref="M42:N42"/>
+    <mergeCell ref="M80:N80"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="D18:E18"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-13 03:37 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -6720,6 +6720,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -6745,6 +6748,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -6770,6 +6776,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -6789,6 +6798,134 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId104"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>12</col>
+      <colOff>0</colOff>
+      <row>83</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="105" name="Image 105" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId105"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>15</col>
+      <colOff>0</colOff>
+      <row>7</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="106" name="Image 106" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId106"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>18</col>
+      <colOff>0</colOff>
+      <row>7</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="107" name="Image 107" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId107"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>87</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="108" name="Image 108" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId108"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>83</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="109" name="Image 109" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId109"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -10170,7 +10307,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T86"/>
+  <dimension ref="A1:T90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10488,6 +10625,26 @@
           <t>MEM Low: 0.295</t>
         </is>
       </c>
+      <c r="P9" s="6" t="inlineStr">
+        <is>
+          <t>BKN Low: 0.575</t>
+        </is>
+      </c>
+      <c r="Q9" s="6" t="inlineStr">
+        <is>
+          <t>DAL Low: 0.335</t>
+        </is>
+      </c>
+      <c r="S9" s="6" t="inlineStr">
+        <is>
+          <t>MIN Low: 0.645</t>
+        </is>
+      </c>
+      <c r="T9" s="6" t="inlineStr">
+        <is>
+          <t>GSW Low: 0.335</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="inlineStr">
@@ -10513,6 +10670,16 @@
       <c r="M10" s="4" t="inlineStr">
         <is>
           <t>Captured: 02:17 AM</t>
+        </is>
+      </c>
+      <c r="P10" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 10:37 PM</t>
+        </is>
+      </c>
+      <c r="S10" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 10:37 PM</t>
         </is>
       </c>
     </row>
@@ -11978,6 +12145,26 @@
           <t>PHI Low: 0.175</t>
         </is>
       </c>
+      <c r="J85" s="6" t="inlineStr">
+        <is>
+          <t>ATL Low: 0.685</t>
+        </is>
+      </c>
+      <c r="K85" s="6" t="inlineStr">
+        <is>
+          <t>DET Low: 0.000</t>
+        </is>
+      </c>
+      <c r="M85" s="6" t="inlineStr">
+        <is>
+          <t>UTA Low: 0.140</t>
+        </is>
+      </c>
+      <c r="N85" s="6" t="inlineStr">
+        <is>
+          <t>MEM Low: 0.005</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="7" t="inlineStr">
@@ -11990,9 +12177,39 @@
           <t>Captured: 08:42 PM</t>
         </is>
       </c>
+      <c r="J86" s="7" t="inlineStr">
+        <is>
+          <t>Captured: 10:37 PM - FINAL</t>
+        </is>
+      </c>
+      <c r="M86" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 10:37 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="88" ht="112.5" customHeight="1"/>
+    <row r="89">
+      <c r="D89" s="6" t="inlineStr">
+        <is>
+          <t>IND Low: 0.375</t>
+        </is>
+      </c>
+      <c r="E89" s="6" t="inlineStr">
+        <is>
+          <t>PHI Low: 0.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="D90" s="7" t="inlineStr">
+        <is>
+          <t>Captured: 10:37 PM - FINAL</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="229">
+  <mergeCells count="239">
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D60:E60"/>
     <mergeCell ref="J82:K82"/>
@@ -12024,12 +12241,14 @@
     <mergeCell ref="D48:E48"/>
     <mergeCell ref="M16:N16"/>
     <mergeCell ref="M74:N74"/>
+    <mergeCell ref="J86:K86"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="G34:H34"/>
     <mergeCell ref="D72:E72"/>
     <mergeCell ref="G68:H68"/>
     <mergeCell ref="D78:E78"/>
     <mergeCell ref="A76:B76"/>
+    <mergeCell ref="S10:T10"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="M36:N36"/>
     <mergeCell ref="G58:H58"/>
@@ -12051,6 +12270,7 @@
     <mergeCell ref="G44:H44"/>
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="J58:K58"/>
+    <mergeCell ref="D88:E88"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="S4:T4"/>
     <mergeCell ref="A48:B48"/>
@@ -12059,7 +12279,9 @@
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D90:E90"/>
     <mergeCell ref="M44:N44"/>
+    <mergeCell ref="P10:Q10"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="G70:H70"/>
@@ -12163,15 +12385,18 @@
     <mergeCell ref="D40:E40"/>
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="D80:E80"/>
+    <mergeCell ref="J84:K84"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="J78:K78"/>
     <mergeCell ref="G82:H82"/>
+    <mergeCell ref="S8:T8"/>
     <mergeCell ref="J30:K30"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="M20:N20"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="G10:H10"/>
+    <mergeCell ref="P8:Q8"/>
     <mergeCell ref="A84:B84"/>
     <mergeCell ref="J80:K80"/>
     <mergeCell ref="D32:E32"/>
@@ -12179,6 +12404,7 @@
     <mergeCell ref="A66:B66"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="A18:B18"/>
+    <mergeCell ref="M84:N84"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="M22:N22"/>
     <mergeCell ref="G74:H74"/>
@@ -12194,6 +12420,7 @@
     <mergeCell ref="M46:N46"/>
     <mergeCell ref="J32:K32"/>
     <mergeCell ref="M28:N28"/>
+    <mergeCell ref="M86:N86"/>
     <mergeCell ref="M42:N42"/>
     <mergeCell ref="M80:N80"/>
     <mergeCell ref="G14:H14"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-13 04:22 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -6832,6 +6832,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -6857,6 +6860,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -6882,6 +6888,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -6907,6 +6916,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -6926,6 +6938,34 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId109"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>18</col>
+      <colOff>0</colOff>
+      <row>11</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="110" name="Image 110" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId110"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -10735,6 +10775,16 @@
           <t>MEM Low: 0.665</t>
         </is>
       </c>
+      <c r="S13" s="6" t="inlineStr">
+        <is>
+          <t>MIN Low: 0.575</t>
+        </is>
+      </c>
+      <c r="T13" s="6" t="inlineStr">
+        <is>
+          <t>GSW Low: 0.310</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="inlineStr">
@@ -10760,6 +10810,11 @@
       <c r="M14" s="4" t="inlineStr">
         <is>
           <t>Captured: 03:19 AM</t>
+        </is>
+      </c>
+      <c r="S14" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 11:22 PM</t>
         </is>
       </c>
     </row>
@@ -12209,7 +12264,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="239">
+  <mergeCells count="241">
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D60:E60"/>
     <mergeCell ref="J82:K82"/>
@@ -12269,8 +12324,8 @@
     <mergeCell ref="M50:N50"/>
     <mergeCell ref="G44:H44"/>
     <mergeCell ref="G22:H22"/>
+    <mergeCell ref="D88:E88"/>
     <mergeCell ref="J58:K58"/>
-    <mergeCell ref="D88:E88"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="S4:T4"/>
     <mergeCell ref="A48:B48"/>
@@ -12280,6 +12335,7 @@
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="D90:E90"/>
+    <mergeCell ref="S12:T12"/>
     <mergeCell ref="M44:N44"/>
     <mergeCell ref="P10:Q10"/>
     <mergeCell ref="J1:K1"/>
@@ -12336,6 +12392,7 @@
     <mergeCell ref="D52:E52"/>
     <mergeCell ref="J24:K24"/>
     <mergeCell ref="M78:N78"/>
+    <mergeCell ref="S14:T14"/>
     <mergeCell ref="A80:B80"/>
     <mergeCell ref="J74:K74"/>
     <mergeCell ref="A3:B3"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-13 05:12 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -12,6 +12,7 @@
     <sheet name="2025-12-10" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="2025-12-11" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="2025-12-12" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="2025-12-13" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -6966,6 +6967,64 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId110"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -12510,4 +12569,119 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="25" customWidth="1" min="1" max="1"/>
+    <col width="25" customWidth="1" min="2" max="2"/>
+    <col width="3" customWidth="1" min="3" max="3"/>
+    <col width="25" customWidth="1" min="4" max="4"/>
+    <col width="25" customWidth="1" min="5" max="5"/>
+    <col width="3" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>NYK @ ORL</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="n"/>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>SAS @ OKC</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>10:30 PM / 2025-12-13</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n"/>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>2:00 AM / 2025-12-13</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-nyk-orl-2025-12-13</t>
+        </is>
+      </c>
+      <c r="D3" s="5" t="inlineStr">
+        <is>
+          <t>https://polymarket.com/event/nba-sas-okc-2025-12-13</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="112.5" customHeight="1"/>
+    <row r="5">
+      <c r="A5" s="6" t="inlineStr">
+        <is>
+          <t>NYK Low: 0.645</t>
+        </is>
+      </c>
+      <c r="B5" s="6" t="inlineStr">
+        <is>
+          <t>ORL Low: 0.345</t>
+        </is>
+      </c>
+      <c r="D5" s="6" t="inlineStr">
+        <is>
+          <t>SAS Low: 0.775</t>
+        </is>
+      </c>
+      <c r="E5" s="6" t="inlineStr">
+        <is>
+          <t>OKC Low: 0.205</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 12:12 AM</t>
+        </is>
+      </c>
+      <c r="D6" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 12:12 AM</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update NBA prices - 2025-12-13 06:14 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -7006,6 +7006,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -7025,6 +7028,59 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>7</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>7</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="4" name="Image 4" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -12577,7 +12633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12668,15 +12724,54 @@
         </is>
       </c>
     </row>
+    <row r="8" ht="112.5" customHeight="1"/>
+    <row r="9">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>NYK Low: 0.350</t>
+        </is>
+      </c>
+      <c r="B9" s="6" t="inlineStr">
+        <is>
+          <t>ORL Low: 0.645</t>
+        </is>
+      </c>
+      <c r="D9" s="6" t="inlineStr">
+        <is>
+          <t>SAS Low: 0.205</t>
+        </is>
+      </c>
+      <c r="E9" s="6" t="inlineStr">
+        <is>
+          <t>OKC Low: 0.775</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 01:14 AM</t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 01:14 AM</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="14">
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D8:E8"/>
     <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D10:E10"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D1:E1"/>
+    <mergeCell ref="A10:B10"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A8:B8"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A6:B6"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-13 07:11 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -7062,6 +7062,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -7081,6 +7084,59 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>11</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="5" name="Image 5" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>11</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="6" name="Image 6" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -12633,7 +12689,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12759,8 +12815,43 @@
         </is>
       </c>
     </row>
+    <row r="12" ht="112.5" customHeight="1"/>
+    <row r="13">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>NYK Low: 0.345</t>
+        </is>
+      </c>
+      <c r="B13" s="6" t="inlineStr">
+        <is>
+          <t>ORL Low: 0.645</t>
+        </is>
+      </c>
+      <c r="D13" s="6" t="inlineStr">
+        <is>
+          <t>SAS Low: 0.205</t>
+        </is>
+      </c>
+      <c r="E13" s="6" t="inlineStr">
+        <is>
+          <t>OKC Low: 0.780</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 02:11 AM</t>
+        </is>
+      </c>
+      <c r="D14" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 02:11 AM</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="18">
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D8:E8"/>
@@ -12769,12 +12860,16 @@
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A14:B14"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-13 08:14 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -7118,6 +7118,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -7137,6 +7140,59 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>15</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="7" name="Image 7" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>15</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="8" name="Image 8" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId8"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -12689,7 +12745,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12850,26 +12906,65 @@
         </is>
       </c>
     </row>
+    <row r="16" ht="112.5" customHeight="1"/>
+    <row r="17">
+      <c r="A17" s="6" t="inlineStr">
+        <is>
+          <t>NYK Low: 0.345</t>
+        </is>
+      </c>
+      <c r="B17" s="6" t="inlineStr">
+        <is>
+          <t>ORL Low: 0.645</t>
+        </is>
+      </c>
+      <c r="D17" s="6" t="inlineStr">
+        <is>
+          <t>SAS Low: 0.785</t>
+        </is>
+      </c>
+      <c r="E17" s="6" t="inlineStr">
+        <is>
+          <t>OKC Low: 0.205</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 03:14 AM</t>
+        </is>
+      </c>
+      <c r="D18" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 03:14 AM</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="22">
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D6:E6"/>
     <mergeCell ref="D8:E8"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D1:E1"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="D14:E14"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-13 09:13 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -7174,6 +7174,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -7193,6 +7196,34 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>19</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="9" name="Image 9" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId9"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -12745,7 +12776,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12941,8 +12972,28 @@
         </is>
       </c>
     </row>
+    <row r="20" ht="112.5" customHeight="1"/>
+    <row r="21">
+      <c r="A21" s="6" t="inlineStr">
+        <is>
+          <t>NYK Low: 0.645</t>
+        </is>
+      </c>
+      <c r="B21" s="6" t="inlineStr">
+        <is>
+          <t>ORL Low: 0.345</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 04:13 AM</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="24">
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="A1:B1"/>
@@ -12960,9 +13011,11 @@
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A22:B22"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="D8:E8"/>
+    <mergeCell ref="A20:B20"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="D14:E14"/>
   </mergeCells>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-13 10:11 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -7224,6 +7224,59 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>23</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="10" name="Image 10" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>19</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="11" name="Image 11" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId11"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -12776,7 +12829,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12984,6 +13037,16 @@
           <t>ORL Low: 0.345</t>
         </is>
       </c>
+      <c r="D21" s="6" t="inlineStr">
+        <is>
+          <t>SAS Low: 0.785</t>
+        </is>
+      </c>
+      <c r="E21" s="6" t="inlineStr">
+        <is>
+          <t>OKC Low: 0.205</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="4" t="inlineStr">
@@ -12991,11 +13054,39 @@
           <t>Captured: 04:13 AM</t>
         </is>
       </c>
+      <c r="D22" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 05:11 AM</t>
+        </is>
+      </c>
+    </row>
+    <row r="24" ht="112.5" customHeight="1"/>
+    <row r="25">
+      <c r="A25" s="6" t="inlineStr">
+        <is>
+          <t>NYK Low: 0.645</t>
+        </is>
+      </c>
+      <c r="B25" s="6" t="inlineStr">
+        <is>
+          <t>ORL Low: 0.345</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 05:11 AM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="28">
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="A24:B24"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D22:E22"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="D6:E6"/>
@@ -13004,6 +13095,7 @@
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A26:B26"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A14:B14"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-13 12:16 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -7258,6 +7258,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -7277,6 +7280,59 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>27</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="12" name="Image 12" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>23</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="13" name="Image 13" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId13"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -12829,7 +12885,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13072,6 +13128,16 @@
           <t>ORL Low: 0.345</t>
         </is>
       </c>
+      <c r="D25" s="6" t="inlineStr">
+        <is>
+          <t>SAS Low: 0.205</t>
+        </is>
+      </c>
+      <c r="E25" s="6" t="inlineStr">
+        <is>
+          <t>OKC Low: 0.785</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="4" t="inlineStr">
@@ -13079,11 +13145,37 @@
           <t>Captured: 05:11 AM</t>
         </is>
       </c>
+      <c r="D26" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 07:16 AM</t>
+        </is>
+      </c>
+    </row>
+    <row r="28" ht="112.5" customHeight="1"/>
+    <row r="29">
+      <c r="A29" s="6" t="inlineStr">
+        <is>
+          <t>NYK Low: 0.645</t>
+        </is>
+      </c>
+      <c r="B29" s="6" t="inlineStr">
+        <is>
+          <t>ORL Low: 0.345</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 07:16 AM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="32">
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A30:B30"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="D22:E22"/>
@@ -13108,8 +13200,11 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D24:E24"/>
     <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A28:B28"/>
     <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D26:E26"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Update NBA prices - 2025-12-13 13:17 UTC
</commit_message>
<xml_diff>
--- a/nba_polymarket_prices.xlsx
+++ b/nba_polymarket_prices.xlsx
@@ -7314,6 +7314,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -7333,6 +7336,59 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>31</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="14" name="Image 14" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>27</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="15" name="Image 15" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId15"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -12885,7 +12941,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13163,6 +13219,16 @@
           <t>ORL Low: 0.345</t>
         </is>
       </c>
+      <c r="D29" s="6" t="inlineStr">
+        <is>
+          <t>SAS Low: 0.785</t>
+        </is>
+      </c>
+      <c r="E29" s="6" t="inlineStr">
+        <is>
+          <t>OKC Low: 0.205</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="4" t="inlineStr">
@@ -13170,9 +13236,34 @@
           <t>Captured: 07:16 AM</t>
         </is>
       </c>
+      <c r="D30" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 08:17 AM</t>
+        </is>
+      </c>
+    </row>
+    <row r="32" ht="112.5" customHeight="1"/>
+    <row r="33">
+      <c r="A33" s="6" t="inlineStr">
+        <is>
+          <t>NYK Low: 0.345</t>
+        </is>
+      </c>
+      <c r="B33" s="6" t="inlineStr">
+        <is>
+          <t>ORL Low: 0.635</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="4" t="inlineStr">
+        <is>
+          <t>Captured: 08:17 AM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="36">
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A30:B30"/>
@@ -13190,6 +13281,8 @@
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D28:E28"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D18:E18"/>
@@ -13201,10 +13294,12 @@
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D30:E30"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D26:E26"/>
+    <mergeCell ref="A34:B34"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>